<commit_message>
auto commit @ _1527
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
+++ b/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F5CC24-DCDD-4252-AB96-FB0C18C04CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95103779-533D-4953-9E2A-61050ADBCCBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Statement" sheetId="2" r:id="rId1"/>
@@ -5277,113 +5277,31 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -5392,14 +5310,107 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -5413,6 +5424,24 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -5437,35 +5466,6 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40 % - Akzent3" xfId="3" builtinId="39"/>
@@ -5755,7 +5755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
+    <sheetView topLeftCell="A221" workbookViewId="0">
       <selection activeCell="F230" sqref="F230"/>
     </sheetView>
   </sheetViews>
@@ -5769,19 +5769,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="88.5" customHeight="1">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="176" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="169"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
+      <c r="I2" s="173"/>
+      <c r="J2" s="173"/>
+      <c r="K2" s="173"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1"/>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
@@ -5791,10 +5791,10 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A6" s="188" t="s">
+      <c r="A6" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="189"/>
+      <c r="B6" s="197"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -5844,70 +5844,70 @@
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A14" s="190" t="s">
+      <c r="A14" s="198" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="191"/>
+      <c r="B14" s="199"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="173" t="s">
+      <c r="B15" s="205" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="174"/>
-      <c r="D15" s="175"/>
+      <c r="C15" s="206"/>
+      <c r="D15" s="207"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1">
       <c r="A16" s="166" t="s">
         <v>401</v>
       </c>
-      <c r="B16" s="179" t="s">
+      <c r="B16" s="211" t="s">
         <v>405</v>
       </c>
-      <c r="C16" s="180"/>
-      <c r="D16" s="181"/>
+      <c r="C16" s="212"/>
+      <c r="D16" s="213"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="167" t="s">
         <v>400</v>
       </c>
-      <c r="B17" s="182" t="s">
+      <c r="B17" s="200" t="s">
         <v>406</v>
       </c>
-      <c r="C17" s="183"/>
-      <c r="D17" s="184"/>
+      <c r="C17" s="201"/>
+      <c r="D17" s="202"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1">
       <c r="A18" s="167" t="s">
         <v>399</v>
       </c>
-      <c r="B18" s="182" t="s">
+      <c r="B18" s="200" t="s">
         <v>404</v>
       </c>
-      <c r="C18" s="183"/>
-      <c r="D18" s="184"/>
+      <c r="C18" s="201"/>
+      <c r="D18" s="202"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1">
       <c r="A19" s="167" t="s">
         <v>402</v>
       </c>
-      <c r="B19" s="182" t="s">
+      <c r="B19" s="200" t="s">
         <v>408</v>
       </c>
-      <c r="C19" s="183"/>
-      <c r="D19" s="184"/>
+      <c r="C19" s="201"/>
+      <c r="D19" s="202"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1">
       <c r="A20" s="167" t="s">
         <v>403</v>
       </c>
-      <c r="B20" s="182" t="s">
+      <c r="B20" s="200" t="s">
         <v>407</v>
       </c>
-      <c r="C20" s="183"/>
-      <c r="D20" s="184"/>
+      <c r="C20" s="201"/>
+      <c r="D20" s="202"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
@@ -5915,70 +5915,70 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" customHeight="1" thickBot="1">
-      <c r="A23" s="170" t="s">
+      <c r="A23" s="203" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="171"/>
+      <c r="B23" s="204"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="176" t="s">
+      <c r="B24" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="177"/>
-      <c r="D24" s="178"/>
+      <c r="C24" s="209"/>
+      <c r="D24" s="210"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1">
       <c r="A25" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="B25" s="179" t="s">
+      <c r="B25" s="211" t="s">
         <v>405</v>
       </c>
-      <c r="C25" s="180"/>
-      <c r="D25" s="181"/>
+      <c r="C25" s="212"/>
+      <c r="D25" s="213"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1">
       <c r="A26" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="B26" s="182" t="s">
+      <c r="B26" s="200" t="s">
         <v>406</v>
       </c>
-      <c r="C26" s="183"/>
-      <c r="D26" s="184"/>
+      <c r="C26" s="201"/>
+      <c r="D26" s="202"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1">
       <c r="A27" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="B27" s="182" t="s">
+      <c r="B27" s="200" t="s">
         <v>404</v>
       </c>
-      <c r="C27" s="183"/>
-      <c r="D27" s="184"/>
+      <c r="C27" s="201"/>
+      <c r="D27" s="202"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1">
       <c r="A28" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="B28" s="182" t="s">
+      <c r="B28" s="200" t="s">
         <v>408</v>
       </c>
-      <c r="C28" s="183"/>
-      <c r="D28" s="184"/>
+      <c r="C28" s="201"/>
+      <c r="D28" s="202"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1">
       <c r="A29" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="B29" s="182" t="s">
+      <c r="B29" s="200" t="s">
         <v>407</v>
       </c>
-      <c r="C29" s="183"/>
-      <c r="D29" s="184"/>
+      <c r="C29" s="201"/>
+      <c r="D29" s="202"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="165"/>
@@ -5990,13 +5990,13 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="76.5" customHeight="1">
-      <c r="A32" s="172" t="s">
+      <c r="A32" s="193" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="168"/>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="168"/>
+      <c r="B32" s="176"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="176"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="35" spans="1:5" ht="15.75" thickBot="1">
@@ -6187,13 +6187,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="57" customHeight="1">
-      <c r="A48" s="172" t="s">
+      <c r="A48" s="193" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="172"/>
-      <c r="C48" s="172"/>
-      <c r="D48" s="172"/>
-      <c r="E48" s="172"/>
+      <c r="B48" s="193"/>
+      <c r="C48" s="193"/>
+      <c r="D48" s="193"/>
+      <c r="E48" s="193"/>
     </row>
     <row r="49" spans="1:5" ht="31.5" customHeight="1" thickBot="1"/>
     <row r="50" spans="1:5" ht="44.25" customHeight="1" thickBot="1">
@@ -6306,13 +6306,13 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A59" s="172" t="s">
+      <c r="A59" s="193" t="s">
         <v>177</v>
       </c>
-      <c r="B59" s="172"/>
-      <c r="C59" s="172"/>
-      <c r="D59" s="172"/>
-      <c r="E59" s="172"/>
+      <c r="B59" s="193"/>
+      <c r="C59" s="193"/>
+      <c r="D59" s="193"/>
+      <c r="E59" s="193"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="10"/>
@@ -6334,12 +6334,12 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="36" customHeight="1">
-      <c r="A64" s="172" t="s">
+      <c r="A64" s="193" t="s">
         <v>178</v>
       </c>
-      <c r="B64" s="172"/>
-      <c r="C64" s="172"/>
-      <c r="D64" s="172"/>
+      <c r="B64" s="193"/>
+      <c r="C64" s="193"/>
+      <c r="D64" s="193"/>
       <c r="E64" s="8"/>
     </row>
     <row r="66" spans="1:5">
@@ -6351,12 +6351,12 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="172" t="s">
+      <c r="A69" s="193" t="s">
         <v>179</v>
       </c>
-      <c r="B69" s="172"/>
-      <c r="C69" s="172"/>
-      <c r="D69" s="172"/>
+      <c r="B69" s="193"/>
+      <c r="C69" s="193"/>
+      <c r="D69" s="193"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="71" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
@@ -6437,13 +6437,13 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A80" s="185" t="s">
+      <c r="A80" s="194" t="s">
         <v>187</v>
       </c>
-      <c r="B80" s="185"/>
-      <c r="C80" s="186"/>
-      <c r="D80" s="186"/>
-      <c r="E80" s="186"/>
+      <c r="B80" s="194"/>
+      <c r="C80" s="190"/>
+      <c r="D80" s="190"/>
+      <c r="E80" s="190"/>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="82" spans="1:4" ht="35.25" customHeight="1" thickBot="1">
@@ -6537,10 +6537,10 @@
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="187" t="s">
+      <c r="A91" s="195" t="s">
         <v>192</v>
       </c>
-      <c r="B91" s="187"/>
+      <c r="B91" s="195"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
@@ -6556,12 +6556,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="70.5" customHeight="1">
-      <c r="A97" s="195" t="s">
+      <c r="A97" s="189" t="s">
         <v>195</v>
       </c>
-      <c r="B97" s="186"/>
-      <c r="C97" s="186"/>
-      <c r="D97" s="186"/>
+      <c r="B97" s="190"/>
+      <c r="C97" s="190"/>
+      <c r="D97" s="190"/>
     </row>
     <row r="98" spans="1:4" ht="15.75" thickBot="1">
       <c r="A98" t="s">
@@ -6677,12 +6677,12 @@
       <c r="D108" s="2"/>
     </row>
     <row r="109" spans="1:4" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A109" s="193" t="s">
+      <c r="A109" s="183" t="s">
         <v>199</v>
       </c>
-      <c r="B109" s="193"/>
-      <c r="C109" s="194"/>
-      <c r="D109" s="194"/>
+      <c r="B109" s="183"/>
+      <c r="C109" s="184"/>
+      <c r="D109" s="184"/>
     </row>
     <row r="110" spans="1:4" ht="15.75" thickBot="1">
       <c r="A110" s="27" t="s">
@@ -6743,9 +6743,9 @@
       <c r="D116" s="57"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="196"/>
-      <c r="B117" s="196"/>
-      <c r="C117" s="197"/>
+      <c r="A117" s="191"/>
+      <c r="B117" s="191"/>
+      <c r="C117" s="192"/>
       <c r="D117" s="2"/>
     </row>
     <row r="118" spans="1:4">
@@ -6763,12 +6763,12 @@
       <c r="D119" s="2"/>
     </row>
     <row r="120" spans="1:4" ht="113.25" customHeight="1" thickBot="1">
-      <c r="A120" s="192" t="s">
+      <c r="A120" s="182" t="s">
         <v>420</v>
       </c>
-      <c r="B120" s="192"/>
-      <c r="C120" s="168"/>
-      <c r="D120" s="168"/>
+      <c r="B120" s="182"/>
+      <c r="C120" s="176"/>
+      <c r="D120" s="176"/>
     </row>
     <row r="121" spans="1:4" ht="29.25" thickBot="1">
       <c r="A121" s="27" t="s">
@@ -6953,12 +6953,12 @@
       <c r="D136" s="2"/>
     </row>
     <row r="137" spans="1:4" ht="38.25" customHeight="1" thickBot="1">
-      <c r="A137" s="192" t="s">
+      <c r="A137" s="182" t="s">
         <v>206</v>
       </c>
-      <c r="B137" s="192"/>
-      <c r="C137" s="168"/>
-      <c r="D137" s="168"/>
+      <c r="B137" s="182"/>
+      <c r="C137" s="176"/>
+      <c r="D137" s="176"/>
     </row>
     <row r="138" spans="1:4" ht="15.75" thickBot="1">
       <c r="A138" s="27" t="s">
@@ -7007,10 +7007,10 @@
       <c r="D141" s="2"/>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="199" t="s">
+      <c r="A142" s="169" t="s">
         <v>258</v>
       </c>
-      <c r="B142" s="199"/>
+      <c r="B142" s="169"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
@@ -7021,12 +7021,12 @@
       <c r="D143" s="2"/>
     </row>
     <row r="144" spans="1:4" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A144" s="192" t="s">
+      <c r="A144" s="182" t="s">
         <v>257</v>
       </c>
-      <c r="B144" s="192"/>
-      <c r="C144" s="168"/>
-      <c r="D144" s="168"/>
+      <c r="B144" s="182"/>
+      <c r="C144" s="176"/>
+      <c r="D144" s="176"/>
     </row>
     <row r="145" spans="1:4" ht="15.75" thickBot="1">
       <c r="A145" s="27" t="s">
@@ -7069,12 +7069,12 @@
       <c r="D150" s="2"/>
     </row>
     <row r="151" spans="1:4" ht="49.5" customHeight="1" thickBot="1">
-      <c r="A151" s="193" t="s">
+      <c r="A151" s="183" t="s">
         <v>210</v>
       </c>
-      <c r="B151" s="193"/>
-      <c r="C151" s="194"/>
-      <c r="D151" s="194"/>
+      <c r="B151" s="183"/>
+      <c r="C151" s="184"/>
+      <c r="D151" s="184"/>
     </row>
     <row r="152" spans="1:4" ht="29.25" thickBot="1">
       <c r="A152" s="27" t="s">
@@ -7153,10 +7153,10 @@
       <c r="D158" s="2"/>
     </row>
     <row r="159" spans="1:4" ht="39" customHeight="1" thickBot="1">
-      <c r="A159" s="198" t="s">
+      <c r="A159" s="170" t="s">
         <v>259</v>
       </c>
-      <c r="B159" s="198"/>
+      <c r="B159" s="170"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
     </row>
@@ -7201,10 +7201,10 @@
       <c r="D163" s="2"/>
     </row>
     <row r="164" spans="1:7">
-      <c r="A164" s="199" t="s">
+      <c r="A164" s="169" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="199"/>
+      <c r="B164" s="169"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
     </row>
@@ -7215,22 +7215,22 @@
       <c r="D165" s="2"/>
     </row>
     <row r="166" spans="1:7" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A166" s="200" t="s">
+      <c r="A166" s="174" t="s">
         <v>215</v>
       </c>
-      <c r="B166" s="200"/>
-      <c r="C166" s="168"/>
-      <c r="D166" s="168"/>
+      <c r="B166" s="174"/>
+      <c r="C166" s="176"/>
+      <c r="D166" s="176"/>
     </row>
     <row r="167" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="A167" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="B167" s="227" t="s">
+      <c r="B167" s="186" t="s">
         <v>428</v>
       </c>
-      <c r="C167" s="226"/>
-      <c r="D167" s="228"/>
+      <c r="C167" s="187"/>
+      <c r="D167" s="188"/>
       <c r="F167" t="s">
         <v>430</v>
       </c>
@@ -7242,12 +7242,12 @@
       <c r="D168" s="2"/>
     </row>
     <row r="169" spans="1:7" ht="75.75" customHeight="1">
-      <c r="A169" s="201" t="s">
+      <c r="A169" s="185" t="s">
         <v>217</v>
       </c>
-      <c r="B169" s="201"/>
-      <c r="C169" s="168"/>
-      <c r="D169" s="168"/>
+      <c r="B169" s="185"/>
+      <c r="C169" s="176"/>
+      <c r="D169" s="176"/>
       <c r="F169" t="s">
         <v>429</v>
       </c>
@@ -7279,7 +7279,7 @@
       <c r="C172" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="G172" s="229"/>
+      <c r="G172" s="168"/>
     </row>
     <row r="173" spans="1:7" ht="15.75" thickBot="1">
       <c r="A173" s="55" t="s">
@@ -7291,7 +7291,7 @@
       <c r="C173" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="G173" s="229"/>
+      <c r="G173" s="168"/>
     </row>
     <row r="174" spans="1:7" ht="15.75" thickBot="1">
       <c r="A174" s="55" t="s">
@@ -7305,20 +7305,20 @@
       </c>
     </row>
     <row r="175" spans="1:7">
-      <c r="A175" s="199"/>
-      <c r="B175" s="199"/>
+      <c r="A175" s="169"/>
+      <c r="B175" s="169"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="41"/>
       <c r="B176" s="41"/>
     </row>
     <row r="177" spans="1:6" ht="63" customHeight="1" thickBot="1">
-      <c r="A177" s="193" t="s">
+      <c r="A177" s="183" t="s">
         <v>220</v>
       </c>
-      <c r="B177" s="193"/>
-      <c r="C177" s="194"/>
-      <c r="D177" s="194"/>
+      <c r="B177" s="183"/>
+      <c r="C177" s="184"/>
+      <c r="D177" s="184"/>
     </row>
     <row r="178" spans="1:6" ht="26.25" customHeight="1" thickBot="1">
       <c r="A178" s="27" t="s">
@@ -7359,20 +7359,20 @@
       <c r="D181" s="57"/>
     </row>
     <row r="182" spans="1:6">
-      <c r="A182" s="207"/>
-      <c r="B182" s="207"/>
+      <c r="A182" s="181"/>
+      <c r="B182" s="181"/>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="43"/>
       <c r="B183" s="43"/>
     </row>
     <row r="184" spans="1:6" ht="54.75" customHeight="1">
-      <c r="A184" s="192" t="s">
+      <c r="A184" s="182" t="s">
         <v>267</v>
       </c>
-      <c r="B184" s="192"/>
-      <c r="C184" s="168"/>
-      <c r="D184" s="168"/>
+      <c r="B184" s="182"/>
+      <c r="C184" s="176"/>
+      <c r="D184" s="176"/>
       <c r="F184" t="s">
         <v>431</v>
       </c>
@@ -7420,12 +7420,12 @@
       <c r="D192" s="2"/>
     </row>
     <row r="193" spans="1:6" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A193" s="202" t="s">
+      <c r="A193" s="177" t="s">
         <v>223</v>
       </c>
-      <c r="B193" s="202"/>
-      <c r="C193" s="203"/>
-      <c r="D193" s="203"/>
+      <c r="B193" s="177"/>
+      <c r="C193" s="178"/>
+      <c r="D193" s="178"/>
     </row>
     <row r="194" spans="1:6" ht="15.75" thickBot="1">
       <c r="A194" s="24" t="s">
@@ -7474,8 +7474,8 @@
       <c r="D198" s="2"/>
     </row>
     <row r="199" spans="1:6">
-      <c r="A199" s="199"/>
-      <c r="B199" s="199"/>
+      <c r="A199" s="169"/>
+      <c r="B199" s="169"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
     </row>
@@ -7486,12 +7486,12 @@
       <c r="D200" s="2"/>
     </row>
     <row r="201" spans="1:6" ht="54.75" customHeight="1">
-      <c r="A201" s="204" t="s">
+      <c r="A201" s="172" t="s">
         <v>272</v>
       </c>
-      <c r="B201" s="204"/>
-      <c r="C201" s="169"/>
-      <c r="D201" s="169"/>
+      <c r="B201" s="172"/>
+      <c r="C201" s="173"/>
+      <c r="D201" s="173"/>
       <c r="F201" t="s">
         <v>435</v>
       </c>
@@ -7530,19 +7530,19 @@
       <c r="B207" s="57"/>
     </row>
     <row r="208" spans="1:6">
-      <c r="A208" s="199"/>
-      <c r="B208" s="199"/>
+      <c r="A208" s="169"/>
+      <c r="B208" s="169"/>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="45"/>
     </row>
     <row r="210" spans="1:4" ht="33" customHeight="1" thickBot="1">
-      <c r="A210" s="205" t="s">
+      <c r="A210" s="179" t="s">
         <v>273</v>
       </c>
-      <c r="B210" s="205"/>
-      <c r="C210" s="206"/>
-      <c r="D210" s="206"/>
+      <c r="B210" s="179"/>
+      <c r="C210" s="180"/>
+      <c r="D210" s="180"/>
     </row>
     <row r="211" spans="1:4" ht="15.75" thickBot="1">
       <c r="A211" s="27" t="s">
@@ -7591,12 +7591,12 @@
       <c r="B216" s="41"/>
     </row>
     <row r="217" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A217" s="200" t="s">
+      <c r="A217" s="174" t="s">
         <v>226</v>
       </c>
-      <c r="B217" s="200"/>
-      <c r="C217" s="168"/>
-      <c r="D217" s="168"/>
+      <c r="B217" s="174"/>
+      <c r="C217" s="176"/>
+      <c r="D217" s="176"/>
     </row>
     <row r="218" spans="1:4" ht="45">
       <c r="A218" s="46" t="s">
@@ -7607,12 +7607,12 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="36" customHeight="1">
-      <c r="A220" s="204" t="s">
+      <c r="A220" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="B220" s="204"/>
-      <c r="C220" s="169"/>
-      <c r="D220" s="169"/>
+      <c r="B220" s="172"/>
+      <c r="C220" s="173"/>
+      <c r="D220" s="173"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="46" t="s">
@@ -7634,12 +7634,12 @@
       </c>
     </row>
     <row r="224" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A224" s="204" t="s">
+      <c r="A224" s="172" t="s">
         <v>229</v>
       </c>
-      <c r="B224" s="204"/>
-      <c r="C224" s="169"/>
-      <c r="D224" s="169"/>
+      <c r="B224" s="172"/>
+      <c r="C224" s="173"/>
+      <c r="D224" s="173"/>
     </row>
     <row r="225" spans="1:6" ht="90">
       <c r="A225" s="46" t="s">
@@ -7655,12 +7655,12 @@
       </c>
     </row>
     <row r="228" spans="1:6" ht="49.5" customHeight="1">
-      <c r="A228" s="204" t="s">
+      <c r="A228" s="172" t="s">
         <v>230</v>
       </c>
-      <c r="B228" s="204"/>
-      <c r="C228" s="169"/>
-      <c r="D228" s="169"/>
+      <c r="B228" s="172"/>
+      <c r="C228" s="173"/>
+      <c r="D228" s="173"/>
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="46" t="s">
@@ -7679,12 +7679,12 @@
       </c>
     </row>
     <row r="231" spans="1:6" ht="33" customHeight="1">
-      <c r="A231" s="204" t="s">
+      <c r="A231" s="172" t="s">
         <v>231</v>
       </c>
-      <c r="B231" s="204"/>
-      <c r="C231" s="169"/>
-      <c r="D231" s="169"/>
+      <c r="B231" s="172"/>
+      <c r="C231" s="173"/>
+      <c r="D231" s="173"/>
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="46" t="s">
@@ -7695,12 +7695,12 @@
       </c>
     </row>
     <row r="234" spans="1:6" ht="41.25" customHeight="1">
-      <c r="A234" s="204" t="s">
+      <c r="A234" s="172" t="s">
         <v>232</v>
       </c>
-      <c r="B234" s="204"/>
-      <c r="C234" s="169"/>
-      <c r="D234" s="169"/>
+      <c r="B234" s="172"/>
+      <c r="C234" s="173"/>
+      <c r="D234" s="173"/>
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="46" t="s">
@@ -7711,12 +7711,12 @@
       </c>
     </row>
     <row r="237" spans="1:6" ht="38.25" customHeight="1">
-      <c r="A237" s="200" t="s">
+      <c r="A237" s="174" t="s">
         <v>233</v>
       </c>
-      <c r="B237" s="200"/>
-      <c r="C237" s="169"/>
-      <c r="D237" s="169"/>
+      <c r="B237" s="174"/>
+      <c r="C237" s="173"/>
+      <c r="D237" s="173"/>
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="46" t="s">
@@ -7732,12 +7732,12 @@
       </c>
     </row>
     <row r="241" spans="1:4" ht="45" customHeight="1">
-      <c r="A241" s="204" t="s">
+      <c r="A241" s="172" t="s">
         <v>234</v>
       </c>
-      <c r="B241" s="204"/>
-      <c r="C241" s="169"/>
-      <c r="D241" s="169"/>
+      <c r="B241" s="172"/>
+      <c r="C241" s="173"/>
+      <c r="D241" s="173"/>
     </row>
     <row r="242" spans="1:4">
       <c r="A242" s="46" t="s">
@@ -7753,12 +7753,12 @@
       </c>
     </row>
     <row r="245" spans="1:4" ht="42" customHeight="1">
-      <c r="A245" s="208" t="s">
+      <c r="A245" s="175" t="s">
         <v>235</v>
       </c>
-      <c r="B245" s="208"/>
-      <c r="C245" s="169"/>
-      <c r="D245" s="169"/>
+      <c r="B245" s="175"/>
+      <c r="C245" s="173"/>
+      <c r="D245" s="173"/>
     </row>
     <row r="246" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="247" spans="1:4" ht="15.75" thickBot="1">
@@ -7811,10 +7811,10 @@
       </c>
     </row>
     <row r="254" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A254" s="204" t="s">
+      <c r="A254" s="172" t="s">
         <v>238</v>
       </c>
-      <c r="B254" s="169"/>
+      <c r="B254" s="173"/>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" s="49"/>
@@ -7825,12 +7825,12 @@
       </c>
     </row>
     <row r="257" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A257" s="204" t="s">
+      <c r="A257" s="172" t="s">
         <v>239</v>
       </c>
-      <c r="B257" s="204"/>
-      <c r="C257" s="169"/>
-      <c r="D257" s="169"/>
+      <c r="B257" s="172"/>
+      <c r="C257" s="173"/>
+      <c r="D257" s="173"/>
     </row>
     <row r="258" spans="1:4">
       <c r="A258" s="46" t="s">
@@ -7838,12 +7838,12 @@
       </c>
     </row>
     <row r="260" spans="1:4">
-      <c r="A260" s="204" t="s">
+      <c r="A260" s="172" t="s">
         <v>240</v>
       </c>
-      <c r="B260" s="204"/>
-      <c r="C260" s="169"/>
-      <c r="D260" s="169"/>
+      <c r="B260" s="172"/>
+      <c r="C260" s="173"/>
+      <c r="D260" s="173"/>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="46" t="s">
@@ -7852,16 +7852,16 @@
     </row>
     <row r="262" spans="1:4" ht="25.5" customHeight="1"/>
     <row r="263" spans="1:4" ht="49.5" customHeight="1">
-      <c r="A263" s="204" t="s">
+      <c r="A263" s="172" t="s">
         <v>241</v>
       </c>
-      <c r="B263" s="204"/>
+      <c r="B263" s="172"/>
     </row>
     <row r="264" spans="1:4" ht="59.25" customHeight="1">
-      <c r="A264" s="204" t="s">
+      <c r="A264" s="172" t="s">
         <v>242</v>
       </c>
-      <c r="B264" s="204"/>
+      <c r="B264" s="172"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="46" t="s">
@@ -7869,12 +7869,12 @@
       </c>
     </row>
     <row r="267" spans="1:4" ht="55.5" customHeight="1" thickBot="1">
-      <c r="A267" s="198" t="s">
+      <c r="A267" s="170" t="s">
         <v>243</v>
       </c>
-      <c r="B267" s="198"/>
-      <c r="C267" s="209"/>
-      <c r="D267" s="209"/>
+      <c r="B267" s="170"/>
+      <c r="C267" s="171"/>
+      <c r="D267" s="171"/>
     </row>
     <row r="268" spans="1:4" ht="15.75" thickBot="1">
       <c r="A268" s="27" t="s">
@@ -7907,8 +7907,8 @@
       <c r="D270" s="12"/>
     </row>
     <row r="271" spans="1:4">
-      <c r="A271" s="199"/>
-      <c r="B271" s="199"/>
+      <c r="A271" s="169"/>
+      <c r="B271" s="169"/>
     </row>
     <row r="272" spans="1:4">
       <c r="A272" s="41"/>
@@ -7933,12 +7933,12 @@
       </c>
     </row>
     <row r="277" spans="1:4" ht="39" customHeight="1">
-      <c r="A277" s="204" t="s">
+      <c r="A277" s="172" t="s">
         <v>245</v>
       </c>
-      <c r="B277" s="204"/>
-      <c r="C277" s="169"/>
-      <c r="D277" s="169"/>
+      <c r="B277" s="172"/>
+      <c r="C277" s="173"/>
+      <c r="D277" s="173"/>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" s="46" t="s">
@@ -7947,12 +7947,12 @@
       <c r="B278" s="8"/>
     </row>
     <row r="280" spans="1:4" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A280" s="198" t="s">
+      <c r="A280" s="170" t="s">
         <v>246</v>
       </c>
-      <c r="B280" s="198"/>
-      <c r="C280" s="209"/>
-      <c r="D280" s="209"/>
+      <c r="B280" s="170"/>
+      <c r="C280" s="171"/>
+      <c r="D280" s="171"/>
     </row>
     <row r="281" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="282" spans="1:4" ht="15.75" thickBot="1">
@@ -7995,54 +7995,6 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="A271:B271"/>
-    <mergeCell ref="A267:D267"/>
-    <mergeCell ref="A277:D277"/>
-    <mergeCell ref="A280:D280"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A264:B264"/>
-    <mergeCell ref="A254:B254"/>
-    <mergeCell ref="A257:D257"/>
-    <mergeCell ref="A260:D260"/>
-    <mergeCell ref="A231:D231"/>
-    <mergeCell ref="A234:D234"/>
-    <mergeCell ref="A237:D237"/>
-    <mergeCell ref="A245:D245"/>
-    <mergeCell ref="A241:D241"/>
-    <mergeCell ref="A217:D217"/>
-    <mergeCell ref="A220:D220"/>
-    <mergeCell ref="A224:D224"/>
-    <mergeCell ref="A228:D228"/>
-    <mergeCell ref="A199:B199"/>
-    <mergeCell ref="A208:B208"/>
-    <mergeCell ref="A193:D193"/>
-    <mergeCell ref="A201:D201"/>
-    <mergeCell ref="A210:D210"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="A184:D184"/>
-    <mergeCell ref="A177:D177"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A166:D166"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="A151:D151"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A117:C117"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A32:E32"/>
@@ -8058,6 +8010,54 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="A151:D151"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A117:C117"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="A193:D193"/>
+    <mergeCell ref="A201:D201"/>
+    <mergeCell ref="A210:D210"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="A184:D184"/>
+    <mergeCell ref="A177:D177"/>
+    <mergeCell ref="A217:D217"/>
+    <mergeCell ref="A220:D220"/>
+    <mergeCell ref="A224:D224"/>
+    <mergeCell ref="A228:D228"/>
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="A208:B208"/>
+    <mergeCell ref="A254:B254"/>
+    <mergeCell ref="A257:D257"/>
+    <mergeCell ref="A260:D260"/>
+    <mergeCell ref="A231:D231"/>
+    <mergeCell ref="A234:D234"/>
+    <mergeCell ref="A237:D237"/>
+    <mergeCell ref="A245:D245"/>
+    <mergeCell ref="A241:D241"/>
+    <mergeCell ref="A271:B271"/>
+    <mergeCell ref="A267:D267"/>
+    <mergeCell ref="A277:D277"/>
+    <mergeCell ref="A280:D280"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A264:B264"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8071,9 +8071,9 @@
   </sheetPr>
   <dimension ref="A1:XFD371"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8104,11 +8104,11 @@
       <c r="D1" s="108" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="221" t="s">
+      <c r="E1" s="214" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="221"/>
-      <c r="G1" s="221"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="214"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
@@ -8190,15 +8190,15 @@
       <c r="P3" s="109"/>
     </row>
     <row r="4" spans="1:26 16384:16384" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A4" s="222" t="s">
+      <c r="A4" s="215" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
+      <c r="B4" s="215"/>
+      <c r="C4" s="215"/>
+      <c r="D4" s="215"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="215"/>
+      <c r="G4" s="215"/>
       <c r="H4" s="152"/>
       <c r="I4" s="153"/>
       <c r="J4" s="153"/>
@@ -8267,12 +8267,12 @@
       <c r="N6" s="97"/>
       <c r="O6" s="97"/>
       <c r="P6" s="97"/>
-      <c r="R6" s="210" t="s">
+      <c r="R6" s="222" t="s">
         <v>285</v>
       </c>
-      <c r="S6" s="211"/>
-      <c r="T6" s="211"/>
-      <c r="U6" s="211"/>
+      <c r="S6" s="223"/>
+      <c r="T6" s="223"/>
+      <c r="U6" s="223"/>
     </row>
     <row r="7" spans="1:26 16384:16384" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="110" t="s">
@@ -8301,10 +8301,10 @@
       <c r="N7" s="65"/>
       <c r="O7" s="66"/>
       <c r="P7" s="66"/>
-      <c r="R7" s="211"/>
-      <c r="S7" s="211"/>
-      <c r="T7" s="211"/>
-      <c r="U7" s="211"/>
+      <c r="R7" s="223"/>
+      <c r="S7" s="223"/>
+      <c r="T7" s="223"/>
+      <c r="U7" s="223"/>
     </row>
     <row r="8" spans="1:26 16384:16384" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="110" t="s">
@@ -8331,10 +8331,10 @@
       <c r="N8" s="64"/>
       <c r="O8" s="64"/>
       <c r="P8" s="64"/>
-      <c r="R8" s="211"/>
-      <c r="S8" s="211"/>
-      <c r="T8" s="211"/>
-      <c r="U8" s="211"/>
+      <c r="R8" s="223"/>
+      <c r="S8" s="223"/>
+      <c r="T8" s="223"/>
+      <c r="U8" s="223"/>
     </row>
     <row r="9" spans="1:26 16384:16384" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A9" s="110" t="s">
@@ -8361,10 +8361,10 @@
       <c r="N9" s="64"/>
       <c r="O9" s="64"/>
       <c r="P9" s="64"/>
-      <c r="R9" s="211"/>
-      <c r="S9" s="211"/>
-      <c r="T9" s="211"/>
-      <c r="U9" s="211"/>
+      <c r="R9" s="223"/>
+      <c r="S9" s="223"/>
+      <c r="T9" s="223"/>
+      <c r="U9" s="223"/>
     </row>
     <row r="10" spans="1:26 16384:16384" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A10" s="110" t="s">
@@ -8391,10 +8391,10 @@
       <c r="N10" s="64"/>
       <c r="O10" s="64"/>
       <c r="P10" s="64"/>
-      <c r="R10" s="211"/>
-      <c r="S10" s="211"/>
-      <c r="T10" s="211"/>
-      <c r="U10" s="211"/>
+      <c r="R10" s="223"/>
+      <c r="S10" s="223"/>
+      <c r="T10" s="223"/>
+      <c r="U10" s="223"/>
       <c r="XFD10" s="75"/>
     </row>
     <row r="11" spans="1:26 16384:16384" s="18" customFormat="1" ht="30.75" thickBot="1">
@@ -8422,10 +8422,10 @@
       <c r="N11" s="64"/>
       <c r="O11" s="64"/>
       <c r="P11" s="64"/>
-      <c r="R11" s="211"/>
-      <c r="S11" s="211"/>
-      <c r="T11" s="211"/>
-      <c r="U11" s="211"/>
+      <c r="R11" s="223"/>
+      <c r="S11" s="223"/>
+      <c r="T11" s="223"/>
+      <c r="U11" s="223"/>
     </row>
     <row r="12" spans="1:26 16384:16384" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A12" s="110" t="s">
@@ -8452,10 +8452,10 @@
       <c r="N12" s="64"/>
       <c r="O12" s="64"/>
       <c r="P12" s="64"/>
-      <c r="R12" s="211"/>
-      <c r="S12" s="211"/>
-      <c r="T12" s="211"/>
-      <c r="U12" s="211"/>
+      <c r="R12" s="223"/>
+      <c r="S12" s="223"/>
+      <c r="T12" s="223"/>
+      <c r="U12" s="223"/>
     </row>
     <row r="13" spans="1:26 16384:16384" s="18" customFormat="1" ht="30.75" thickBot="1">
       <c r="A13" s="110" t="s">
@@ -8483,10 +8483,10 @@
       <c r="O13" s="64"/>
       <c r="P13" s="64"/>
       <c r="Q13" s="19"/>
-      <c r="R13" s="211"/>
-      <c r="S13" s="211"/>
-      <c r="T13" s="211"/>
-      <c r="U13" s="211"/>
+      <c r="R13" s="223"/>
+      <c r="S13" s="223"/>
+      <c r="T13" s="223"/>
+      <c r="U13" s="223"/>
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
       <c r="X13" s="19"/>
@@ -8519,10 +8519,10 @@
       <c r="O14" s="72"/>
       <c r="P14" s="72"/>
       <c r="Q14" s="19"/>
-      <c r="R14" s="211"/>
-      <c r="S14" s="211"/>
-      <c r="T14" s="211"/>
-      <c r="U14" s="211"/>
+      <c r="R14" s="223"/>
+      <c r="S14" s="223"/>
+      <c r="T14" s="223"/>
+      <c r="U14" s="223"/>
       <c r="V14" s="19"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
@@ -8555,10 +8555,10 @@
       <c r="O15" s="72"/>
       <c r="P15" s="72"/>
       <c r="Q15" s="19"/>
-      <c r="R15" s="211"/>
-      <c r="S15" s="211"/>
-      <c r="T15" s="211"/>
-      <c r="U15" s="211"/>
+      <c r="R15" s="223"/>
+      <c r="S15" s="223"/>
+      <c r="T15" s="223"/>
+      <c r="U15" s="223"/>
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
@@ -8591,10 +8591,10 @@
       <c r="O16" s="72"/>
       <c r="P16" s="72"/>
       <c r="Q16" s="19"/>
-      <c r="R16" s="211"/>
-      <c r="S16" s="211"/>
-      <c r="T16" s="211"/>
-      <c r="U16" s="211"/>
+      <c r="R16" s="223"/>
+      <c r="S16" s="223"/>
+      <c r="T16" s="223"/>
+      <c r="U16" s="223"/>
       <c r="V16" s="19"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
@@ -8627,10 +8627,10 @@
       <c r="O17" s="72"/>
       <c r="P17" s="72"/>
       <c r="Q17" s="19"/>
-      <c r="R17" s="211"/>
-      <c r="S17" s="211"/>
-      <c r="T17" s="211"/>
-      <c r="U17" s="211"/>
+      <c r="R17" s="223"/>
+      <c r="S17" s="223"/>
+      <c r="T17" s="223"/>
+      <c r="U17" s="223"/>
       <c r="V17" s="19"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
@@ -8962,15 +8962,15 @@
       <c r="Z26" s="19"/>
     </row>
     <row r="27" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A27" s="212" t="s">
+      <c r="A27" s="216" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="213"/>
-      <c r="C27" s="213"/>
-      <c r="D27" s="213"/>
-      <c r="E27" s="213"/>
-      <c r="F27" s="213"/>
-      <c r="G27" s="213"/>
+      <c r="B27" s="217"/>
+      <c r="C27" s="217"/>
+      <c r="D27" s="217"/>
+      <c r="E27" s="217"/>
+      <c r="F27" s="217"/>
+      <c r="G27" s="217"/>
       <c r="H27" s="141"/>
       <c r="I27" s="142"/>
       <c r="J27" s="142"/>
@@ -9280,15 +9280,15 @@
       <c r="Z35" s="19"/>
     </row>
     <row r="36" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A36" s="212" t="s">
+      <c r="A36" s="216" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="213"/>
-      <c r="C36" s="214"/>
-      <c r="D36" s="213"/>
-      <c r="E36" s="213"/>
-      <c r="F36" s="213"/>
-      <c r="G36" s="214"/>
+      <c r="B36" s="217"/>
+      <c r="C36" s="218"/>
+      <c r="D36" s="217"/>
+      <c r="E36" s="217"/>
+      <c r="F36" s="217"/>
+      <c r="G36" s="218"/>
       <c r="H36" s="141"/>
       <c r="I36" s="142"/>
       <c r="J36" s="142"/>
@@ -9382,11 +9382,11 @@
       <c r="Z38" s="19"/>
     </row>
     <row r="39" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A39" s="223" t="s">
+      <c r="A39" s="219" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="224"/>
-      <c r="C39" s="225"/>
+      <c r="B39" s="220"/>
+      <c r="C39" s="221"/>
       <c r="D39" s="126"/>
       <c r="E39" s="127"/>
       <c r="F39" s="127"/>
@@ -10484,15 +10484,15 @@
       <c r="Z69" s="19"/>
     </row>
     <row r="70" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A70" s="212" t="s">
+      <c r="A70" s="216" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="213"/>
-      <c r="C70" s="213"/>
-      <c r="D70" s="214"/>
-      <c r="E70" s="213"/>
-      <c r="F70" s="213"/>
-      <c r="G70" s="213"/>
+      <c r="B70" s="217"/>
+      <c r="C70" s="217"/>
+      <c r="D70" s="218"/>
+      <c r="E70" s="217"/>
+      <c r="F70" s="217"/>
+      <c r="G70" s="217"/>
       <c r="H70" s="141"/>
       <c r="I70" s="142"/>
       <c r="J70" s="142"/>
@@ -10910,15 +10910,15 @@
       <c r="Z81" s="19"/>
     </row>
     <row r="82" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A82" s="212" t="s">
+      <c r="A82" s="216" t="s">
         <v>135</v>
       </c>
-      <c r="B82" s="214"/>
-      <c r="C82" s="214"/>
-      <c r="D82" s="215"/>
-      <c r="E82" s="213"/>
-      <c r="F82" s="213"/>
-      <c r="G82" s="213"/>
+      <c r="B82" s="218"/>
+      <c r="C82" s="218"/>
+      <c r="D82" s="224"/>
+      <c r="E82" s="217"/>
+      <c r="F82" s="217"/>
+      <c r="G82" s="217"/>
       <c r="H82" s="141"/>
       <c r="I82" s="142"/>
       <c r="J82" s="142"/>
@@ -11120,15 +11120,15 @@
       <c r="Z87" s="19"/>
     </row>
     <row r="88" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A88" s="212" t="s">
+      <c r="A88" s="216" t="s">
         <v>141</v>
       </c>
-      <c r="B88" s="214"/>
-      <c r="C88" s="215"/>
-      <c r="D88" s="215"/>
-      <c r="E88" s="213"/>
-      <c r="F88" s="213"/>
-      <c r="G88" s="213"/>
+      <c r="B88" s="218"/>
+      <c r="C88" s="224"/>
+      <c r="D88" s="224"/>
+      <c r="E88" s="217"/>
+      <c r="F88" s="217"/>
+      <c r="G88" s="217"/>
       <c r="H88" s="141"/>
       <c r="I88" s="142"/>
       <c r="J88" s="142"/>
@@ -11330,15 +11330,15 @@
       <c r="Z93" s="19"/>
     </row>
     <row r="94" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A94" s="216" t="s">
+      <c r="A94" s="225" t="s">
         <v>147</v>
       </c>
-      <c r="B94" s="217"/>
-      <c r="C94" s="218"/>
-      <c r="D94" s="218"/>
-      <c r="E94" s="219"/>
-      <c r="F94" s="219"/>
-      <c r="G94" s="219"/>
+      <c r="B94" s="226"/>
+      <c r="C94" s="227"/>
+      <c r="D94" s="227"/>
+      <c r="E94" s="228"/>
+      <c r="F94" s="228"/>
+      <c r="G94" s="228"/>
       <c r="H94" s="141"/>
       <c r="I94" s="142"/>
       <c r="J94" s="142"/>
@@ -11432,15 +11432,15 @@
       <c r="Z96" s="19"/>
     </row>
     <row r="97" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A97" s="212" t="s">
+      <c r="A97" s="216" t="s">
         <v>150</v>
       </c>
-      <c r="B97" s="213"/>
-      <c r="C97" s="213"/>
-      <c r="D97" s="213"/>
-      <c r="E97" s="213"/>
-      <c r="F97" s="213"/>
-      <c r="G97" s="213"/>
+      <c r="B97" s="217"/>
+      <c r="C97" s="217"/>
+      <c r="D97" s="217"/>
+      <c r="E97" s="217"/>
+      <c r="F97" s="217"/>
+      <c r="G97" s="217"/>
       <c r="H97" s="141"/>
       <c r="I97" s="142"/>
       <c r="J97" s="142"/>
@@ -11498,15 +11498,15 @@
       <c r="Z98" s="19"/>
     </row>
     <row r="99" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A99" s="212" t="s">
+      <c r="A99" s="216" t="s">
         <v>152</v>
       </c>
-      <c r="B99" s="214"/>
-      <c r="C99" s="214"/>
-      <c r="D99" s="214"/>
-      <c r="E99" s="213"/>
-      <c r="F99" s="213"/>
-      <c r="G99" s="213"/>
+      <c r="B99" s="218"/>
+      <c r="C99" s="218"/>
+      <c r="D99" s="218"/>
+      <c r="E99" s="217"/>
+      <c r="F99" s="217"/>
+      <c r="G99" s="217"/>
       <c r="H99" s="141"/>
       <c r="I99" s="142"/>
       <c r="J99" s="142"/>
@@ -11636,15 +11636,15 @@
       <c r="Z102" s="19"/>
     </row>
     <row r="103" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A103" s="220" t="s">
+      <c r="A103" s="229" t="s">
         <v>157</v>
       </c>
-      <c r="B103" s="215"/>
-      <c r="C103" s="215"/>
-      <c r="D103" s="215"/>
-      <c r="E103" s="214"/>
-      <c r="F103" s="214"/>
-      <c r="G103" s="214"/>
+      <c r="B103" s="224"/>
+      <c r="C103" s="224"/>
+      <c r="D103" s="224"/>
+      <c r="E103" s="218"/>
+      <c r="F103" s="218"/>
+      <c r="G103" s="218"/>
       <c r="H103" s="141"/>
       <c r="I103" s="142"/>
       <c r="J103" s="142"/>
@@ -11810,15 +11810,15 @@
       <c r="Z107" s="19"/>
     </row>
     <row r="108" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A108" s="212" t="s">
+      <c r="A108" s="216" t="s">
         <v>162</v>
       </c>
-      <c r="B108" s="214"/>
-      <c r="C108" s="215"/>
-      <c r="D108" s="215"/>
-      <c r="E108" s="213"/>
-      <c r="F108" s="213"/>
-      <c r="G108" s="213"/>
+      <c r="B108" s="218"/>
+      <c r="C108" s="224"/>
+      <c r="D108" s="224"/>
+      <c r="E108" s="217"/>
+      <c r="F108" s="217"/>
+      <c r="G108" s="217"/>
       <c r="H108" s="141"/>
       <c r="I108" s="142"/>
       <c r="J108" s="142"/>
@@ -11982,15 +11982,15 @@
       <c r="Z112" s="19"/>
     </row>
     <row r="113" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A113" s="212" t="s">
+      <c r="A113" s="216" t="s">
         <v>168</v>
       </c>
-      <c r="B113" s="214"/>
-      <c r="C113" s="215"/>
-      <c r="D113" s="215"/>
-      <c r="E113" s="213"/>
-      <c r="F113" s="213"/>
-      <c r="G113" s="213"/>
+      <c r="B113" s="218"/>
+      <c r="C113" s="224"/>
+      <c r="D113" s="224"/>
+      <c r="E113" s="217"/>
+      <c r="F113" s="217"/>
+      <c r="G113" s="217"/>
       <c r="H113" s="141"/>
       <c r="I113" s="142"/>
       <c r="J113" s="142"/>
@@ -15947,11 +15947,6 @@
   </sheetData>
   <autoFilter ref="B1:B473" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="15">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A39:C39"/>
     <mergeCell ref="R6:U17"/>
     <mergeCell ref="A70:G70"/>
     <mergeCell ref="A108:G108"/>
@@ -15962,6 +15957,11 @@
     <mergeCell ref="A97:G97"/>
     <mergeCell ref="A99:G99"/>
     <mergeCell ref="A103:G103"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="36" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
auto commit @14.11.2020: 13:22:27,25
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
+++ b/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95103779-533D-4953-9E2A-61050ADBCCBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EE596E-1757-45F4-B323-43B7638A0A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,25 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Documentation'!$B$1:$B$473</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Test Documentation'!$A$1:$P$116</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="454">
   <si>
     <t>TR.A.1</t>
   </si>
@@ -3979,6 +3987,39 @@
   </si>
   <si>
     <t>https://openwrt.org/docs/guide-user/base-system/dhcp_configuration</t>
+  </si>
+  <si>
+    <t>browseer</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>oder über git hash</t>
+  </si>
+  <si>
+    <t>https://openwrt.org/docs/guide-developer/security</t>
+  </si>
+  <si>
+    <t>https://openwrt.org/faq/how_to_get_a_list_of_connected_clients</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>siehe TR.D.28</t>
+  </si>
+  <si>
+    <t>shows md5 + sha2 for user to check. Uses simple checks with hardcoded metadata to verify that the firmware is correct for the device</t>
+  </si>
+  <si>
+    <t>no signature</t>
+  </si>
+  <si>
+    <t>can be installed</t>
+  </si>
+  <si>
+    <t>can be installed? Danish?</t>
   </si>
 </sst>
 </file>
@@ -8071,9 +8112,9 @@
   </sheetPr>
   <dimension ref="A1:XFD371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8319,7 +8360,9 @@
       <c r="D8" s="110" t="s">
         <v>288</v>
       </c>
-      <c r="E8" s="113"/>
+      <c r="E8" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="F8" s="113"/>
       <c r="G8" s="113"/>
       <c r="H8" s="74"/>
@@ -8349,7 +8392,9 @@
       <c r="D9" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="E9" s="113"/>
+      <c r="E9" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="F9" s="113"/>
       <c r="G9" s="113"/>
       <c r="H9" s="67"/>
@@ -8379,7 +8424,9 @@
       <c r="D10" s="110" t="s">
         <v>288</v>
       </c>
-      <c r="E10" s="113"/>
+      <c r="E10" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="F10" s="113"/>
       <c r="G10" s="113"/>
       <c r="H10" s="67"/>
@@ -8411,7 +8458,9 @@
         <v>290</v>
       </c>
       <c r="E11" s="113"/>
-      <c r="F11" s="113"/>
+      <c r="F11" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="G11" s="113"/>
       <c r="H11" s="67"/>
       <c r="I11" s="76"/>
@@ -8440,7 +8489,9 @@
       <c r="D12" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="E12" s="113"/>
+      <c r="E12" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="F12" s="113"/>
       <c r="G12" s="113"/>
       <c r="H12" s="67"/>
@@ -8468,9 +8519,11 @@
         <v>312</v>
       </c>
       <c r="D13" s="110" t="s">
-        <v>291</v>
-      </c>
-      <c r="E13" s="113"/>
+        <v>443</v>
+      </c>
+      <c r="E13" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="F13" s="113"/>
       <c r="G13" s="113"/>
       <c r="H13" s="67"/>
@@ -8507,7 +8560,9 @@
         <v>286</v>
       </c>
       <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
+      <c r="F14" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="G14" s="115"/>
       <c r="H14" s="69"/>
       <c r="I14" s="69"/>
@@ -8543,7 +8598,9 @@
         <v>286</v>
       </c>
       <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
+      <c r="F15" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="G15" s="115"/>
       <c r="H15" s="69"/>
       <c r="I15" s="69"/>
@@ -8614,7 +8671,9 @@
       <c r="D17" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="E17" s="113"/>
+      <c r="E17" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="F17" s="113"/>
       <c r="G17" s="115"/>
       <c r="H17" s="69"/>
@@ -8650,10 +8709,14 @@
       <c r="D18" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E18" s="119"/>
+      <c r="E18" s="119" t="s">
+        <v>280</v>
+      </c>
       <c r="F18" s="113"/>
       <c r="G18" s="115"/>
-      <c r="H18" s="69"/>
+      <c r="H18" s="69" t="s">
+        <v>444</v>
+      </c>
       <c r="I18" s="84"/>
       <c r="J18" s="85"/>
       <c r="K18" s="82"/>
@@ -8723,7 +8786,9 @@
         <v>292</v>
       </c>
       <c r="E20" s="119"/>
-      <c r="F20" s="113"/>
+      <c r="F20" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="G20" s="115"/>
       <c r="H20" s="86"/>
       <c r="I20" s="86"/>
@@ -8759,7 +8824,9 @@
         <v>286</v>
       </c>
       <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
+      <c r="F21" s="113" t="s">
+        <v>280</v>
+      </c>
       <c r="G21" s="115"/>
       <c r="H21" s="84"/>
       <c r="I21" s="84"/>
@@ -9006,7 +9073,9 @@
       </c>
       <c r="E28" s="121"/>
       <c r="F28" s="121"/>
-      <c r="G28" s="90"/>
+      <c r="G28" s="90" t="s">
+        <v>280</v>
+      </c>
       <c r="H28" s="82"/>
       <c r="I28" s="82"/>
       <c r="J28" s="82"/>
@@ -9040,7 +9109,9 @@
       <c r="D29" s="110" t="s">
         <v>293</v>
       </c>
-      <c r="E29" s="121"/>
+      <c r="E29" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F29" s="121"/>
       <c r="G29" s="90"/>
       <c r="H29" s="69"/>
@@ -9076,7 +9147,9 @@
       <c r="D30" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="E30" s="121"/>
+      <c r="E30" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F30" s="121"/>
       <c r="G30" s="90"/>
       <c r="H30" s="69"/>
@@ -9113,7 +9186,9 @@
         <v>286</v>
       </c>
       <c r="E31" s="121"/>
-      <c r="F31" s="121"/>
+      <c r="F31" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G31" s="90"/>
       <c r="H31" s="82"/>
       <c r="I31" s="82"/>
@@ -9148,7 +9223,9 @@
       <c r="D32" s="110" t="s">
         <v>288</v>
       </c>
-      <c r="E32" s="121"/>
+      <c r="E32" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F32" s="121"/>
       <c r="G32" s="90"/>
       <c r="H32" s="69"/>
@@ -9184,7 +9261,9 @@
       <c r="D33" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="E33" s="121"/>
+      <c r="E33" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F33" s="121"/>
       <c r="G33" s="90"/>
       <c r="H33" s="69"/>
@@ -9220,7 +9299,9 @@
       <c r="D34" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="E34" s="121"/>
+      <c r="E34" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F34" s="121"/>
       <c r="G34" s="90"/>
       <c r="H34" s="69"/>
@@ -9256,7 +9337,9 @@
       <c r="D35" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="E35" s="121"/>
+      <c r="E35" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F35" s="121"/>
       <c r="G35" s="90"/>
       <c r="H35" s="69"/>
@@ -9322,7 +9405,9 @@
       <c r="D37" s="124" t="s">
         <v>292</v>
       </c>
-      <c r="E37" s="121"/>
+      <c r="E37" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F37" s="90"/>
       <c r="G37" s="122"/>
       <c r="H37" s="69"/>
@@ -9358,7 +9443,9 @@
       <c r="D38" s="124" t="s">
         <v>286</v>
       </c>
-      <c r="E38" s="121"/>
+      <c r="E38" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F38" s="90"/>
       <c r="G38" s="122"/>
       <c r="H38" s="69"/>
@@ -9420,7 +9507,9 @@
         <v>91</v>
       </c>
       <c r="D40" s="118"/>
-      <c r="E40" s="129"/>
+      <c r="E40" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F40" s="121"/>
       <c r="G40" s="90"/>
       <c r="H40" s="69"/>
@@ -9456,7 +9545,9 @@
       <c r="D41" s="118" t="s">
         <v>294</v>
       </c>
-      <c r="E41" s="129"/>
+      <c r="E41" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F41" s="121"/>
       <c r="G41" s="90"/>
       <c r="H41" s="69"/>
@@ -9492,7 +9583,9 @@
       <c r="D42" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E42" s="129"/>
+      <c r="E42" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F42" s="121"/>
       <c r="G42" s="90"/>
       <c r="H42" s="69"/>
@@ -9600,7 +9693,9 @@
       <c r="D45" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E45" s="129"/>
+      <c r="E45" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F45" s="121"/>
       <c r="G45" s="90"/>
       <c r="H45" s="69"/>
@@ -9636,7 +9731,9 @@
       <c r="D46" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E46" s="129"/>
+      <c r="E46" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F46" s="121"/>
       <c r="G46" s="90"/>
       <c r="H46" s="69"/>
@@ -9674,7 +9771,9 @@
       </c>
       <c r="E47" s="129"/>
       <c r="F47" s="121"/>
-      <c r="G47" s="90"/>
+      <c r="G47" s="90" t="s">
+        <v>280</v>
+      </c>
       <c r="H47" s="69"/>
       <c r="I47" s="69"/>
       <c r="J47" s="69"/>
@@ -9708,7 +9807,9 @@
       <c r="D48" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E48" s="129"/>
+      <c r="E48" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F48" s="121"/>
       <c r="G48" s="90"/>
       <c r="H48" s="69"/>
@@ -9744,7 +9845,9 @@
       <c r="D49" s="118" t="s">
         <v>295</v>
       </c>
-      <c r="E49" s="131"/>
+      <c r="E49" s="131" t="s">
+        <v>280</v>
+      </c>
       <c r="F49" s="121"/>
       <c r="G49" s="90"/>
       <c r="H49" s="69"/>
@@ -9780,7 +9883,9 @@
       <c r="D50" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E50" s="129"/>
+      <c r="E50" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F50" s="121"/>
       <c r="G50" s="90"/>
       <c r="H50" s="69"/>
@@ -9816,7 +9921,9 @@
       <c r="D51" s="118" t="s">
         <v>296</v>
       </c>
-      <c r="E51" s="129"/>
+      <c r="E51" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F51" s="121"/>
       <c r="G51" s="90"/>
       <c r="H51" s="82"/>
@@ -9852,7 +9959,9 @@
       <c r="D52" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E52" s="129"/>
+      <c r="E52" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F52" s="121"/>
       <c r="G52" s="90"/>
       <c r="H52" s="69"/>
@@ -9888,7 +9997,9 @@
       <c r="D53" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E53" s="129"/>
+      <c r="E53" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F53" s="121"/>
       <c r="G53" s="90"/>
       <c r="H53" s="69"/>
@@ -9926,7 +10037,9 @@
       </c>
       <c r="E54" s="129"/>
       <c r="F54" s="121"/>
-      <c r="G54" s="90"/>
+      <c r="G54" s="90" t="s">
+        <v>280</v>
+      </c>
       <c r="H54" s="82"/>
       <c r="I54" s="82"/>
       <c r="J54" s="82"/>
@@ -9962,7 +10075,9 @@
       </c>
       <c r="E55" s="129"/>
       <c r="F55" s="121"/>
-      <c r="G55" s="90"/>
+      <c r="G55" s="90" t="s">
+        <v>280</v>
+      </c>
       <c r="H55" s="82"/>
       <c r="I55" s="82"/>
       <c r="J55" s="82"/>
@@ -10066,7 +10181,9 @@
       </c>
       <c r="E58" s="129"/>
       <c r="F58" s="121"/>
-      <c r="G58" s="90"/>
+      <c r="G58" s="90" t="s">
+        <v>280</v>
+      </c>
       <c r="H58" s="82"/>
       <c r="I58" s="69"/>
       <c r="J58" s="69"/>
@@ -10100,7 +10217,9 @@
       <c r="D59" s="118" t="s">
         <v>288</v>
       </c>
-      <c r="E59" s="129"/>
+      <c r="E59" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F59" s="121"/>
       <c r="G59" s="90"/>
       <c r="H59" s="69"/>
@@ -10172,7 +10291,9 @@
       <c r="D61" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E61" s="129"/>
+      <c r="E61" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F61" s="121"/>
       <c r="G61" s="90"/>
       <c r="H61" s="69"/>
@@ -10180,7 +10301,9 @@
       <c r="J61" s="69"/>
       <c r="K61" s="69"/>
       <c r="L61" s="69"/>
-      <c r="M61" s="130"/>
+      <c r="M61" s="130" t="s">
+        <v>445</v>
+      </c>
       <c r="N61" s="71"/>
       <c r="O61" s="71"/>
       <c r="P61" s="70"/>
@@ -10244,7 +10367,9 @@
       <c r="D63" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E63" s="129"/>
+      <c r="E63" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F63" s="121"/>
       <c r="G63" s="90"/>
       <c r="H63" s="82"/>
@@ -10252,7 +10377,9 @@
       <c r="J63" s="82"/>
       <c r="K63" s="82"/>
       <c r="L63" s="82"/>
-      <c r="M63" s="130"/>
+      <c r="M63" s="130" t="s">
+        <v>446</v>
+      </c>
       <c r="N63" s="72"/>
       <c r="O63" s="72"/>
       <c r="P63" s="72"/>
@@ -10280,7 +10407,9 @@
       <c r="D64" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E64" s="129"/>
+      <c r="E64" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F64" s="121"/>
       <c r="G64" s="90"/>
       <c r="H64" s="69"/>
@@ -10317,7 +10446,9 @@
         <v>286</v>
       </c>
       <c r="E65" s="129"/>
-      <c r="F65" s="121"/>
+      <c r="F65" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G65" s="90"/>
       <c r="H65" s="69"/>
       <c r="I65" s="69"/>
@@ -10352,7 +10483,9 @@
       <c r="D66" s="118" t="s">
         <v>295</v>
       </c>
-      <c r="E66" s="129"/>
+      <c r="E66" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F66" s="121"/>
       <c r="G66" s="90"/>
       <c r="H66" s="69"/>
@@ -10388,7 +10521,9 @@
       <c r="D67" s="118" t="s">
         <v>295</v>
       </c>
-      <c r="E67" s="129"/>
+      <c r="E67" s="129" t="s">
+        <v>448</v>
+      </c>
       <c r="F67" s="121"/>
       <c r="G67" s="90"/>
       <c r="H67" s="69"/>
@@ -10411,7 +10546,7 @@
       <c r="Y67" s="19"/>
       <c r="Z67" s="19"/>
     </row>
-    <row r="68" spans="1:26" s="18" customFormat="1" ht="30.75" thickBot="1">
+    <row r="68" spans="1:26" s="18" customFormat="1" ht="45.75" thickBot="1">
       <c r="A68" s="110" t="s">
         <v>121</v>
       </c>
@@ -10424,7 +10559,9 @@
       <c r="D68" s="118" t="s">
         <v>295</v>
       </c>
-      <c r="E68" s="129"/>
+      <c r="E68" s="129" t="s">
+        <v>448</v>
+      </c>
       <c r="F68" s="121"/>
       <c r="G68" s="90"/>
       <c r="H68" s="69"/>
@@ -10432,7 +10569,9 @@
       <c r="J68" s="69"/>
       <c r="K68" s="69"/>
       <c r="L68" s="69"/>
-      <c r="M68" s="130"/>
+      <c r="M68" s="130" t="s">
+        <v>447</v>
+      </c>
       <c r="N68" s="71"/>
       <c r="O68" s="71"/>
       <c r="P68" s="71"/>
@@ -10460,7 +10599,9 @@
       <c r="D69" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E69" s="129"/>
+      <c r="E69" s="129" t="s">
+        <v>448</v>
+      </c>
       <c r="F69" s="121"/>
       <c r="G69" s="90"/>
       <c r="H69" s="69"/>
@@ -10468,7 +10609,9 @@
       <c r="J69" s="69"/>
       <c r="K69" s="69"/>
       <c r="L69" s="69"/>
-      <c r="M69" s="130"/>
+      <c r="M69" s="130" t="s">
+        <v>449</v>
+      </c>
       <c r="N69" s="71"/>
       <c r="O69" s="71"/>
       <c r="P69" s="70"/>
@@ -10526,7 +10669,9 @@
       <c r="D71" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E71" s="129"/>
+      <c r="E71" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F71" s="121"/>
       <c r="G71" s="90"/>
       <c r="H71" s="69"/>
@@ -10562,7 +10707,9 @@
       <c r="D72" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E72" s="129"/>
+      <c r="E72" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F72" s="121"/>
       <c r="G72" s="90"/>
       <c r="H72" s="69"/>
@@ -10598,7 +10745,9 @@
       <c r="D73" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E73" s="129"/>
+      <c r="E73" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F73" s="121"/>
       <c r="G73" s="90"/>
       <c r="H73" s="69"/>
@@ -10635,7 +10784,9 @@
         <v>286</v>
       </c>
       <c r="E74" s="129"/>
-      <c r="F74" s="121"/>
+      <c r="F74" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G74" s="90"/>
       <c r="H74" s="69"/>
       <c r="I74" s="69"/>
@@ -10657,7 +10808,7 @@
       <c r="Y74" s="19"/>
       <c r="Z74" s="19"/>
     </row>
-    <row r="75" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
+    <row r="75" spans="1:26" s="18" customFormat="1" ht="75.75" thickBot="1">
       <c r="A75" s="110" t="s">
         <v>128</v>
       </c>
@@ -10670,7 +10821,9 @@
       <c r="D75" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="E75" s="129"/>
+      <c r="E75" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F75" s="121"/>
       <c r="G75" s="90"/>
       <c r="H75" s="69"/>
@@ -10678,7 +10831,9 @@
       <c r="J75" s="69"/>
       <c r="K75" s="69"/>
       <c r="L75" s="69"/>
-      <c r="M75" s="130"/>
+      <c r="M75" s="130" t="s">
+        <v>450</v>
+      </c>
       <c r="N75" s="71"/>
       <c r="O75" s="71"/>
       <c r="P75" s="71"/>
@@ -10706,7 +10861,9 @@
       <c r="D76" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E76" s="129"/>
+      <c r="E76" s="129" t="s">
+        <v>448</v>
+      </c>
       <c r="F76" s="121"/>
       <c r="G76" s="90"/>
       <c r="H76" s="82"/>
@@ -10714,7 +10871,9 @@
       <c r="J76" s="69"/>
       <c r="K76" s="69"/>
       <c r="L76" s="69"/>
-      <c r="M76" s="130"/>
+      <c r="M76" s="130" t="s">
+        <v>451</v>
+      </c>
       <c r="N76" s="71"/>
       <c r="O76" s="71"/>
       <c r="P76" s="71"/>
@@ -10742,7 +10901,9 @@
       <c r="D77" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="E77" s="129"/>
+      <c r="E77" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F77" s="121"/>
       <c r="G77" s="90"/>
       <c r="H77" s="69"/>
@@ -10778,7 +10939,9 @@
       <c r="D78" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E78" s="129"/>
+      <c r="E78" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F78" s="121"/>
       <c r="G78" s="90"/>
       <c r="H78" s="69"/>
@@ -10814,7 +10977,9 @@
       <c r="D79" s="101" t="s">
         <v>291</v>
       </c>
-      <c r="E79" s="129"/>
+      <c r="E79" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F79" s="121"/>
       <c r="G79" s="90"/>
       <c r="H79" s="69"/>
@@ -10852,7 +11017,9 @@
       </c>
       <c r="E80" s="129"/>
       <c r="F80" s="121"/>
-      <c r="G80" s="90"/>
+      <c r="G80" s="90" t="s">
+        <v>280</v>
+      </c>
       <c r="H80" s="69"/>
       <c r="I80" s="69"/>
       <c r="J80" s="69"/>
@@ -10886,7 +11053,9 @@
       <c r="D81" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E81" s="129"/>
+      <c r="E81" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F81" s="121"/>
       <c r="G81" s="90"/>
       <c r="H81" s="69"/>
@@ -10952,7 +11121,9 @@
       <c r="D83" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E83" s="129"/>
+      <c r="E83" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F83" s="121"/>
       <c r="G83" s="90"/>
       <c r="H83" s="69"/>
@@ -10988,7 +11159,9 @@
       <c r="D84" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E84" s="129"/>
+      <c r="E84" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F84" s="121"/>
       <c r="G84" s="90"/>
       <c r="H84" s="69"/>
@@ -11024,7 +11197,9 @@
       <c r="D85" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="E85" s="129"/>
+      <c r="E85" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F85" s="121"/>
       <c r="G85" s="90"/>
       <c r="H85" s="69"/>
@@ -11060,7 +11235,9 @@
       <c r="D86" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E86" s="129"/>
+      <c r="E86" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F86" s="121"/>
       <c r="G86" s="90"/>
       <c r="H86" s="69"/>
@@ -11096,7 +11273,9 @@
       <c r="D87" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="E87" s="129"/>
+      <c r="E87" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F87" s="121"/>
       <c r="G87" s="90"/>
       <c r="H87" s="69"/>
@@ -11162,7 +11341,9 @@
       <c r="D89" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E89" s="129"/>
+      <c r="E89" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F89" s="121"/>
       <c r="G89" s="90"/>
       <c r="H89" s="69"/>
@@ -11198,7 +11379,9 @@
       <c r="D90" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="E90" s="129"/>
+      <c r="E90" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F90" s="121"/>
       <c r="G90" s="90"/>
       <c r="H90" s="69"/>
@@ -11234,7 +11417,9 @@
       <c r="D91" s="101" t="s">
         <v>301</v>
       </c>
-      <c r="E91" s="129"/>
+      <c r="E91" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F91" s="121"/>
       <c r="G91" s="90"/>
       <c r="H91" s="69"/>
@@ -11278,7 +11463,9 @@
       <c r="J92" s="69"/>
       <c r="K92" s="69"/>
       <c r="L92" s="69"/>
-      <c r="M92" s="116"/>
+      <c r="M92" s="116" t="s">
+        <v>452</v>
+      </c>
       <c r="N92" s="71"/>
       <c r="O92" s="71"/>
       <c r="P92" s="71"/>
@@ -11314,7 +11501,9 @@
       <c r="J93" s="69"/>
       <c r="K93" s="69"/>
       <c r="L93" s="69"/>
-      <c r="M93" s="116"/>
+      <c r="M93" s="116" t="s">
+        <v>453</v>
+      </c>
       <c r="N93" s="71"/>
       <c r="O93" s="71"/>
       <c r="P93" s="71"/>
@@ -11372,7 +11561,9 @@
       <c r="D95" s="124" t="s">
         <v>291</v>
       </c>
-      <c r="E95" s="121"/>
+      <c r="E95" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F95" s="121"/>
       <c r="G95" s="90"/>
       <c r="H95" s="69"/>
@@ -11408,7 +11599,9 @@
       <c r="D96" s="124" t="s">
         <v>286</v>
       </c>
-      <c r="E96" s="121"/>
+      <c r="E96" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F96" s="121"/>
       <c r="G96" s="90"/>
       <c r="H96" s="69"/>
@@ -11474,7 +11667,9 @@
       <c r="D98" s="104" t="s">
         <v>302</v>
       </c>
-      <c r="E98" s="121"/>
+      <c r="E98" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="F98" s="121"/>
       <c r="G98" s="90"/>
       <c r="H98" s="69"/>

</xml_diff>

<commit_message>
auto commit @14.11.2020: 17:52:32,94
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
+++ b/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EE596E-1757-45F4-B323-43B7638A0A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35403F2B-FF65-4411-A304-CCF19E5A5D77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="454">
   <si>
     <t>TR.A.1</t>
   </si>
@@ -4016,10 +4016,10 @@
     <t>no signature</t>
   </si>
   <si>
-    <t>can be installed</t>
-  </si>
-  <si>
     <t>can be installed? Danish?</t>
+  </si>
+  <si>
+    <t>can be installed. Not in standard installation</t>
   </si>
 </sst>
 </file>
@@ -5319,30 +5319,122 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -5351,100 +5443,50 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5454,18 +5496,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5475,36 +5505,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5810,19 +5810,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="88.5" customHeight="1">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="169" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="173"/>
-      <c r="K2" s="173"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1"/>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
@@ -5832,10 +5832,10 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A6" s="196" t="s">
+      <c r="A6" s="189" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="197"/>
+      <c r="B6" s="190"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -5885,70 +5885,70 @@
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A14" s="198" t="s">
+      <c r="A14" s="191" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="199"/>
+      <c r="B14" s="192"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="205" t="s">
+      <c r="B15" s="174" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="206"/>
-      <c r="D15" s="207"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="176"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1">
       <c r="A16" s="166" t="s">
         <v>401</v>
       </c>
-      <c r="B16" s="211" t="s">
+      <c r="B16" s="180" t="s">
         <v>405</v>
       </c>
-      <c r="C16" s="212"/>
-      <c r="D16" s="213"/>
+      <c r="C16" s="181"/>
+      <c r="D16" s="182"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="167" t="s">
         <v>400</v>
       </c>
-      <c r="B17" s="200" t="s">
+      <c r="B17" s="183" t="s">
         <v>406</v>
       </c>
-      <c r="C17" s="201"/>
-      <c r="D17" s="202"/>
+      <c r="C17" s="184"/>
+      <c r="D17" s="185"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1">
       <c r="A18" s="167" t="s">
         <v>399</v>
       </c>
-      <c r="B18" s="200" t="s">
+      <c r="B18" s="183" t="s">
         <v>404</v>
       </c>
-      <c r="C18" s="201"/>
-      <c r="D18" s="202"/>
+      <c r="C18" s="184"/>
+      <c r="D18" s="185"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1">
       <c r="A19" s="167" t="s">
         <v>402</v>
       </c>
-      <c r="B19" s="200" t="s">
+      <c r="B19" s="183" t="s">
         <v>408</v>
       </c>
-      <c r="C19" s="201"/>
-      <c r="D19" s="202"/>
+      <c r="C19" s="184"/>
+      <c r="D19" s="185"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1">
       <c r="A20" s="167" t="s">
         <v>403</v>
       </c>
-      <c r="B20" s="200" t="s">
+      <c r="B20" s="183" t="s">
         <v>407</v>
       </c>
-      <c r="C20" s="201"/>
-      <c r="D20" s="202"/>
+      <c r="C20" s="184"/>
+      <c r="D20" s="185"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
@@ -5956,70 +5956,70 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" customHeight="1" thickBot="1">
-      <c r="A23" s="203" t="s">
+      <c r="A23" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="204"/>
+      <c r="B23" s="172"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="208" t="s">
+      <c r="B24" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="209"/>
-      <c r="D24" s="210"/>
+      <c r="C24" s="178"/>
+      <c r="D24" s="179"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1">
       <c r="A25" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="B25" s="211" t="s">
+      <c r="B25" s="180" t="s">
         <v>405</v>
       </c>
-      <c r="C25" s="212"/>
-      <c r="D25" s="213"/>
+      <c r="C25" s="181"/>
+      <c r="D25" s="182"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1">
       <c r="A26" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="B26" s="200" t="s">
+      <c r="B26" s="183" t="s">
         <v>406</v>
       </c>
-      <c r="C26" s="201"/>
-      <c r="D26" s="202"/>
+      <c r="C26" s="184"/>
+      <c r="D26" s="185"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1">
       <c r="A27" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="B27" s="200" t="s">
+      <c r="B27" s="183" t="s">
         <v>404</v>
       </c>
-      <c r="C27" s="201"/>
-      <c r="D27" s="202"/>
+      <c r="C27" s="184"/>
+      <c r="D27" s="185"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1">
       <c r="A28" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="B28" s="200" t="s">
+      <c r="B28" s="183" t="s">
         <v>408</v>
       </c>
-      <c r="C28" s="201"/>
-      <c r="D28" s="202"/>
+      <c r="C28" s="184"/>
+      <c r="D28" s="185"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1">
       <c r="A29" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="B29" s="200" t="s">
+      <c r="B29" s="183" t="s">
         <v>407</v>
       </c>
-      <c r="C29" s="201"/>
-      <c r="D29" s="202"/>
+      <c r="C29" s="184"/>
+      <c r="D29" s="185"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="165"/>
@@ -6031,13 +6031,13 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="76.5" customHeight="1">
-      <c r="A32" s="193" t="s">
+      <c r="A32" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="176"/>
-      <c r="C32" s="176"/>
-      <c r="D32" s="176"/>
-      <c r="E32" s="176"/>
+      <c r="B32" s="169"/>
+      <c r="C32" s="169"/>
+      <c r="D32" s="169"/>
+      <c r="E32" s="169"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="35" spans="1:5" ht="15.75" thickBot="1">
@@ -6228,13 +6228,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="57" customHeight="1">
-      <c r="A48" s="193" t="s">
+      <c r="A48" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="193"/>
-      <c r="C48" s="193"/>
-      <c r="D48" s="193"/>
-      <c r="E48" s="193"/>
+      <c r="B48" s="173"/>
+      <c r="C48" s="173"/>
+      <c r="D48" s="173"/>
+      <c r="E48" s="173"/>
     </row>
     <row r="49" spans="1:5" ht="31.5" customHeight="1" thickBot="1"/>
     <row r="50" spans="1:5" ht="44.25" customHeight="1" thickBot="1">
@@ -6347,13 +6347,13 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A59" s="193" t="s">
+      <c r="A59" s="173" t="s">
         <v>177</v>
       </c>
-      <c r="B59" s="193"/>
-      <c r="C59" s="193"/>
-      <c r="D59" s="193"/>
-      <c r="E59" s="193"/>
+      <c r="B59" s="173"/>
+      <c r="C59" s="173"/>
+      <c r="D59" s="173"/>
+      <c r="E59" s="173"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="10"/>
@@ -6375,12 +6375,12 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="36" customHeight="1">
-      <c r="A64" s="193" t="s">
+      <c r="A64" s="173" t="s">
         <v>178</v>
       </c>
-      <c r="B64" s="193"/>
-      <c r="C64" s="193"/>
-      <c r="D64" s="193"/>
+      <c r="B64" s="173"/>
+      <c r="C64" s="173"/>
+      <c r="D64" s="173"/>
       <c r="E64" s="8"/>
     </row>
     <row r="66" spans="1:5">
@@ -6392,12 +6392,12 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="193" t="s">
+      <c r="A69" s="173" t="s">
         <v>179</v>
       </c>
-      <c r="B69" s="193"/>
-      <c r="C69" s="193"/>
-      <c r="D69" s="193"/>
+      <c r="B69" s="173"/>
+      <c r="C69" s="173"/>
+      <c r="D69" s="173"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="71" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
@@ -6478,13 +6478,13 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A80" s="194" t="s">
+      <c r="A80" s="186" t="s">
         <v>187</v>
       </c>
-      <c r="B80" s="194"/>
-      <c r="C80" s="190"/>
-      <c r="D80" s="190"/>
-      <c r="E80" s="190"/>
+      <c r="B80" s="186"/>
+      <c r="C80" s="187"/>
+      <c r="D80" s="187"/>
+      <c r="E80" s="187"/>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="82" spans="1:4" ht="35.25" customHeight="1" thickBot="1">
@@ -6578,10 +6578,10 @@
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="195" t="s">
+      <c r="A91" s="188" t="s">
         <v>192</v>
       </c>
-      <c r="B91" s="195"/>
+      <c r="B91" s="188"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
@@ -6597,12 +6597,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="70.5" customHeight="1">
-      <c r="A97" s="189" t="s">
+      <c r="A97" s="196" t="s">
         <v>195</v>
       </c>
-      <c r="B97" s="190"/>
-      <c r="C97" s="190"/>
-      <c r="D97" s="190"/>
+      <c r="B97" s="187"/>
+      <c r="C97" s="187"/>
+      <c r="D97" s="187"/>
     </row>
     <row r="98" spans="1:4" ht="15.75" thickBot="1">
       <c r="A98" t="s">
@@ -6718,12 +6718,12 @@
       <c r="D108" s="2"/>
     </row>
     <row r="109" spans="1:4" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A109" s="183" t="s">
+      <c r="A109" s="194" t="s">
         <v>199</v>
       </c>
-      <c r="B109" s="183"/>
-      <c r="C109" s="184"/>
-      <c r="D109" s="184"/>
+      <c r="B109" s="194"/>
+      <c r="C109" s="195"/>
+      <c r="D109" s="195"/>
     </row>
     <row r="110" spans="1:4" ht="15.75" thickBot="1">
       <c r="A110" s="27" t="s">
@@ -6784,9 +6784,9 @@
       <c r="D116" s="57"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="191"/>
-      <c r="B117" s="191"/>
-      <c r="C117" s="192"/>
+      <c r="A117" s="197"/>
+      <c r="B117" s="197"/>
+      <c r="C117" s="198"/>
       <c r="D117" s="2"/>
     </row>
     <row r="118" spans="1:4">
@@ -6804,12 +6804,12 @@
       <c r="D119" s="2"/>
     </row>
     <row r="120" spans="1:4" ht="113.25" customHeight="1" thickBot="1">
-      <c r="A120" s="182" t="s">
+      <c r="A120" s="193" t="s">
         <v>420</v>
       </c>
-      <c r="B120" s="182"/>
-      <c r="C120" s="176"/>
-      <c r="D120" s="176"/>
+      <c r="B120" s="193"/>
+      <c r="C120" s="169"/>
+      <c r="D120" s="169"/>
     </row>
     <row r="121" spans="1:4" ht="29.25" thickBot="1">
       <c r="A121" s="27" t="s">
@@ -6994,12 +6994,12 @@
       <c r="D136" s="2"/>
     </row>
     <row r="137" spans="1:4" ht="38.25" customHeight="1" thickBot="1">
-      <c r="A137" s="182" t="s">
+      <c r="A137" s="193" t="s">
         <v>206</v>
       </c>
-      <c r="B137" s="182"/>
-      <c r="C137" s="176"/>
-      <c r="D137" s="176"/>
+      <c r="B137" s="193"/>
+      <c r="C137" s="169"/>
+      <c r="D137" s="169"/>
     </row>
     <row r="138" spans="1:4" ht="15.75" thickBot="1">
       <c r="A138" s="27" t="s">
@@ -7048,10 +7048,10 @@
       <c r="D141" s="2"/>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="169" t="s">
+      <c r="A142" s="200" t="s">
         <v>258</v>
       </c>
-      <c r="B142" s="169"/>
+      <c r="B142" s="200"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
@@ -7062,12 +7062,12 @@
       <c r="D143" s="2"/>
     </row>
     <row r="144" spans="1:4" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A144" s="182" t="s">
+      <c r="A144" s="193" t="s">
         <v>257</v>
       </c>
-      <c r="B144" s="182"/>
-      <c r="C144" s="176"/>
-      <c r="D144" s="176"/>
+      <c r="B144" s="193"/>
+      <c r="C144" s="169"/>
+      <c r="D144" s="169"/>
     </row>
     <row r="145" spans="1:4" ht="15.75" thickBot="1">
       <c r="A145" s="27" t="s">
@@ -7110,12 +7110,12 @@
       <c r="D150" s="2"/>
     </row>
     <row r="151" spans="1:4" ht="49.5" customHeight="1" thickBot="1">
-      <c r="A151" s="183" t="s">
+      <c r="A151" s="194" t="s">
         <v>210</v>
       </c>
-      <c r="B151" s="183"/>
-      <c r="C151" s="184"/>
-      <c r="D151" s="184"/>
+      <c r="B151" s="194"/>
+      <c r="C151" s="195"/>
+      <c r="D151" s="195"/>
     </row>
     <row r="152" spans="1:4" ht="29.25" thickBot="1">
       <c r="A152" s="27" t="s">
@@ -7194,10 +7194,10 @@
       <c r="D158" s="2"/>
     </row>
     <row r="159" spans="1:4" ht="39" customHeight="1" thickBot="1">
-      <c r="A159" s="170" t="s">
+      <c r="A159" s="199" t="s">
         <v>259</v>
       </c>
-      <c r="B159" s="170"/>
+      <c r="B159" s="199"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
     </row>
@@ -7242,10 +7242,10 @@
       <c r="D163" s="2"/>
     </row>
     <row r="164" spans="1:7">
-      <c r="A164" s="169" t="s">
+      <c r="A164" s="200" t="s">
         <v>214</v>
       </c>
-      <c r="B164" s="169"/>
+      <c r="B164" s="200"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
     </row>
@@ -7256,22 +7256,22 @@
       <c r="D165" s="2"/>
     </row>
     <row r="166" spans="1:7" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A166" s="174" t="s">
+      <c r="A166" s="201" t="s">
         <v>215</v>
       </c>
-      <c r="B166" s="174"/>
-      <c r="C166" s="176"/>
-      <c r="D166" s="176"/>
+      <c r="B166" s="201"/>
+      <c r="C166" s="169"/>
+      <c r="D166" s="169"/>
     </row>
     <row r="167" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="A167" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="B167" s="186" t="s">
+      <c r="B167" s="203" t="s">
         <v>428</v>
       </c>
-      <c r="C167" s="187"/>
-      <c r="D167" s="188"/>
+      <c r="C167" s="204"/>
+      <c r="D167" s="205"/>
       <c r="F167" t="s">
         <v>430</v>
       </c>
@@ -7283,12 +7283,12 @@
       <c r="D168" s="2"/>
     </row>
     <row r="169" spans="1:7" ht="75.75" customHeight="1">
-      <c r="A169" s="185" t="s">
+      <c r="A169" s="202" t="s">
         <v>217</v>
       </c>
-      <c r="B169" s="185"/>
-      <c r="C169" s="176"/>
-      <c r="D169" s="176"/>
+      <c r="B169" s="202"/>
+      <c r="C169" s="169"/>
+      <c r="D169" s="169"/>
       <c r="F169" t="s">
         <v>429</v>
       </c>
@@ -7346,20 +7346,20 @@
       </c>
     </row>
     <row r="175" spans="1:7">
-      <c r="A175" s="169"/>
-      <c r="B175" s="169"/>
+      <c r="A175" s="200"/>
+      <c r="B175" s="200"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="41"/>
       <c r="B176" s="41"/>
     </row>
     <row r="177" spans="1:6" ht="63" customHeight="1" thickBot="1">
-      <c r="A177" s="183" t="s">
+      <c r="A177" s="194" t="s">
         <v>220</v>
       </c>
-      <c r="B177" s="183"/>
-      <c r="C177" s="184"/>
-      <c r="D177" s="184"/>
+      <c r="B177" s="194"/>
+      <c r="C177" s="195"/>
+      <c r="D177" s="195"/>
     </row>
     <row r="178" spans="1:6" ht="26.25" customHeight="1" thickBot="1">
       <c r="A178" s="27" t="s">
@@ -7400,20 +7400,20 @@
       <c r="D181" s="57"/>
     </row>
     <row r="182" spans="1:6">
-      <c r="A182" s="181"/>
-      <c r="B182" s="181"/>
+      <c r="A182" s="211"/>
+      <c r="B182" s="211"/>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="43"/>
       <c r="B183" s="43"/>
     </row>
     <row r="184" spans="1:6" ht="54.75" customHeight="1">
-      <c r="A184" s="182" t="s">
+      <c r="A184" s="193" t="s">
         <v>267</v>
       </c>
-      <c r="B184" s="182"/>
-      <c r="C184" s="176"/>
-      <c r="D184" s="176"/>
+      <c r="B184" s="193"/>
+      <c r="C184" s="169"/>
+      <c r="D184" s="169"/>
       <c r="F184" t="s">
         <v>431</v>
       </c>
@@ -7461,12 +7461,12 @@
       <c r="D192" s="2"/>
     </row>
     <row r="193" spans="1:6" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A193" s="177" t="s">
+      <c r="A193" s="206" t="s">
         <v>223</v>
       </c>
-      <c r="B193" s="177"/>
-      <c r="C193" s="178"/>
-      <c r="D193" s="178"/>
+      <c r="B193" s="206"/>
+      <c r="C193" s="207"/>
+      <c r="D193" s="207"/>
     </row>
     <row r="194" spans="1:6" ht="15.75" thickBot="1">
       <c r="A194" s="24" t="s">
@@ -7515,8 +7515,8 @@
       <c r="D198" s="2"/>
     </row>
     <row r="199" spans="1:6">
-      <c r="A199" s="169"/>
-      <c r="B199" s="169"/>
+      <c r="A199" s="200"/>
+      <c r="B199" s="200"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
     </row>
@@ -7527,12 +7527,12 @@
       <c r="D200" s="2"/>
     </row>
     <row r="201" spans="1:6" ht="54.75" customHeight="1">
-      <c r="A201" s="172" t="s">
+      <c r="A201" s="208" t="s">
         <v>272</v>
       </c>
-      <c r="B201" s="172"/>
-      <c r="C201" s="173"/>
-      <c r="D201" s="173"/>
+      <c r="B201" s="208"/>
+      <c r="C201" s="170"/>
+      <c r="D201" s="170"/>
       <c r="F201" t="s">
         <v>435</v>
       </c>
@@ -7571,19 +7571,19 @@
       <c r="B207" s="57"/>
     </row>
     <row r="208" spans="1:6">
-      <c r="A208" s="169"/>
-      <c r="B208" s="169"/>
+      <c r="A208" s="200"/>
+      <c r="B208" s="200"/>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="45"/>
     </row>
     <row r="210" spans="1:4" ht="33" customHeight="1" thickBot="1">
-      <c r="A210" s="179" t="s">
+      <c r="A210" s="209" t="s">
         <v>273</v>
       </c>
-      <c r="B210" s="179"/>
-      <c r="C210" s="180"/>
-      <c r="D210" s="180"/>
+      <c r="B210" s="209"/>
+      <c r="C210" s="210"/>
+      <c r="D210" s="210"/>
     </row>
     <row r="211" spans="1:4" ht="15.75" thickBot="1">
       <c r="A211" s="27" t="s">
@@ -7632,12 +7632,12 @@
       <c r="B216" s="41"/>
     </row>
     <row r="217" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A217" s="174" t="s">
+      <c r="A217" s="201" t="s">
         <v>226</v>
       </c>
-      <c r="B217" s="174"/>
-      <c r="C217" s="176"/>
-      <c r="D217" s="176"/>
+      <c r="B217" s="201"/>
+      <c r="C217" s="169"/>
+      <c r="D217" s="169"/>
     </row>
     <row r="218" spans="1:4" ht="45">
       <c r="A218" s="46" t="s">
@@ -7648,12 +7648,12 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="36" customHeight="1">
-      <c r="A220" s="172" t="s">
+      <c r="A220" s="208" t="s">
         <v>228</v>
       </c>
-      <c r="B220" s="172"/>
-      <c r="C220" s="173"/>
-      <c r="D220" s="173"/>
+      <c r="B220" s="208"/>
+      <c r="C220" s="170"/>
+      <c r="D220" s="170"/>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="46" t="s">
@@ -7675,12 +7675,12 @@
       </c>
     </row>
     <row r="224" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A224" s="172" t="s">
+      <c r="A224" s="208" t="s">
         <v>229</v>
       </c>
-      <c r="B224" s="172"/>
-      <c r="C224" s="173"/>
-      <c r="D224" s="173"/>
+      <c r="B224" s="208"/>
+      <c r="C224" s="170"/>
+      <c r="D224" s="170"/>
     </row>
     <row r="225" spans="1:6" ht="90">
       <c r="A225" s="46" t="s">
@@ -7696,12 +7696,12 @@
       </c>
     </row>
     <row r="228" spans="1:6" ht="49.5" customHeight="1">
-      <c r="A228" s="172" t="s">
+      <c r="A228" s="208" t="s">
         <v>230</v>
       </c>
-      <c r="B228" s="172"/>
-      <c r="C228" s="173"/>
-      <c r="D228" s="173"/>
+      <c r="B228" s="208"/>
+      <c r="C228" s="170"/>
+      <c r="D228" s="170"/>
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="46" t="s">
@@ -7720,12 +7720,12 @@
       </c>
     </row>
     <row r="231" spans="1:6" ht="33" customHeight="1">
-      <c r="A231" s="172" t="s">
+      <c r="A231" s="208" t="s">
         <v>231</v>
       </c>
-      <c r="B231" s="172"/>
-      <c r="C231" s="173"/>
-      <c r="D231" s="173"/>
+      <c r="B231" s="208"/>
+      <c r="C231" s="170"/>
+      <c r="D231" s="170"/>
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="46" t="s">
@@ -7736,12 +7736,12 @@
       </c>
     </row>
     <row r="234" spans="1:6" ht="41.25" customHeight="1">
-      <c r="A234" s="172" t="s">
+      <c r="A234" s="208" t="s">
         <v>232</v>
       </c>
-      <c r="B234" s="172"/>
-      <c r="C234" s="173"/>
-      <c r="D234" s="173"/>
+      <c r="B234" s="208"/>
+      <c r="C234" s="170"/>
+      <c r="D234" s="170"/>
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="46" t="s">
@@ -7752,12 +7752,12 @@
       </c>
     </row>
     <row r="237" spans="1:6" ht="38.25" customHeight="1">
-      <c r="A237" s="174" t="s">
+      <c r="A237" s="201" t="s">
         <v>233</v>
       </c>
-      <c r="B237" s="174"/>
-      <c r="C237" s="173"/>
-      <c r="D237" s="173"/>
+      <c r="B237" s="201"/>
+      <c r="C237" s="170"/>
+      <c r="D237" s="170"/>
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="46" t="s">
@@ -7773,12 +7773,12 @@
       </c>
     </row>
     <row r="241" spans="1:4" ht="45" customHeight="1">
-      <c r="A241" s="172" t="s">
+      <c r="A241" s="208" t="s">
         <v>234</v>
       </c>
-      <c r="B241" s="172"/>
-      <c r="C241" s="173"/>
-      <c r="D241" s="173"/>
+      <c r="B241" s="208"/>
+      <c r="C241" s="170"/>
+      <c r="D241" s="170"/>
     </row>
     <row r="242" spans="1:4">
       <c r="A242" s="46" t="s">
@@ -7794,12 +7794,12 @@
       </c>
     </row>
     <row r="245" spans="1:4" ht="42" customHeight="1">
-      <c r="A245" s="175" t="s">
+      <c r="A245" s="212" t="s">
         <v>235</v>
       </c>
-      <c r="B245" s="175"/>
-      <c r="C245" s="173"/>
-      <c r="D245" s="173"/>
+      <c r="B245" s="212"/>
+      <c r="C245" s="170"/>
+      <c r="D245" s="170"/>
     </row>
     <row r="246" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="247" spans="1:4" ht="15.75" thickBot="1">
@@ -7852,10 +7852,10 @@
       </c>
     </row>
     <row r="254" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A254" s="172" t="s">
+      <c r="A254" s="208" t="s">
         <v>238</v>
       </c>
-      <c r="B254" s="173"/>
+      <c r="B254" s="170"/>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" s="49"/>
@@ -7866,12 +7866,12 @@
       </c>
     </row>
     <row r="257" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A257" s="172" t="s">
+      <c r="A257" s="208" t="s">
         <v>239</v>
       </c>
-      <c r="B257" s="172"/>
-      <c r="C257" s="173"/>
-      <c r="D257" s="173"/>
+      <c r="B257" s="208"/>
+      <c r="C257" s="170"/>
+      <c r="D257" s="170"/>
     </row>
     <row r="258" spans="1:4">
       <c r="A258" s="46" t="s">
@@ -7879,12 +7879,12 @@
       </c>
     </row>
     <row r="260" spans="1:4">
-      <c r="A260" s="172" t="s">
+      <c r="A260" s="208" t="s">
         <v>240</v>
       </c>
-      <c r="B260" s="172"/>
-      <c r="C260" s="173"/>
-      <c r="D260" s="173"/>
+      <c r="B260" s="208"/>
+      <c r="C260" s="170"/>
+      <c r="D260" s="170"/>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="46" t="s">
@@ -7893,16 +7893,16 @@
     </row>
     <row r="262" spans="1:4" ht="25.5" customHeight="1"/>
     <row r="263" spans="1:4" ht="49.5" customHeight="1">
-      <c r="A263" s="172" t="s">
+      <c r="A263" s="208" t="s">
         <v>241</v>
       </c>
-      <c r="B263" s="172"/>
+      <c r="B263" s="208"/>
     </row>
     <row r="264" spans="1:4" ht="59.25" customHeight="1">
-      <c r="A264" s="172" t="s">
+      <c r="A264" s="208" t="s">
         <v>242</v>
       </c>
-      <c r="B264" s="172"/>
+      <c r="B264" s="208"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="46" t="s">
@@ -7910,12 +7910,12 @@
       </c>
     </row>
     <row r="267" spans="1:4" ht="55.5" customHeight="1" thickBot="1">
-      <c r="A267" s="170" t="s">
+      <c r="A267" s="199" t="s">
         <v>243</v>
       </c>
-      <c r="B267" s="170"/>
-      <c r="C267" s="171"/>
-      <c r="D267" s="171"/>
+      <c r="B267" s="199"/>
+      <c r="C267" s="213"/>
+      <c r="D267" s="213"/>
     </row>
     <row r="268" spans="1:4" ht="15.75" thickBot="1">
       <c r="A268" s="27" t="s">
@@ -7948,8 +7948,8 @@
       <c r="D270" s="12"/>
     </row>
     <row r="271" spans="1:4">
-      <c r="A271" s="169"/>
-      <c r="B271" s="169"/>
+      <c r="A271" s="200"/>
+      <c r="B271" s="200"/>
     </row>
     <row r="272" spans="1:4">
       <c r="A272" s="41"/>
@@ -7974,12 +7974,12 @@
       </c>
     </row>
     <row r="277" spans="1:4" ht="39" customHeight="1">
-      <c r="A277" s="172" t="s">
+      <c r="A277" s="208" t="s">
         <v>245</v>
       </c>
-      <c r="B277" s="172"/>
-      <c r="C277" s="173"/>
-      <c r="D277" s="173"/>
+      <c r="B277" s="208"/>
+      <c r="C277" s="170"/>
+      <c r="D277" s="170"/>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" s="46" t="s">
@@ -7988,12 +7988,12 @@
       <c r="B278" s="8"/>
     </row>
     <row r="280" spans="1:4" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A280" s="170" t="s">
+      <c r="A280" s="199" t="s">
         <v>246</v>
       </c>
-      <c r="B280" s="170"/>
-      <c r="C280" s="171"/>
-      <c r="D280" s="171"/>
+      <c r="B280" s="199"/>
+      <c r="C280" s="213"/>
+      <c r="D280" s="213"/>
     </row>
     <row r="281" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="282" spans="1:4" ht="15.75" thickBot="1">
@@ -8036,6 +8036,54 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A271:B271"/>
+    <mergeCell ref="A267:D267"/>
+    <mergeCell ref="A277:D277"/>
+    <mergeCell ref="A280:D280"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A264:B264"/>
+    <mergeCell ref="A254:B254"/>
+    <mergeCell ref="A257:D257"/>
+    <mergeCell ref="A260:D260"/>
+    <mergeCell ref="A231:D231"/>
+    <mergeCell ref="A234:D234"/>
+    <mergeCell ref="A237:D237"/>
+    <mergeCell ref="A245:D245"/>
+    <mergeCell ref="A241:D241"/>
+    <mergeCell ref="A217:D217"/>
+    <mergeCell ref="A220:D220"/>
+    <mergeCell ref="A224:D224"/>
+    <mergeCell ref="A228:D228"/>
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="A208:B208"/>
+    <mergeCell ref="A193:D193"/>
+    <mergeCell ref="A201:D201"/>
+    <mergeCell ref="A210:D210"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="A184:D184"/>
+    <mergeCell ref="A177:D177"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="A151:D151"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A117:C117"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A32:E32"/>
@@ -8051,54 +8099,6 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="A151:D151"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A117:C117"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A166:D166"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="A193:D193"/>
-    <mergeCell ref="A201:D201"/>
-    <mergeCell ref="A210:D210"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="A184:D184"/>
-    <mergeCell ref="A177:D177"/>
-    <mergeCell ref="A217:D217"/>
-    <mergeCell ref="A220:D220"/>
-    <mergeCell ref="A224:D224"/>
-    <mergeCell ref="A228:D228"/>
-    <mergeCell ref="A199:B199"/>
-    <mergeCell ref="A208:B208"/>
-    <mergeCell ref="A254:B254"/>
-    <mergeCell ref="A257:D257"/>
-    <mergeCell ref="A260:D260"/>
-    <mergeCell ref="A231:D231"/>
-    <mergeCell ref="A234:D234"/>
-    <mergeCell ref="A237:D237"/>
-    <mergeCell ref="A245:D245"/>
-    <mergeCell ref="A241:D241"/>
-    <mergeCell ref="A271:B271"/>
-    <mergeCell ref="A267:D267"/>
-    <mergeCell ref="A277:D277"/>
-    <mergeCell ref="A280:D280"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A264:B264"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8113,8 +8113,8 @@
   <dimension ref="A1:XFD371"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
+      <pane ySplit="2" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8145,11 +8145,11 @@
       <c r="D1" s="108" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="214" t="s">
+      <c r="E1" s="225" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
@@ -8231,15 +8231,15 @@
       <c r="P3" s="109"/>
     </row>
     <row r="4" spans="1:26 16384:16384" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A4" s="215" t="s">
+      <c r="A4" s="226" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="215"/>
-      <c r="C4" s="215"/>
-      <c r="D4" s="215"/>
-      <c r="E4" s="215"/>
-      <c r="F4" s="215"/>
-      <c r="G4" s="215"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
       <c r="H4" s="152"/>
       <c r="I4" s="153"/>
       <c r="J4" s="153"/>
@@ -8308,12 +8308,12 @@
       <c r="N6" s="97"/>
       <c r="O6" s="97"/>
       <c r="P6" s="97"/>
-      <c r="R6" s="222" t="s">
+      <c r="R6" s="214" t="s">
         <v>285</v>
       </c>
-      <c r="S6" s="223"/>
-      <c r="T6" s="223"/>
-      <c r="U6" s="223"/>
+      <c r="S6" s="215"/>
+      <c r="T6" s="215"/>
+      <c r="U6" s="215"/>
     </row>
     <row r="7" spans="1:26 16384:16384" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="110" t="s">
@@ -8342,10 +8342,10 @@
       <c r="N7" s="65"/>
       <c r="O7" s="66"/>
       <c r="P7" s="66"/>
-      <c r="R7" s="223"/>
-      <c r="S7" s="223"/>
-      <c r="T7" s="223"/>
-      <c r="U7" s="223"/>
+      <c r="R7" s="215"/>
+      <c r="S7" s="215"/>
+      <c r="T7" s="215"/>
+      <c r="U7" s="215"/>
     </row>
     <row r="8" spans="1:26 16384:16384" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="110" t="s">
@@ -8374,10 +8374,10 @@
       <c r="N8" s="64"/>
       <c r="O8" s="64"/>
       <c r="P8" s="64"/>
-      <c r="R8" s="223"/>
-      <c r="S8" s="223"/>
-      <c r="T8" s="223"/>
-      <c r="U8" s="223"/>
+      <c r="R8" s="215"/>
+      <c r="S8" s="215"/>
+      <c r="T8" s="215"/>
+      <c r="U8" s="215"/>
     </row>
     <row r="9" spans="1:26 16384:16384" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A9" s="110" t="s">
@@ -8406,10 +8406,10 @@
       <c r="N9" s="64"/>
       <c r="O9" s="64"/>
       <c r="P9" s="64"/>
-      <c r="R9" s="223"/>
-      <c r="S9" s="223"/>
-      <c r="T9" s="223"/>
-      <c r="U9" s="223"/>
+      <c r="R9" s="215"/>
+      <c r="S9" s="215"/>
+      <c r="T9" s="215"/>
+      <c r="U9" s="215"/>
     </row>
     <row r="10" spans="1:26 16384:16384" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A10" s="110" t="s">
@@ -8438,10 +8438,10 @@
       <c r="N10" s="64"/>
       <c r="O10" s="64"/>
       <c r="P10" s="64"/>
-      <c r="R10" s="223"/>
-      <c r="S10" s="223"/>
-      <c r="T10" s="223"/>
-      <c r="U10" s="223"/>
+      <c r="R10" s="215"/>
+      <c r="S10" s="215"/>
+      <c r="T10" s="215"/>
+      <c r="U10" s="215"/>
       <c r="XFD10" s="75"/>
     </row>
     <row r="11" spans="1:26 16384:16384" s="18" customFormat="1" ht="30.75" thickBot="1">
@@ -8471,10 +8471,10 @@
       <c r="N11" s="64"/>
       <c r="O11" s="64"/>
       <c r="P11" s="64"/>
-      <c r="R11" s="223"/>
-      <c r="S11" s="223"/>
-      <c r="T11" s="223"/>
-      <c r="U11" s="223"/>
+      <c r="R11" s="215"/>
+      <c r="S11" s="215"/>
+      <c r="T11" s="215"/>
+      <c r="U11" s="215"/>
     </row>
     <row r="12" spans="1:26 16384:16384" s="18" customFormat="1" ht="15.75" thickBot="1">
       <c r="A12" s="110" t="s">
@@ -8503,10 +8503,10 @@
       <c r="N12" s="64"/>
       <c r="O12" s="64"/>
       <c r="P12" s="64"/>
-      <c r="R12" s="223"/>
-      <c r="S12" s="223"/>
-      <c r="T12" s="223"/>
-      <c r="U12" s="223"/>
+      <c r="R12" s="215"/>
+      <c r="S12" s="215"/>
+      <c r="T12" s="215"/>
+      <c r="U12" s="215"/>
     </row>
     <row r="13" spans="1:26 16384:16384" s="18" customFormat="1" ht="30.75" thickBot="1">
       <c r="A13" s="110" t="s">
@@ -8536,10 +8536,10 @@
       <c r="O13" s="64"/>
       <c r="P13" s="64"/>
       <c r="Q13" s="19"/>
-      <c r="R13" s="223"/>
-      <c r="S13" s="223"/>
-      <c r="T13" s="223"/>
-      <c r="U13" s="223"/>
+      <c r="R13" s="215"/>
+      <c r="S13" s="215"/>
+      <c r="T13" s="215"/>
+      <c r="U13" s="215"/>
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
       <c r="X13" s="19"/>
@@ -8574,10 +8574,10 @@
       <c r="O14" s="72"/>
       <c r="P14" s="72"/>
       <c r="Q14" s="19"/>
-      <c r="R14" s="223"/>
-      <c r="S14" s="223"/>
-      <c r="T14" s="223"/>
-      <c r="U14" s="223"/>
+      <c r="R14" s="215"/>
+      <c r="S14" s="215"/>
+      <c r="T14" s="215"/>
+      <c r="U14" s="215"/>
       <c r="V14" s="19"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
@@ -8612,10 +8612,10 @@
       <c r="O15" s="72"/>
       <c r="P15" s="72"/>
       <c r="Q15" s="19"/>
-      <c r="R15" s="223"/>
-      <c r="S15" s="223"/>
-      <c r="T15" s="223"/>
-      <c r="U15" s="223"/>
+      <c r="R15" s="215"/>
+      <c r="S15" s="215"/>
+      <c r="T15" s="215"/>
+      <c r="U15" s="215"/>
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
@@ -8648,10 +8648,10 @@
       <c r="O16" s="72"/>
       <c r="P16" s="72"/>
       <c r="Q16" s="19"/>
-      <c r="R16" s="223"/>
-      <c r="S16" s="223"/>
-      <c r="T16" s="223"/>
-      <c r="U16" s="223"/>
+      <c r="R16" s="215"/>
+      <c r="S16" s="215"/>
+      <c r="T16" s="215"/>
+      <c r="U16" s="215"/>
       <c r="V16" s="19"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
@@ -8686,10 +8686,10 @@
       <c r="O17" s="72"/>
       <c r="P17" s="72"/>
       <c r="Q17" s="19"/>
-      <c r="R17" s="223"/>
-      <c r="S17" s="223"/>
-      <c r="T17" s="223"/>
-      <c r="U17" s="223"/>
+      <c r="R17" s="215"/>
+      <c r="S17" s="215"/>
+      <c r="T17" s="215"/>
+      <c r="U17" s="215"/>
       <c r="V17" s="19"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
@@ -9469,11 +9469,11 @@
       <c r="Z38" s="19"/>
     </row>
     <row r="39" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A39" s="219" t="s">
+      <c r="A39" s="227" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="220"/>
-      <c r="C39" s="221"/>
+      <c r="B39" s="228"/>
+      <c r="C39" s="229"/>
       <c r="D39" s="126"/>
       <c r="E39" s="127"/>
       <c r="F39" s="127"/>
@@ -11084,7 +11084,7 @@
       </c>
       <c r="B82" s="218"/>
       <c r="C82" s="218"/>
-      <c r="D82" s="224"/>
+      <c r="D82" s="219"/>
       <c r="E82" s="217"/>
       <c r="F82" s="217"/>
       <c r="G82" s="217"/>
@@ -11303,8 +11303,8 @@
         <v>141</v>
       </c>
       <c r="B88" s="218"/>
-      <c r="C88" s="224"/>
-      <c r="D88" s="224"/>
+      <c r="C88" s="219"/>
+      <c r="D88" s="219"/>
       <c r="E88" s="217"/>
       <c r="F88" s="217"/>
       <c r="G88" s="217"/>
@@ -11442,7 +11442,7 @@
       <c r="Y91" s="19"/>
       <c r="Z91" s="19"/>
     </row>
-    <row r="92" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
+    <row r="92" spans="1:26" s="18" customFormat="1" ht="30.75" thickBot="1">
       <c r="A92" s="117" t="s">
         <v>145</v>
       </c>
@@ -11464,7 +11464,7 @@
       <c r="K92" s="69"/>
       <c r="L92" s="69"/>
       <c r="M92" s="116" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="N92" s="71"/>
       <c r="O92" s="71"/>
@@ -11502,7 +11502,7 @@
       <c r="K93" s="69"/>
       <c r="L93" s="69"/>
       <c r="M93" s="116" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N93" s="71"/>
       <c r="O93" s="71"/>
@@ -11519,15 +11519,15 @@
       <c r="Z93" s="19"/>
     </row>
     <row r="94" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A94" s="225" t="s">
+      <c r="A94" s="220" t="s">
         <v>147</v>
       </c>
-      <c r="B94" s="226"/>
-      <c r="C94" s="227"/>
-      <c r="D94" s="227"/>
-      <c r="E94" s="228"/>
-      <c r="F94" s="228"/>
-      <c r="G94" s="228"/>
+      <c r="B94" s="221"/>
+      <c r="C94" s="222"/>
+      <c r="D94" s="222"/>
+      <c r="E94" s="223"/>
+      <c r="F94" s="223"/>
+      <c r="G94" s="223"/>
       <c r="H94" s="141"/>
       <c r="I94" s="142"/>
       <c r="J94" s="142"/>
@@ -11735,7 +11735,9 @@
       <c r="D100" s="101" t="s">
         <v>291</v>
       </c>
-      <c r="E100" s="131"/>
+      <c r="E100" s="131" t="s">
+        <v>280</v>
+      </c>
       <c r="F100" s="121"/>
       <c r="G100" s="90"/>
       <c r="H100" s="69"/>
@@ -11807,7 +11809,9 @@
       <c r="D102" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="E102" s="129"/>
+      <c r="E102" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F102" s="121"/>
       <c r="G102" s="90"/>
       <c r="H102" s="69"/>
@@ -11831,12 +11835,12 @@
       <c r="Z102" s="19"/>
     </row>
     <row r="103" spans="1:26" s="18" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A103" s="229" t="s">
+      <c r="A103" s="224" t="s">
         <v>157</v>
       </c>
-      <c r="B103" s="224"/>
-      <c r="C103" s="224"/>
-      <c r="D103" s="224"/>
+      <c r="B103" s="219"/>
+      <c r="C103" s="219"/>
+      <c r="D103" s="219"/>
       <c r="E103" s="218"/>
       <c r="F103" s="218"/>
       <c r="G103" s="218"/>
@@ -11874,7 +11878,9 @@
         <v>286</v>
       </c>
       <c r="E104" s="129"/>
-      <c r="F104" s="121"/>
+      <c r="F104" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G104" s="90"/>
       <c r="H104" s="69"/>
       <c r="I104" s="69"/>
@@ -11910,7 +11916,9 @@
         <v>286</v>
       </c>
       <c r="E105" s="129"/>
-      <c r="F105" s="121"/>
+      <c r="F105" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G105" s="90"/>
       <c r="H105" s="82"/>
       <c r="I105" s="69"/>
@@ -11946,7 +11954,9 @@
         <v>286</v>
       </c>
       <c r="E106" s="129"/>
-      <c r="F106" s="121"/>
+      <c r="F106" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G106" s="90"/>
       <c r="H106" s="82"/>
       <c r="I106" s="69"/>
@@ -11982,7 +11992,9 @@
         <v>286</v>
       </c>
       <c r="E107" s="132"/>
-      <c r="F107" s="163"/>
+      <c r="F107" s="163" t="s">
+        <v>280</v>
+      </c>
       <c r="G107" s="164"/>
       <c r="H107" s="69"/>
       <c r="I107" s="70"/>
@@ -12009,8 +12021,8 @@
         <v>162</v>
       </c>
       <c r="B108" s="218"/>
-      <c r="C108" s="224"/>
-      <c r="D108" s="224"/>
+      <c r="C108" s="219"/>
+      <c r="D108" s="219"/>
       <c r="E108" s="217"/>
       <c r="F108" s="217"/>
       <c r="G108" s="217"/>
@@ -12048,7 +12060,9 @@
         <v>286</v>
       </c>
       <c r="E109" s="129"/>
-      <c r="F109" s="121"/>
+      <c r="F109" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G109" s="90"/>
       <c r="H109" s="80"/>
       <c r="I109" s="80"/>
@@ -12083,7 +12097,9 @@
       <c r="D110" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="E110" s="129"/>
+      <c r="E110" s="129" t="s">
+        <v>280</v>
+      </c>
       <c r="F110" s="121"/>
       <c r="G110" s="90"/>
       <c r="H110" s="80"/>
@@ -12118,7 +12134,9 @@
         <v>303</v>
       </c>
       <c r="E111" s="129"/>
-      <c r="F111" s="121"/>
+      <c r="F111" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G111" s="90"/>
       <c r="H111" s="80"/>
       <c r="I111" s="80"/>
@@ -12154,7 +12172,9 @@
         <v>295</v>
       </c>
       <c r="E112" s="129"/>
-      <c r="F112" s="121"/>
+      <c r="F112" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G112" s="90"/>
       <c r="H112" s="80"/>
       <c r="I112" s="80"/>
@@ -12181,8 +12201,8 @@
         <v>168</v>
       </c>
       <c r="B113" s="218"/>
-      <c r="C113" s="224"/>
-      <c r="D113" s="224"/>
+      <c r="C113" s="219"/>
+      <c r="D113" s="219"/>
       <c r="E113" s="217"/>
       <c r="F113" s="217"/>
       <c r="G113" s="217"/>
@@ -12220,7 +12240,9 @@
         <v>286</v>
       </c>
       <c r="E114" s="129"/>
-      <c r="F114" s="121"/>
+      <c r="F114" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G114" s="90"/>
       <c r="H114" s="80"/>
       <c r="I114" s="80"/>
@@ -12256,7 +12278,9 @@
         <v>286</v>
       </c>
       <c r="E115" s="129"/>
-      <c r="F115" s="121"/>
+      <c r="F115" s="121" t="s">
+        <v>280</v>
+      </c>
       <c r="G115" s="90"/>
       <c r="H115" s="82"/>
       <c r="I115" s="80"/>
@@ -12292,7 +12316,9 @@
         <v>286</v>
       </c>
       <c r="E116" s="138"/>
-      <c r="F116" s="139"/>
+      <c r="F116" s="139" t="s">
+        <v>280</v>
+      </c>
       <c r="G116" s="140"/>
       <c r="H116" s="82"/>
       <c r="I116" s="80"/>
@@ -16142,6 +16168,11 @@
   </sheetData>
   <autoFilter ref="B1:B473" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="15">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A39:C39"/>
     <mergeCell ref="R6:U17"/>
     <mergeCell ref="A70:G70"/>
     <mergeCell ref="A108:G108"/>
@@ -16152,11 +16183,6 @@
     <mergeCell ref="A97:G97"/>
     <mergeCell ref="A99:G99"/>
     <mergeCell ref="A103:G103"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="36" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
auto commit @16.11.2020: 21:00:43,84
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
+++ b/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0D83FD-B810-448C-8226-1CF1BF480DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC07A60-0CF2-4FDA-99E9-18FEC0497E0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="478">
   <si>
     <t>TR.A.1</t>
   </si>
@@ -3932,9 +3932,6 @@
     <t>https://openwrt.org/docs/guide-user/firewall/fw3_network</t>
   </si>
   <si>
-    <t>OpenWrt uses an open source component called firewall3 (fw3). Fw3 is a netfilter/iptable rule builder application. These rulles are then passed to the firewall in the linux kernel (iptables / netfilter). All firewall componentes are completely open source. https://openwrt.org/docs/guide-user/firewall/overview https://netfilter.org/projects/iptables/index.html</t>
-  </si>
-  <si>
     <t>https://openwrt.org/docs/techref/odhcpd</t>
   </si>
   <si>
@@ -4086,6 +4083,17 @@
   </si>
   <si>
     <t>no such attacks are known / ssh audit results are available in the results folder</t>
+  </si>
+  <si>
+    <t>Metadata embedded into firmware package file</t>
+  </si>
+  <si>
+    <t>SHA256 / MD5 hashes [not checked, just displayed for the user to check]</t>
+  </si>
+  <si>
+    <t>OpenWrt uses an open source component called firewall3 (fw3). Fw3 is a netfilter/iptable rule builder application. All firewall componentes are completely open source. https://openwrt.org/docs/guide-user/firewall/overview https://netfilter.org/projects/iptables/index.html
+- iptables - 1.8.3-1: https://ipset.netfilter.org/iptables.man.html
+- firewall - 2019-11-22-8174814a-2</t>
   </si>
 </sst>
 </file>
@@ -5483,30 +5491,169 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -5515,97 +5662,50 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5615,18 +5715,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5637,86 +5725,6 @@
     <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="5" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="10" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -6007,8 +6015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A194" sqref="A194:D194"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6021,19 +6029,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="88.5" customHeight="1">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="175" t="s">
         <v>274</v>
       </c>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="173"/>
-      <c r="K2" s="173"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="176"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1"/>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
@@ -6043,10 +6051,10 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A6" s="196" t="s">
+      <c r="A6" s="200" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="230"/>
+      <c r="B6" s="201"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6061,42 +6069,42 @@
       <c r="A7" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="236" t="s">
+      <c r="B7" s="195" t="s">
         <v>390</v>
       </c>
-      <c r="C7" s="232"/>
-      <c r="D7" s="233"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="170"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="236" t="s">
+      <c r="B8" s="195" t="s">
         <v>389</v>
       </c>
-      <c r="C8" s="234"/>
+      <c r="C8" s="204"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="236" t="s">
+      <c r="B9" s="195" t="s">
         <v>391</v>
       </c>
-      <c r="C9" s="234"/>
+      <c r="C9" s="204"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="237" t="s">
+      <c r="B10" s="205" t="s">
         <v>402</v>
       </c>
-      <c r="C10" s="235"/>
+      <c r="C10" s="206"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="B11" s="231"/>
-      <c r="C11" s="231"/>
+      <c r="B11" s="169"/>
+      <c r="C11" s="169"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
@@ -6105,86 +6113,86 @@
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A14" s="197" t="s">
+      <c r="A14" s="202" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="198"/>
+      <c r="B14" s="203"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1" thickBot="1">
       <c r="A15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="204" t="s">
+      <c r="B15" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="205"/>
-      <c r="D15" s="206"/>
+      <c r="C15" s="181"/>
+      <c r="D15" s="182"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1">
       <c r="A16" s="164" t="s">
-        <v>438</v>
-      </c>
-      <c r="B16" s="210" t="s">
-        <v>442</v>
-      </c>
-      <c r="C16" s="211"/>
-      <c r="D16" s="212"/>
+        <v>437</v>
+      </c>
+      <c r="B16" s="186" t="s">
+        <v>441</v>
+      </c>
+      <c r="C16" s="187"/>
+      <c r="D16" s="188"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="165" t="s">
-        <v>439</v>
-      </c>
-      <c r="B17" s="238" t="s">
-        <v>443</v>
-      </c>
-      <c r="C17" s="229"/>
-      <c r="D17" s="229"/>
-      <c r="E17" s="229"/>
-      <c r="F17" s="229"/>
-      <c r="G17" s="229"/>
-      <c r="H17" s="229"/>
+        <v>438</v>
+      </c>
+      <c r="B17" s="207" t="s">
+        <v>442</v>
+      </c>
+      <c r="C17" s="208"/>
+      <c r="D17" s="208"/>
+      <c r="E17" s="208"/>
+      <c r="F17" s="208"/>
+      <c r="G17" s="208"/>
+      <c r="H17" s="208"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" s="165" t="s">
-        <v>439</v>
-      </c>
-      <c r="B18" s="238" t="s">
-        <v>444</v>
-      </c>
-      <c r="C18" s="229"/>
-      <c r="D18" s="229"/>
-      <c r="E18" s="229"/>
-      <c r="F18" s="229"/>
-      <c r="G18" s="229"/>
-      <c r="H18" s="229"/>
+        <v>438</v>
+      </c>
+      <c r="B18" s="207" t="s">
+        <v>443</v>
+      </c>
+      <c r="C18" s="208"/>
+      <c r="D18" s="208"/>
+      <c r="E18" s="208"/>
+      <c r="F18" s="208"/>
+      <c r="G18" s="208"/>
+      <c r="H18" s="208"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" s="165" t="s">
+        <v>439</v>
+      </c>
+      <c r="B19" s="189" t="s">
+        <v>444</v>
+      </c>
+      <c r="C19" s="190"/>
+      <c r="D19" s="191"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A20" s="171" t="s">
         <v>440</v>
       </c>
-      <c r="B19" s="199" t="s">
+      <c r="B20" s="192" t="s">
         <v>445</v>
       </c>
-      <c r="C19" s="200"/>
-      <c r="D19" s="201"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A20" s="239" t="s">
-        <v>441</v>
-      </c>
-      <c r="B20" s="240" t="s">
+      <c r="C20" s="193"/>
+      <c r="D20" s="194"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A21" s="172" t="s">
         <v>446</v>
       </c>
-      <c r="C20" s="241"/>
-      <c r="D20" s="242"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A21" s="243" t="s">
-        <v>447</v>
-      </c>
-      <c r="B21" s="244"/>
-      <c r="C21" s="245"/>
-      <c r="D21" s="246"/>
+      <c r="B21" s="209"/>
+      <c r="C21" s="210"/>
+      <c r="D21" s="211"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6" t="s">
@@ -6192,70 +6200,70 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" thickBot="1">
-      <c r="A25" s="202" t="s">
+      <c r="A25" s="177" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="203"/>
+      <c r="B25" s="178"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
       <c r="A26" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="207" t="s">
+      <c r="B26" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="208"/>
-      <c r="D26" s="209"/>
+      <c r="C26" s="184"/>
+      <c r="D26" s="185"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1">
       <c r="A27" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="B27" s="210" t="s">
+      <c r="B27" s="186" t="s">
         <v>398</v>
       </c>
-      <c r="C27" s="211"/>
-      <c r="D27" s="212"/>
+      <c r="C27" s="187"/>
+      <c r="D27" s="188"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="A28" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="B28" s="199" t="s">
+      <c r="B28" s="189" t="s">
         <v>399</v>
       </c>
-      <c r="C28" s="200"/>
-      <c r="D28" s="201"/>
+      <c r="C28" s="190"/>
+      <c r="D28" s="191"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1">
       <c r="A29" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B29" s="199" t="s">
+      <c r="B29" s="189" t="s">
         <v>397</v>
       </c>
-      <c r="C29" s="200"/>
-      <c r="D29" s="201"/>
+      <c r="C29" s="190"/>
+      <c r="D29" s="191"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1">
       <c r="A30" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="B30" s="199" t="s">
+      <c r="B30" s="189" t="s">
         <v>401</v>
       </c>
-      <c r="C30" s="200"/>
-      <c r="D30" s="201"/>
+      <c r="C30" s="190"/>
+      <c r="D30" s="191"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="A31" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B31" s="199" t="s">
+      <c r="B31" s="189" t="s">
         <v>400</v>
       </c>
-      <c r="C31" s="200"/>
-      <c r="D31" s="201"/>
+      <c r="C31" s="190"/>
+      <c r="D31" s="191"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="163"/>
@@ -6267,13 +6275,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="76.5" customHeight="1">
-      <c r="A34" s="193" t="s">
+      <c r="A34" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="176"/>
-      <c r="C34" s="176"/>
-      <c r="D34" s="176"/>
-      <c r="E34" s="176"/>
+      <c r="B34" s="175"/>
+      <c r="C34" s="175"/>
+      <c r="D34" s="175"/>
+      <c r="E34" s="175"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="37" spans="1:5" ht="15.75" thickBot="1">
@@ -6304,7 +6312,7 @@
         <v>23</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>24</v>
@@ -6321,7 +6329,7 @@
         <v>23</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>24</v>
@@ -6338,7 +6346,7 @@
         <v>23</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>24</v>
@@ -6355,7 +6363,7 @@
         <v>23</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>24</v>
@@ -6372,7 +6380,7 @@
         <v>23</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>24</v>
@@ -6389,7 +6397,7 @@
         <v>23</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>24</v>
@@ -6403,13 +6411,13 @@
         <v>22</v>
       </c>
       <c r="C44" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E44" s="9" t="s">
         <v>450</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1">
@@ -6420,13 +6428,13 @@
         <v>404</v>
       </c>
       <c r="C45" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E45" s="9" t="s">
         <v>450</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1">
@@ -6437,13 +6445,13 @@
         <v>405</v>
       </c>
       <c r="C46" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>450</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1">
@@ -6454,13 +6462,13 @@
         <v>22</v>
       </c>
       <c r="C47" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E47" s="9" t="s">
         <v>450</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1">
@@ -6471,13 +6479,13 @@
         <v>404</v>
       </c>
       <c r="C48" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E48" s="9" t="s">
         <v>450</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1">
@@ -6488,13 +6496,13 @@
         <v>405</v>
       </c>
       <c r="C49" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>450</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" thickBot="1">
@@ -6504,14 +6512,14 @@
       <c r="B50" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="247" t="s">
+      <c r="C50" s="173" t="s">
+        <v>452</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E50" s="173" t="s">
         <v>453</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="E50" s="247" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1">
@@ -6521,14 +6529,14 @@
       <c r="B51" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="C51" s="247" t="s">
+      <c r="C51" s="173" t="s">
+        <v>452</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E51" s="173" t="s">
         <v>453</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="E51" s="247" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1">
@@ -6538,14 +6546,14 @@
       <c r="B52" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="C52" s="247" t="s">
+      <c r="C52" s="173" t="s">
+        <v>452</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E52" s="173" t="s">
         <v>453</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="E52" s="247" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1">
@@ -6555,14 +6563,14 @@
       <c r="B53" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="247" t="s">
+      <c r="C53" s="173" t="s">
+        <v>452</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E53" s="173" t="s">
         <v>453</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="E53" s="247" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1">
@@ -6572,14 +6580,14 @@
       <c r="B54" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="C54" s="247" t="s">
+      <c r="C54" s="173" t="s">
+        <v>452</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E54" s="173" t="s">
         <v>453</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="E54" s="247" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1">
@@ -6589,24 +6597,24 @@
       <c r="B55" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="C55" s="247" t="s">
+      <c r="C55" s="173" t="s">
+        <v>452</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E55" s="173" t="s">
         <v>453</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="E55" s="247" t="s">
-        <v>454</v>
-      </c>
     </row>
     <row r="58" spans="1:5" ht="57" customHeight="1">
-      <c r="A58" s="193" t="s">
+      <c r="A58" s="179" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="193"/>
-      <c r="C58" s="193"/>
-      <c r="D58" s="193"/>
-      <c r="E58" s="193"/>
+      <c r="B58" s="179"/>
+      <c r="C58" s="179"/>
+      <c r="D58" s="179"/>
+      <c r="E58" s="179"/>
     </row>
     <row r="59" spans="1:5" ht="31.5" customHeight="1" thickBot="1"/>
     <row r="60" spans="1:5" ht="44.25" customHeight="1" thickBot="1">
@@ -6719,13 +6727,13 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A69" s="193" t="s">
+      <c r="A69" s="179" t="s">
         <v>174</v>
       </c>
-      <c r="B69" s="193"/>
-      <c r="C69" s="193"/>
-      <c r="D69" s="193"/>
-      <c r="E69" s="193"/>
+      <c r="B69" s="179"/>
+      <c r="C69" s="179"/>
+      <c r="D69" s="179"/>
+      <c r="E69" s="179"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="10"/>
@@ -6735,7 +6743,7 @@
         <v>26</v>
       </c>
       <c r="B71" s="167" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C71" t="s">
         <v>406</v>
@@ -6748,12 +6756,12 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="36" customHeight="1">
-      <c r="A74" s="193" t="s">
+      <c r="A74" s="179" t="s">
         <v>175</v>
       </c>
-      <c r="B74" s="193"/>
-      <c r="C74" s="193"/>
-      <c r="D74" s="193"/>
+      <c r="B74" s="179"/>
+      <c r="C74" s="179"/>
+      <c r="D74" s="179"/>
       <c r="E74" s="8"/>
     </row>
     <row r="76" spans="1:5">
@@ -6761,16 +6769,16 @@
         <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="193" t="s">
+      <c r="A79" s="179" t="s">
         <v>176</v>
       </c>
-      <c r="B79" s="193"/>
-      <c r="C79" s="193"/>
-      <c r="D79" s="193"/>
+      <c r="B79" s="179"/>
+      <c r="C79" s="179"/>
+      <c r="D79" s="179"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="81" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
@@ -6789,7 +6797,7 @@
         <v>180</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>181</v>
@@ -6800,7 +6808,7 @@
         <v>407</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>9</v>
@@ -6851,13 +6859,13 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A90" s="194" t="s">
+      <c r="A90" s="197" t="s">
         <v>183</v>
       </c>
-      <c r="B90" s="194"/>
-      <c r="C90" s="190"/>
-      <c r="D90" s="190"/>
-      <c r="E90" s="190"/>
+      <c r="B90" s="197"/>
+      <c r="C90" s="198"/>
+      <c r="D90" s="198"/>
+      <c r="E90" s="198"/>
     </row>
     <row r="91" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="92" spans="1:5" ht="35.25" customHeight="1" thickBot="1">
@@ -6882,10 +6890,10 @@
         <v>413</v>
       </c>
       <c r="C93" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D93" s="35" t="s">
         <v>458</v>
-      </c>
-      <c r="D93" s="35" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="45.75" thickBot="1">
@@ -6893,13 +6901,13 @@
         <v>22</v>
       </c>
       <c r="B94" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D94" s="35" t="s">
         <v>460</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="D94" s="35" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15.75" thickBot="1">
@@ -6959,17 +6967,17 @@
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="195" t="s">
+      <c r="A101" s="199" t="s">
         <v>188</v>
       </c>
-      <c r="B101" s="195"/>
+      <c r="B101" s="199"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B103" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -6978,12 +6986,12 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="70.5" customHeight="1">
-      <c r="A107" s="189" t="s">
+      <c r="A107" s="215" t="s">
         <v>191</v>
       </c>
-      <c r="B107" s="190"/>
-      <c r="C107" s="190"/>
-      <c r="D107" s="190"/>
+      <c r="B107" s="198"/>
+      <c r="C107" s="198"/>
+      <c r="D107" s="198"/>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1">
       <c r="A108" t="s">
@@ -7099,12 +7107,12 @@
       <c r="D118" s="2"/>
     </row>
     <row r="119" spans="1:4" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A119" s="183" t="s">
+      <c r="A119" s="213" t="s">
         <v>195</v>
       </c>
-      <c r="B119" s="183"/>
-      <c r="C119" s="184"/>
-      <c r="D119" s="184"/>
+      <c r="B119" s="213"/>
+      <c r="C119" s="214"/>
+      <c r="D119" s="214"/>
     </row>
     <row r="120" spans="1:4" ht="15.75" thickBot="1">
       <c r="A120" s="25" t="s">
@@ -7165,9 +7173,9 @@
       <c r="D126" s="55"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="191"/>
-      <c r="B127" s="191"/>
-      <c r="C127" s="192"/>
+      <c r="A127" s="216"/>
+      <c r="B127" s="216"/>
+      <c r="C127" s="217"/>
       <c r="D127" s="2"/>
     </row>
     <row r="128" spans="1:4">
@@ -7185,12 +7193,12 @@
       <c r="D129" s="2"/>
     </row>
     <row r="130" spans="1:4" ht="113.25" customHeight="1" thickBot="1">
-      <c r="A130" s="182" t="s">
+      <c r="A130" s="212" t="s">
         <v>411</v>
       </c>
-      <c r="B130" s="182"/>
-      <c r="C130" s="176"/>
-      <c r="D130" s="176"/>
+      <c r="B130" s="212"/>
+      <c r="C130" s="175"/>
+      <c r="D130" s="175"/>
     </row>
     <row r="131" spans="1:4" ht="29.25" thickBot="1">
       <c r="A131" s="25" t="s">
@@ -7375,12 +7383,12 @@
       <c r="D146" s="2"/>
     </row>
     <row r="147" spans="1:4" ht="38.25" customHeight="1" thickBot="1">
-      <c r="A147" s="182" t="s">
+      <c r="A147" s="212" t="s">
         <v>202</v>
       </c>
-      <c r="B147" s="182"/>
-      <c r="C147" s="176"/>
-      <c r="D147" s="176"/>
+      <c r="B147" s="212"/>
+      <c r="C147" s="175"/>
+      <c r="D147" s="175"/>
     </row>
     <row r="148" spans="1:4" ht="15.75" thickBot="1">
       <c r="A148" s="25" t="s">
@@ -7398,11 +7406,11 @@
       <c r="A149" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="B149" s="248" t="s">
-        <v>464</v>
+      <c r="B149" s="174" t="s">
+        <v>463</v>
       </c>
       <c r="C149" s="54" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D149" s="2"/>
     </row>
@@ -7411,10 +7419,10 @@
         <v>412</v>
       </c>
       <c r="B150" s="53" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C150" s="54" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D150" s="2"/>
     </row>
@@ -7429,10 +7437,10 @@
       <c r="D151" s="2"/>
     </row>
     <row r="152" spans="1:4">
-      <c r="A152" s="169" t="s">
+      <c r="A152" s="219" t="s">
         <v>253</v>
       </c>
-      <c r="B152" s="169"/>
+      <c r="B152" s="219"/>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
     </row>
@@ -7443,12 +7451,12 @@
       <c r="D153" s="2"/>
     </row>
     <row r="154" spans="1:4" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A154" s="182" t="s">
+      <c r="A154" s="212" t="s">
         <v>252</v>
       </c>
-      <c r="B154" s="182"/>
-      <c r="C154" s="176"/>
-      <c r="D154" s="176"/>
+      <c r="B154" s="212"/>
+      <c r="C154" s="175"/>
+      <c r="D154" s="175"/>
     </row>
     <row r="155" spans="1:4" ht="15.75" thickBot="1">
       <c r="A155" s="25" t="s">
@@ -7462,10 +7470,10 @@
     </row>
     <row r="156" spans="1:4" ht="15.75" thickBot="1">
       <c r="A156" s="54" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B156" s="55" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -7495,12 +7503,12 @@
       <c r="D160" s="2"/>
     </row>
     <row r="161" spans="1:4" ht="49.5" customHeight="1" thickBot="1">
-      <c r="A161" s="183" t="s">
+      <c r="A161" s="213" t="s">
         <v>206</v>
       </c>
-      <c r="B161" s="183"/>
-      <c r="C161" s="184"/>
-      <c r="D161" s="184"/>
+      <c r="B161" s="213"/>
+      <c r="C161" s="214"/>
+      <c r="D161" s="214"/>
     </row>
     <row r="162" spans="1:4" ht="29.25" thickBot="1">
       <c r="A162" s="25" t="s">
@@ -7571,10 +7579,10 @@
       <c r="D168" s="2"/>
     </row>
     <row r="169" spans="1:4" ht="39" customHeight="1" thickBot="1">
-      <c r="A169" s="170" t="s">
+      <c r="A169" s="218" t="s">
         <v>254</v>
       </c>
-      <c r="B169" s="170"/>
+      <c r="B169" s="218"/>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
     </row>
@@ -7590,7 +7598,7 @@
     </row>
     <row r="171" spans="1:4" ht="30.75" thickBot="1">
       <c r="A171" s="53" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B171" s="55" t="s">
         <v>255</v>
@@ -7600,10 +7608,10 @@
     </row>
     <row r="172" spans="1:4" ht="15.75" thickBot="1">
       <c r="A172" s="53" t="s">
+        <v>467</v>
+      </c>
+      <c r="B172" s="55" t="s">
         <v>468</v>
-      </c>
-      <c r="B172" s="55" t="s">
-        <v>469</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -7619,10 +7627,10 @@
       <c r="D173" s="2"/>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="169" t="s">
+      <c r="A174" s="219" t="s">
         <v>210</v>
       </c>
-      <c r="B174" s="169"/>
+      <c r="B174" s="219"/>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
     </row>
@@ -7633,22 +7641,22 @@
       <c r="D175" s="2"/>
     </row>
     <row r="176" spans="1:4" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A176" s="174" t="s">
+      <c r="A176" s="220" t="s">
         <v>211</v>
       </c>
-      <c r="B176" s="174"/>
-      <c r="C176" s="176"/>
-      <c r="D176" s="176"/>
+      <c r="B176" s="220"/>
+      <c r="C176" s="175"/>
+      <c r="D176" s="175"/>
     </row>
     <row r="177" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="A177" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="B177" s="186" t="s">
+      <c r="B177" s="222" t="s">
         <v>414</v>
       </c>
-      <c r="C177" s="187"/>
-      <c r="D177" s="188"/>
+      <c r="C177" s="223"/>
+      <c r="D177" s="224"/>
     </row>
     <row r="178" spans="1:7">
       <c r="A178" s="2"/>
@@ -7657,12 +7665,12 @@
       <c r="D178" s="2"/>
     </row>
     <row r="179" spans="1:7" ht="75.75" customHeight="1">
-      <c r="A179" s="185" t="s">
+      <c r="A179" s="221" t="s">
         <v>213</v>
       </c>
-      <c r="B179" s="185"/>
-      <c r="C179" s="176"/>
-      <c r="D179" s="176"/>
+      <c r="B179" s="221"/>
+      <c r="C179" s="175"/>
+      <c r="D179" s="175"/>
     </row>
     <row r="180" spans="1:7" ht="15.75" thickBot="1">
       <c r="A180" s="2"/>
@@ -7683,25 +7691,25 @@
     </row>
     <row r="182" spans="1:7" ht="60.75" thickBot="1">
       <c r="A182" s="53" t="s">
+        <v>469</v>
+      </c>
+      <c r="B182" s="167" t="s">
+        <v>471</v>
+      </c>
+      <c r="C182" s="53" t="s">
         <v>470</v>
-      </c>
-      <c r="B182" s="167" t="s">
-        <v>472</v>
-      </c>
-      <c r="C182" s="53" t="s">
-        <v>471</v>
       </c>
       <c r="G182" s="166"/>
     </row>
     <row r="183" spans="1:7" ht="45.75" thickBot="1">
       <c r="A183" s="53" t="s">
+        <v>472</v>
+      </c>
+      <c r="B183" s="53" t="s">
         <v>473</v>
       </c>
-      <c r="B183" s="53" t="s">
+      <c r="C183" s="54" t="s">
         <v>474</v>
-      </c>
-      <c r="C183" s="54" t="s">
-        <v>475</v>
       </c>
       <c r="G183" s="166"/>
     </row>
@@ -7717,20 +7725,20 @@
       </c>
     </row>
     <row r="185" spans="1:7">
-      <c r="A185" s="169"/>
-      <c r="B185" s="169"/>
+      <c r="A185" s="219"/>
+      <c r="B185" s="219"/>
     </row>
     <row r="186" spans="1:7">
       <c r="A186" s="39"/>
       <c r="B186" s="39"/>
     </row>
     <row r="187" spans="1:7" ht="63" customHeight="1" thickBot="1">
-      <c r="A187" s="183" t="s">
+      <c r="A187" s="213" t="s">
         <v>216</v>
       </c>
-      <c r="B187" s="183"/>
-      <c r="C187" s="184"/>
-      <c r="D187" s="184"/>
+      <c r="B187" s="213"/>
+      <c r="C187" s="214"/>
+      <c r="D187" s="214"/>
     </row>
     <row r="188" spans="1:7" ht="26.25" customHeight="1" thickBot="1">
       <c r="A188" s="25" t="s">
@@ -7771,20 +7779,20 @@
       <c r="D191" s="55"/>
     </row>
     <row r="192" spans="1:7">
-      <c r="A192" s="181"/>
-      <c r="B192" s="181"/>
+      <c r="A192" s="230"/>
+      <c r="B192" s="230"/>
     </row>
     <row r="193" spans="1:6">
       <c r="A193" s="41"/>
       <c r="B193" s="41"/>
     </row>
     <row r="194" spans="1:6" ht="54.75" customHeight="1">
-      <c r="A194" s="182" t="s">
+      <c r="A194" s="212" t="s">
         <v>260</v>
       </c>
-      <c r="B194" s="182"/>
-      <c r="C194" s="176"/>
-      <c r="D194" s="176"/>
+      <c r="B194" s="212"/>
+      <c r="C194" s="175"/>
+      <c r="D194" s="175"/>
       <c r="F194" t="s">
         <v>415</v>
       </c>
@@ -7832,12 +7840,12 @@
       <c r="D202" s="2"/>
     </row>
     <row r="203" spans="1:6" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A203" s="177" t="s">
+      <c r="A203" s="225" t="s">
         <v>219</v>
       </c>
-      <c r="B203" s="177"/>
-      <c r="C203" s="178"/>
-      <c r="D203" s="178"/>
+      <c r="B203" s="225"/>
+      <c r="C203" s="226"/>
+      <c r="D203" s="226"/>
     </row>
     <row r="204" spans="1:6" ht="15.75" thickBot="1">
       <c r="A204" s="22" t="s">
@@ -7886,8 +7894,8 @@
       <c r="D208" s="2"/>
     </row>
     <row r="209" spans="1:6">
-      <c r="A209" s="169"/>
-      <c r="B209" s="169"/>
+      <c r="A209" s="219"/>
+      <c r="B209" s="219"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
     </row>
@@ -7898,12 +7906,12 @@
       <c r="D210" s="2"/>
     </row>
     <row r="211" spans="1:6" ht="54.75" customHeight="1">
-      <c r="A211" s="172" t="s">
+      <c r="A211" s="227" t="s">
         <v>265</v>
       </c>
-      <c r="B211" s="172"/>
-      <c r="C211" s="173"/>
-      <c r="D211" s="173"/>
+      <c r="B211" s="227"/>
+      <c r="C211" s="176"/>
+      <c r="D211" s="176"/>
       <c r="F211" t="s">
         <v>419</v>
       </c>
@@ -7926,11 +7934,15 @@
       </c>
     </row>
     <row r="214" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A214" s="53"/>
+      <c r="A214" s="53" t="s">
+        <v>475</v>
+      </c>
       <c r="B214" s="55"/>
     </row>
-    <row r="215" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A215" s="53"/>
+    <row r="215" spans="1:6" ht="30.75" thickBot="1">
+      <c r="A215" s="53" t="s">
+        <v>476</v>
+      </c>
       <c r="B215" s="55"/>
     </row>
     <row r="216" spans="1:6" ht="15.75" thickBot="1">
@@ -7942,19 +7954,19 @@
       <c r="B217" s="55"/>
     </row>
     <row r="218" spans="1:6">
-      <c r="A218" s="169"/>
-      <c r="B218" s="169"/>
+      <c r="A218" s="219"/>
+      <c r="B218" s="219"/>
     </row>
     <row r="219" spans="1:6">
       <c r="A219" s="43"/>
     </row>
     <row r="220" spans="1:6" ht="33" customHeight="1" thickBot="1">
-      <c r="A220" s="179" t="s">
+      <c r="A220" s="228" t="s">
         <v>266</v>
       </c>
-      <c r="B220" s="179"/>
-      <c r="C220" s="180"/>
-      <c r="D220" s="180"/>
+      <c r="B220" s="228"/>
+      <c r="C220" s="229"/>
+      <c r="D220" s="229"/>
     </row>
     <row r="221" spans="1:6" ht="15.75" thickBot="1">
       <c r="A221" s="25" t="s">
@@ -8003,12 +8015,12 @@
       <c r="B226" s="39"/>
     </row>
     <row r="227" spans="1:6" ht="47.25" customHeight="1">
-      <c r="A227" s="174" t="s">
+      <c r="A227" s="220" t="s">
         <v>222</v>
       </c>
-      <c r="B227" s="174"/>
-      <c r="C227" s="176"/>
-      <c r="D227" s="176"/>
+      <c r="B227" s="220"/>
+      <c r="C227" s="175"/>
+      <c r="D227" s="175"/>
     </row>
     <row r="228" spans="1:6" ht="45">
       <c r="A228" s="44" t="s">
@@ -8019,12 +8031,12 @@
       </c>
     </row>
     <row r="230" spans="1:6" ht="36" customHeight="1">
-      <c r="A230" s="172" t="s">
+      <c r="A230" s="227" t="s">
         <v>224</v>
       </c>
-      <c r="B230" s="172"/>
-      <c r="C230" s="173"/>
-      <c r="D230" s="173"/>
+      <c r="B230" s="227"/>
+      <c r="C230" s="176"/>
+      <c r="D230" s="176"/>
     </row>
     <row r="231" spans="1:6">
       <c r="A231" s="44" t="s">
@@ -8046,19 +8058,19 @@
       </c>
     </row>
     <row r="234" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A234" s="172" t="s">
+      <c r="A234" s="227" t="s">
         <v>225</v>
       </c>
-      <c r="B234" s="172"/>
-      <c r="C234" s="173"/>
-      <c r="D234" s="173"/>
-    </row>
-    <row r="235" spans="1:6" ht="90">
+      <c r="B234" s="227"/>
+      <c r="C234" s="176"/>
+      <c r="D234" s="176"/>
+    </row>
+    <row r="235" spans="1:6" ht="105">
       <c r="A235" s="44" t="s">
         <v>223</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>424</v>
+        <v>477</v>
       </c>
     </row>
     <row r="237" spans="1:6" ht="20.25">
@@ -8067,12 +8079,12 @@
       </c>
     </row>
     <row r="238" spans="1:6" ht="49.5" customHeight="1">
-      <c r="A238" s="172" t="s">
+      <c r="A238" s="227" t="s">
         <v>226</v>
       </c>
-      <c r="B238" s="172"/>
-      <c r="C238" s="173"/>
-      <c r="D238" s="173"/>
+      <c r="B238" s="227"/>
+      <c r="C238" s="176"/>
+      <c r="D238" s="176"/>
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="44" t="s">
@@ -8082,21 +8094,21 @@
         <v>9</v>
       </c>
       <c r="F239" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="240" spans="1:6">
       <c r="F240" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="33" customHeight="1">
-      <c r="A241" s="172" t="s">
+      <c r="A241" s="227" t="s">
         <v>227</v>
       </c>
-      <c r="B241" s="172"/>
-      <c r="C241" s="173"/>
-      <c r="D241" s="173"/>
+      <c r="B241" s="227"/>
+      <c r="C241" s="176"/>
+      <c r="D241" s="176"/>
     </row>
     <row r="242" spans="1:4">
       <c r="A242" s="44" t="s">
@@ -8107,12 +8119,12 @@
       </c>
     </row>
     <row r="244" spans="1:4" ht="41.25" customHeight="1">
-      <c r="A244" s="172" t="s">
+      <c r="A244" s="227" t="s">
         <v>228</v>
       </c>
-      <c r="B244" s="172"/>
-      <c r="C244" s="173"/>
-      <c r="D244" s="173"/>
+      <c r="B244" s="227"/>
+      <c r="C244" s="176"/>
+      <c r="D244" s="176"/>
     </row>
     <row r="245" spans="1:4">
       <c r="A245" s="44" t="s">
@@ -8123,12 +8135,12 @@
       </c>
     </row>
     <row r="247" spans="1:4" ht="38.25" customHeight="1">
-      <c r="A247" s="174" t="s">
+      <c r="A247" s="220" t="s">
         <v>229</v>
       </c>
-      <c r="B247" s="174"/>
-      <c r="C247" s="173"/>
-      <c r="D247" s="173"/>
+      <c r="B247" s="220"/>
+      <c r="C247" s="176"/>
+      <c r="D247" s="176"/>
     </row>
     <row r="248" spans="1:4">
       <c r="A248" s="44" t="s">
@@ -8144,12 +8156,12 @@
       </c>
     </row>
     <row r="251" spans="1:4" ht="45" customHeight="1">
-      <c r="A251" s="172" t="s">
+      <c r="A251" s="227" t="s">
         <v>230</v>
       </c>
-      <c r="B251" s="172"/>
-      <c r="C251" s="173"/>
-      <c r="D251" s="173"/>
+      <c r="B251" s="227"/>
+      <c r="C251" s="176"/>
+      <c r="D251" s="176"/>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" s="44" t="s">
@@ -8165,12 +8177,12 @@
       </c>
     </row>
     <row r="255" spans="1:4" ht="42" customHeight="1">
-      <c r="A255" s="175" t="s">
+      <c r="A255" s="231" t="s">
         <v>231</v>
       </c>
-      <c r="B255" s="175"/>
-      <c r="C255" s="173"/>
-      <c r="D255" s="173"/>
+      <c r="B255" s="231"/>
+      <c r="C255" s="176"/>
+      <c r="D255" s="176"/>
     </row>
     <row r="256" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="257" spans="1:4" ht="15.75" thickBot="1">
@@ -8223,10 +8235,10 @@
       </c>
     </row>
     <row r="264" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A264" s="172" t="s">
+      <c r="A264" s="227" t="s">
         <v>234</v>
       </c>
-      <c r="B264" s="173"/>
+      <c r="B264" s="176"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="47"/>
@@ -8237,12 +8249,12 @@
       </c>
     </row>
     <row r="267" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A267" s="172" t="s">
+      <c r="A267" s="227" t="s">
         <v>235</v>
       </c>
-      <c r="B267" s="172"/>
-      <c r="C267" s="173"/>
-      <c r="D267" s="173"/>
+      <c r="B267" s="227"/>
+      <c r="C267" s="176"/>
+      <c r="D267" s="176"/>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" s="44" t="s">
@@ -8250,12 +8262,12 @@
       </c>
     </row>
     <row r="270" spans="1:4">
-      <c r="A270" s="172" t="s">
+      <c r="A270" s="227" t="s">
         <v>236</v>
       </c>
-      <c r="B270" s="172"/>
-      <c r="C270" s="173"/>
-      <c r="D270" s="173"/>
+      <c r="B270" s="227"/>
+      <c r="C270" s="176"/>
+      <c r="D270" s="176"/>
     </row>
     <row r="271" spans="1:4">
       <c r="A271" s="44" t="s">
@@ -8264,16 +8276,16 @@
     </row>
     <row r="272" spans="1:4" ht="25.5" customHeight="1"/>
     <row r="273" spans="1:4" ht="49.5" customHeight="1">
-      <c r="A273" s="172" t="s">
+      <c r="A273" s="227" t="s">
         <v>237</v>
       </c>
-      <c r="B273" s="172"/>
+      <c r="B273" s="227"/>
     </row>
     <row r="274" spans="1:4" ht="59.25" customHeight="1">
-      <c r="A274" s="172" t="s">
+      <c r="A274" s="227" t="s">
         <v>238</v>
       </c>
-      <c r="B274" s="172"/>
+      <c r="B274" s="227"/>
     </row>
     <row r="275" spans="1:4">
       <c r="A275" s="44" t="s">
@@ -8281,12 +8293,12 @@
       </c>
     </row>
     <row r="277" spans="1:4" ht="55.5" customHeight="1" thickBot="1">
-      <c r="A277" s="170" t="s">
+      <c r="A277" s="218" t="s">
         <v>239</v>
       </c>
-      <c r="B277" s="170"/>
-      <c r="C277" s="171"/>
-      <c r="D277" s="171"/>
+      <c r="B277" s="218"/>
+      <c r="C277" s="232"/>
+      <c r="D277" s="232"/>
     </row>
     <row r="278" spans="1:4" ht="15.75" thickBot="1">
       <c r="A278" s="25" t="s">
@@ -8319,8 +8331,8 @@
       <c r="D280" s="12"/>
     </row>
     <row r="281" spans="1:4">
-      <c r="A281" s="169"/>
-      <c r="B281" s="169"/>
+      <c r="A281" s="219"/>
+      <c r="B281" s="219"/>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" s="39"/>
@@ -8345,12 +8357,12 @@
       </c>
     </row>
     <row r="287" spans="1:4" ht="39" customHeight="1">
-      <c r="A287" s="172" t="s">
+      <c r="A287" s="227" t="s">
         <v>241</v>
       </c>
-      <c r="B287" s="172"/>
-      <c r="C287" s="173"/>
-      <c r="D287" s="173"/>
+      <c r="B287" s="227"/>
+      <c r="C287" s="176"/>
+      <c r="D287" s="176"/>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="44" t="s">
@@ -8359,12 +8371,12 @@
       <c r="B288" s="8"/>
     </row>
     <row r="290" spans="1:4" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A290" s="170" t="s">
+      <c r="A290" s="218" t="s">
         <v>242</v>
       </c>
-      <c r="B290" s="170"/>
-      <c r="C290" s="171"/>
-      <c r="D290" s="171"/>
+      <c r="B290" s="218"/>
+      <c r="C290" s="232"/>
+      <c r="D290" s="232"/>
     </row>
     <row r="291" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="292" spans="1:4" ht="15.75" thickBot="1">
@@ -8407,6 +8419,60 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="A281:B281"/>
+    <mergeCell ref="A277:D277"/>
+    <mergeCell ref="A287:D287"/>
+    <mergeCell ref="A290:D290"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="A264:B264"/>
+    <mergeCell ref="A267:D267"/>
+    <mergeCell ref="A270:D270"/>
+    <mergeCell ref="A241:D241"/>
+    <mergeCell ref="A244:D244"/>
+    <mergeCell ref="A247:D247"/>
+    <mergeCell ref="A255:D255"/>
+    <mergeCell ref="A251:D251"/>
+    <mergeCell ref="A227:D227"/>
+    <mergeCell ref="A230:D230"/>
+    <mergeCell ref="A234:D234"/>
+    <mergeCell ref="A238:D238"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A203:D203"/>
+    <mergeCell ref="A211:D211"/>
+    <mergeCell ref="A220:D220"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="A194:D194"/>
+    <mergeCell ref="A187:D187"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A176:D176"/>
+    <mergeCell ref="A179:D179"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="B177:D177"/>
+    <mergeCell ref="A147:D147"/>
+    <mergeCell ref="A154:D154"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A34:E34"/>
@@ -8421,60 +8487,6 @@
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A147:D147"/>
-    <mergeCell ref="A154:D154"/>
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A127:C127"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A176:D176"/>
-    <mergeCell ref="A179:D179"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="B177:D177"/>
-    <mergeCell ref="A203:D203"/>
-    <mergeCell ref="A211:D211"/>
-    <mergeCell ref="A220:D220"/>
-    <mergeCell ref="A185:B185"/>
-    <mergeCell ref="A192:B192"/>
-    <mergeCell ref="A194:D194"/>
-    <mergeCell ref="A187:D187"/>
-    <mergeCell ref="A227:D227"/>
-    <mergeCell ref="A230:D230"/>
-    <mergeCell ref="A234:D234"/>
-    <mergeCell ref="A238:D238"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A264:B264"/>
-    <mergeCell ref="A267:D267"/>
-    <mergeCell ref="A270:D270"/>
-    <mergeCell ref="A241:D241"/>
-    <mergeCell ref="A244:D244"/>
-    <mergeCell ref="A247:D247"/>
-    <mergeCell ref="A255:D255"/>
-    <mergeCell ref="A251:D251"/>
-    <mergeCell ref="A281:B281"/>
-    <mergeCell ref="A277:D277"/>
-    <mergeCell ref="A287:D287"/>
-    <mergeCell ref="A290:D290"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="A274:B274"/>
   </mergeCells>
   <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8522,11 +8534,11 @@
       <c r="D1" s="106" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="213" t="s">
+      <c r="E1" s="244" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="213"/>
-      <c r="G1" s="213"/>
+      <c r="F1" s="244"/>
+      <c r="G1" s="244"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -8608,15 +8620,15 @@
       <c r="P3" s="107"/>
     </row>
     <row r="4" spans="1:26 16384:16384" s="16" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A4" s="214" t="s">
+      <c r="A4" s="245" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="214"/>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
+      <c r="B4" s="245"/>
+      <c r="C4" s="245"/>
+      <c r="D4" s="245"/>
+      <c r="E4" s="245"/>
+      <c r="F4" s="245"/>
+      <c r="G4" s="245"/>
       <c r="H4" s="150"/>
       <c r="I4" s="151"/>
       <c r="J4" s="151"/>
@@ -8685,12 +8697,12 @@
       <c r="N6" s="95"/>
       <c r="O6" s="95"/>
       <c r="P6" s="95"/>
-      <c r="R6" s="221" t="s">
+      <c r="R6" s="233" t="s">
         <v>278</v>
       </c>
-      <c r="S6" s="222"/>
-      <c r="T6" s="222"/>
-      <c r="U6" s="222"/>
+      <c r="S6" s="234"/>
+      <c r="T6" s="234"/>
+      <c r="U6" s="234"/>
     </row>
     <row r="7" spans="1:26 16384:16384" s="16" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="108" t="s">
@@ -8719,10 +8731,10 @@
       <c r="N7" s="63"/>
       <c r="O7" s="64"/>
       <c r="P7" s="64"/>
-      <c r="R7" s="222"/>
-      <c r="S7" s="222"/>
-      <c r="T7" s="222"/>
-      <c r="U7" s="222"/>
+      <c r="R7" s="234"/>
+      <c r="S7" s="234"/>
+      <c r="T7" s="234"/>
+      <c r="U7" s="234"/>
     </row>
     <row r="8" spans="1:26 16384:16384" s="16" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="108" t="s">
@@ -8751,10 +8763,10 @@
       <c r="N8" s="62"/>
       <c r="O8" s="62"/>
       <c r="P8" s="62"/>
-      <c r="R8" s="222"/>
-      <c r="S8" s="222"/>
-      <c r="T8" s="222"/>
-      <c r="U8" s="222"/>
+      <c r="R8" s="234"/>
+      <c r="S8" s="234"/>
+      <c r="T8" s="234"/>
+      <c r="U8" s="234"/>
     </row>
     <row r="9" spans="1:26 16384:16384" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A9" s="108" t="s">
@@ -8783,10 +8795,10 @@
       <c r="N9" s="62"/>
       <c r="O9" s="62"/>
       <c r="P9" s="62"/>
-      <c r="R9" s="222"/>
-      <c r="S9" s="222"/>
-      <c r="T9" s="222"/>
-      <c r="U9" s="222"/>
+      <c r="R9" s="234"/>
+      <c r="S9" s="234"/>
+      <c r="T9" s="234"/>
+      <c r="U9" s="234"/>
     </row>
     <row r="10" spans="1:26 16384:16384" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A10" s="108" t="s">
@@ -8815,10 +8827,10 @@
       <c r="N10" s="62"/>
       <c r="O10" s="62"/>
       <c r="P10" s="62"/>
-      <c r="R10" s="222"/>
-      <c r="S10" s="222"/>
-      <c r="T10" s="222"/>
-      <c r="U10" s="222"/>
+      <c r="R10" s="234"/>
+      <c r="S10" s="234"/>
+      <c r="T10" s="234"/>
+      <c r="U10" s="234"/>
       <c r="XFD10" s="73"/>
     </row>
     <row r="11" spans="1:26 16384:16384" s="16" customFormat="1" ht="30.75" thickBot="1">
@@ -8848,10 +8860,10 @@
       <c r="N11" s="62"/>
       <c r="O11" s="62"/>
       <c r="P11" s="62"/>
-      <c r="R11" s="222"/>
-      <c r="S11" s="222"/>
-      <c r="T11" s="222"/>
-      <c r="U11" s="222"/>
+      <c r="R11" s="234"/>
+      <c r="S11" s="234"/>
+      <c r="T11" s="234"/>
+      <c r="U11" s="234"/>
     </row>
     <row r="12" spans="1:26 16384:16384" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A12" s="108" t="s">
@@ -8880,10 +8892,10 @@
       <c r="N12" s="62"/>
       <c r="O12" s="62"/>
       <c r="P12" s="62"/>
-      <c r="R12" s="222"/>
-      <c r="S12" s="222"/>
-      <c r="T12" s="222"/>
-      <c r="U12" s="222"/>
+      <c r="R12" s="234"/>
+      <c r="S12" s="234"/>
+      <c r="T12" s="234"/>
+      <c r="U12" s="234"/>
     </row>
     <row r="13" spans="1:26 16384:16384" s="16" customFormat="1" ht="30.75" thickBot="1">
       <c r="A13" s="108" t="s">
@@ -8896,7 +8908,7 @@
         <v>305</v>
       </c>
       <c r="D13" s="108" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E13" s="111" t="s">
         <v>273</v>
@@ -8913,10 +8925,10 @@
       <c r="O13" s="62"/>
       <c r="P13" s="62"/>
       <c r="Q13" s="17"/>
-      <c r="R13" s="222"/>
-      <c r="S13" s="222"/>
-      <c r="T13" s="222"/>
-      <c r="U13" s="222"/>
+      <c r="R13" s="234"/>
+      <c r="S13" s="234"/>
+      <c r="T13" s="234"/>
+      <c r="U13" s="234"/>
       <c r="V13" s="17"/>
       <c r="W13" s="17"/>
       <c r="X13" s="17"/>
@@ -8951,10 +8963,10 @@
       <c r="O14" s="70"/>
       <c r="P14" s="70"/>
       <c r="Q14" s="17"/>
-      <c r="R14" s="222"/>
-      <c r="S14" s="222"/>
-      <c r="T14" s="222"/>
-      <c r="U14" s="222"/>
+      <c r="R14" s="234"/>
+      <c r="S14" s="234"/>
+      <c r="T14" s="234"/>
+      <c r="U14" s="234"/>
       <c r="V14" s="17"/>
       <c r="W14" s="17"/>
       <c r="X14" s="17"/>
@@ -8989,10 +9001,10 @@
       <c r="O15" s="70"/>
       <c r="P15" s="70"/>
       <c r="Q15" s="17"/>
-      <c r="R15" s="222"/>
-      <c r="S15" s="222"/>
-      <c r="T15" s="222"/>
-      <c r="U15" s="222"/>
+      <c r="R15" s="234"/>
+      <c r="S15" s="234"/>
+      <c r="T15" s="234"/>
+      <c r="U15" s="234"/>
       <c r="V15" s="17"/>
       <c r="W15" s="17"/>
       <c r="X15" s="17"/>
@@ -9025,10 +9037,10 @@
       <c r="O16" s="70"/>
       <c r="P16" s="70"/>
       <c r="Q16" s="17"/>
-      <c r="R16" s="222"/>
-      <c r="S16" s="222"/>
-      <c r="T16" s="222"/>
-      <c r="U16" s="222"/>
+      <c r="R16" s="234"/>
+      <c r="S16" s="234"/>
+      <c r="T16" s="234"/>
+      <c r="U16" s="234"/>
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
       <c r="X16" s="17"/>
@@ -9063,10 +9075,10 @@
       <c r="O17" s="70"/>
       <c r="P17" s="70"/>
       <c r="Q17" s="17"/>
-      <c r="R17" s="222"/>
-      <c r="S17" s="222"/>
-      <c r="T17" s="222"/>
-      <c r="U17" s="222"/>
+      <c r="R17" s="234"/>
+      <c r="S17" s="234"/>
+      <c r="T17" s="234"/>
+      <c r="U17" s="234"/>
       <c r="V17" s="17"/>
       <c r="W17" s="17"/>
       <c r="X17" s="17"/>
@@ -9092,7 +9104,7 @@
       <c r="F18" s="111"/>
       <c r="G18" s="113"/>
       <c r="H18" s="67" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I18" s="82"/>
       <c r="J18" s="83"/>
@@ -9406,15 +9418,15 @@
       <c r="Z26" s="17"/>
     </row>
     <row r="27" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A27" s="215" t="s">
+      <c r="A27" s="235" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="216"/>
-      <c r="C27" s="216"/>
-      <c r="D27" s="216"/>
-      <c r="E27" s="216"/>
-      <c r="F27" s="216"/>
-      <c r="G27" s="216"/>
+      <c r="B27" s="236"/>
+      <c r="C27" s="236"/>
+      <c r="D27" s="236"/>
+      <c r="E27" s="236"/>
+      <c r="F27" s="236"/>
+      <c r="G27" s="236"/>
       <c r="H27" s="139"/>
       <c r="I27" s="140"/>
       <c r="J27" s="140"/>
@@ -9740,15 +9752,15 @@
       <c r="Z35" s="17"/>
     </row>
     <row r="36" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A36" s="215" t="s">
+      <c r="A36" s="235" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="216"/>
-      <c r="C36" s="217"/>
-      <c r="D36" s="216"/>
-      <c r="E36" s="216"/>
-      <c r="F36" s="216"/>
-      <c r="G36" s="217"/>
+      <c r="B36" s="236"/>
+      <c r="C36" s="237"/>
+      <c r="D36" s="236"/>
+      <c r="E36" s="236"/>
+      <c r="F36" s="236"/>
+      <c r="G36" s="237"/>
       <c r="H36" s="139"/>
       <c r="I36" s="140"/>
       <c r="J36" s="140"/>
@@ -9846,11 +9858,11 @@
       <c r="Z38" s="17"/>
     </row>
     <row r="39" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A39" s="218" t="s">
+      <c r="A39" s="246" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="219"/>
-      <c r="C39" s="220"/>
+      <c r="B39" s="247"/>
+      <c r="C39" s="248"/>
       <c r="D39" s="124"/>
       <c r="E39" s="125"/>
       <c r="F39" s="125"/>
@@ -10679,7 +10691,7 @@
       <c r="K61" s="67"/>
       <c r="L61" s="67"/>
       <c r="M61" s="128" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="N61" s="69"/>
       <c r="O61" s="69"/>
@@ -10755,7 +10767,7 @@
       <c r="K63" s="80"/>
       <c r="L63" s="80"/>
       <c r="M63" s="128" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N63" s="70"/>
       <c r="O63" s="70"/>
@@ -10899,7 +10911,7 @@
         <v>288</v>
       </c>
       <c r="E67" s="127" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F67" s="119"/>
       <c r="G67" s="88"/>
@@ -10937,7 +10949,7 @@
         <v>288</v>
       </c>
       <c r="E68" s="127" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F68" s="119"/>
       <c r="G68" s="88"/>
@@ -10947,7 +10959,7 @@
       <c r="K68" s="67"/>
       <c r="L68" s="67"/>
       <c r="M68" s="128" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="N68" s="69"/>
       <c r="O68" s="69"/>
@@ -10977,7 +10989,7 @@
         <v>279</v>
       </c>
       <c r="E69" s="127" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F69" s="119"/>
       <c r="G69" s="88"/>
@@ -10987,7 +10999,7 @@
       <c r="K69" s="67"/>
       <c r="L69" s="67"/>
       <c r="M69" s="128" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="N69" s="69"/>
       <c r="O69" s="69"/>
@@ -11004,15 +11016,15 @@
       <c r="Z69" s="17"/>
     </row>
     <row r="70" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A70" s="215" t="s">
+      <c r="A70" s="235" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="216"/>
-      <c r="C70" s="216"/>
-      <c r="D70" s="217"/>
-      <c r="E70" s="216"/>
-      <c r="F70" s="216"/>
-      <c r="G70" s="216"/>
+      <c r="B70" s="236"/>
+      <c r="C70" s="236"/>
+      <c r="D70" s="237"/>
+      <c r="E70" s="236"/>
+      <c r="F70" s="236"/>
+      <c r="G70" s="236"/>
       <c r="H70" s="139"/>
       <c r="I70" s="140"/>
       <c r="J70" s="140"/>
@@ -11209,7 +11221,7 @@
       <c r="K75" s="67"/>
       <c r="L75" s="67"/>
       <c r="M75" s="128" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="N75" s="69"/>
       <c r="O75" s="69"/>
@@ -11239,7 +11251,7 @@
         <v>279</v>
       </c>
       <c r="E76" s="127" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F76" s="119"/>
       <c r="G76" s="88"/>
@@ -11249,7 +11261,7 @@
       <c r="K76" s="67"/>
       <c r="L76" s="67"/>
       <c r="M76" s="128" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N76" s="69"/>
       <c r="O76" s="69"/>
@@ -11456,15 +11468,15 @@
       <c r="Z81" s="17"/>
     </row>
     <row r="82" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A82" s="215" t="s">
+      <c r="A82" s="235" t="s">
         <v>132</v>
       </c>
-      <c r="B82" s="217"/>
-      <c r="C82" s="217"/>
-      <c r="D82" s="223"/>
-      <c r="E82" s="216"/>
-      <c r="F82" s="216"/>
-      <c r="G82" s="216"/>
+      <c r="B82" s="237"/>
+      <c r="C82" s="237"/>
+      <c r="D82" s="238"/>
+      <c r="E82" s="236"/>
+      <c r="F82" s="236"/>
+      <c r="G82" s="236"/>
       <c r="H82" s="139"/>
       <c r="I82" s="140"/>
       <c r="J82" s="140"/>
@@ -11676,15 +11688,15 @@
       <c r="Z87" s="17"/>
     </row>
     <row r="88" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A88" s="215" t="s">
+      <c r="A88" s="235" t="s">
         <v>138</v>
       </c>
-      <c r="B88" s="217"/>
-      <c r="C88" s="223"/>
-      <c r="D88" s="223"/>
-      <c r="E88" s="216"/>
-      <c r="F88" s="216"/>
-      <c r="G88" s="216"/>
+      <c r="B88" s="237"/>
+      <c r="C88" s="238"/>
+      <c r="D88" s="238"/>
+      <c r="E88" s="236"/>
+      <c r="F88" s="236"/>
+      <c r="G88" s="236"/>
       <c r="H88" s="139"/>
       <c r="I88" s="140"/>
       <c r="J88" s="140"/>
@@ -11841,7 +11853,7 @@
       <c r="K92" s="67"/>
       <c r="L92" s="67"/>
       <c r="M92" s="114" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N92" s="69"/>
       <c r="O92" s="69"/>
@@ -11879,7 +11891,7 @@
       <c r="K93" s="67"/>
       <c r="L93" s="67"/>
       <c r="M93" s="114" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="N93" s="69"/>
       <c r="O93" s="69"/>
@@ -11896,15 +11908,15 @@
       <c r="Z93" s="17"/>
     </row>
     <row r="94" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A94" s="224" t="s">
+      <c r="A94" s="239" t="s">
         <v>144</v>
       </c>
-      <c r="B94" s="225"/>
-      <c r="C94" s="226"/>
-      <c r="D94" s="226"/>
-      <c r="E94" s="227"/>
-      <c r="F94" s="227"/>
-      <c r="G94" s="227"/>
+      <c r="B94" s="240"/>
+      <c r="C94" s="241"/>
+      <c r="D94" s="241"/>
+      <c r="E94" s="242"/>
+      <c r="F94" s="242"/>
+      <c r="G94" s="242"/>
       <c r="H94" s="139"/>
       <c r="I94" s="140"/>
       <c r="J94" s="140"/>
@@ -12002,15 +12014,15 @@
       <c r="Z96" s="17"/>
     </row>
     <row r="97" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A97" s="215" t="s">
+      <c r="A97" s="235" t="s">
         <v>147</v>
       </c>
-      <c r="B97" s="216"/>
-      <c r="C97" s="216"/>
-      <c r="D97" s="216"/>
-      <c r="E97" s="216"/>
-      <c r="F97" s="216"/>
-      <c r="G97" s="216"/>
+      <c r="B97" s="236"/>
+      <c r="C97" s="236"/>
+      <c r="D97" s="236"/>
+      <c r="E97" s="236"/>
+      <c r="F97" s="236"/>
+      <c r="G97" s="236"/>
       <c r="H97" s="139"/>
       <c r="I97" s="140"/>
       <c r="J97" s="140"/>
@@ -12070,15 +12082,15 @@
       <c r="Z98" s="17"/>
     </row>
     <row r="99" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A99" s="215" t="s">
+      <c r="A99" s="235" t="s">
         <v>149</v>
       </c>
-      <c r="B99" s="217"/>
-      <c r="C99" s="217"/>
-      <c r="D99" s="217"/>
-      <c r="E99" s="216"/>
-      <c r="F99" s="216"/>
-      <c r="G99" s="216"/>
+      <c r="B99" s="237"/>
+      <c r="C99" s="237"/>
+      <c r="D99" s="237"/>
+      <c r="E99" s="236"/>
+      <c r="F99" s="236"/>
+      <c r="G99" s="236"/>
       <c r="H99" s="139"/>
       <c r="I99" s="140"/>
       <c r="J99" s="140"/>
@@ -12212,15 +12224,15 @@
       <c r="Z102" s="17"/>
     </row>
     <row r="103" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A103" s="228" t="s">
+      <c r="A103" s="243" t="s">
         <v>154</v>
       </c>
-      <c r="B103" s="223"/>
-      <c r="C103" s="223"/>
-      <c r="D103" s="223"/>
-      <c r="E103" s="217"/>
-      <c r="F103" s="217"/>
-      <c r="G103" s="217"/>
+      <c r="B103" s="238"/>
+      <c r="C103" s="238"/>
+      <c r="D103" s="238"/>
+      <c r="E103" s="237"/>
+      <c r="F103" s="237"/>
+      <c r="G103" s="237"/>
       <c r="H103" s="139"/>
       <c r="I103" s="140"/>
       <c r="J103" s="140"/>
@@ -12394,15 +12406,15 @@
       <c r="Z107" s="17"/>
     </row>
     <row r="108" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A108" s="215" t="s">
+      <c r="A108" s="235" t="s">
         <v>159</v>
       </c>
-      <c r="B108" s="217"/>
-      <c r="C108" s="223"/>
-      <c r="D108" s="223"/>
-      <c r="E108" s="216"/>
-      <c r="F108" s="216"/>
-      <c r="G108" s="216"/>
+      <c r="B108" s="237"/>
+      <c r="C108" s="238"/>
+      <c r="D108" s="238"/>
+      <c r="E108" s="236"/>
+      <c r="F108" s="236"/>
+      <c r="G108" s="236"/>
       <c r="H108" s="139"/>
       <c r="I108" s="140"/>
       <c r="J108" s="140"/>
@@ -12574,15 +12586,15 @@
       <c r="Z112" s="17"/>
     </row>
     <row r="113" spans="1:26" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A113" s="215" t="s">
+      <c r="A113" s="235" t="s">
         <v>165</v>
       </c>
-      <c r="B113" s="217"/>
-      <c r="C113" s="223"/>
-      <c r="D113" s="223"/>
-      <c r="E113" s="216"/>
-      <c r="F113" s="216"/>
-      <c r="G113" s="216"/>
+      <c r="B113" s="237"/>
+      <c r="C113" s="238"/>
+      <c r="D113" s="238"/>
+      <c r="E113" s="236"/>
+      <c r="F113" s="236"/>
+      <c r="G113" s="236"/>
       <c r="H113" s="139"/>
       <c r="I113" s="140"/>
       <c r="J113" s="140"/>
@@ -16545,6 +16557,11 @@
   </sheetData>
   <autoFilter ref="B1:B473" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="15">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A39:C39"/>
     <mergeCell ref="R6:U17"/>
     <mergeCell ref="A70:G70"/>
     <mergeCell ref="A108:G108"/>
@@ -16555,11 +16572,6 @@
     <mergeCell ref="A97:G97"/>
     <mergeCell ref="A99:G99"/>
     <mergeCell ref="A103:G103"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="25" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
auto commit @26.11.2020: 15:13:39,33
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
+++ b/Bachelorarbeit/ICS and Test Docu_HW edit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6CFA71-C672-471D-9BFF-54A332604510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C9CB6D-93B3-475F-873C-8301BAD0E727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Statement" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="594">
   <si>
     <t>Im Rahmen von [BSI TR-03148 -P] muss ein Implementation Conformance Statement ausgefüllt werden. Im folgenden finden Sie eine Vorlage für das ICS. Das Originaldokument ist auf Englisch, weswegen hier die englischen Formulierungen übernommen wurden, da keine offizielle Übersetzung des Dokuments existiert. Die Eintragungen können aber auf deutsch oder englisch gemacht werden. Die hier eingetragenen Beispieldaten sind durch Echtdaten zu ersetzen. Alternativ oder ergänzend zu dem ICS in dieser Tabelle kann auch das ICS aus [BSI TR-03148-P] als Vorlage genutzt werden.</t>
   </si>
@@ -4884,9 +4884,6 @@
     </r>
   </si>
   <si>
-    <t>can be installed. Not in standard installation</t>
-  </si>
-  <si>
     <t>TR.G.5</t>
   </si>
   <si>
@@ -4918,9 +4915,6 @@
       </rPr>
       <t xml:space="preserve"> support forwarding of DANE packets according to [IETF RFC 6698].</t>
     </r>
-  </si>
-  <si>
-    <t>can be installed? Danish?</t>
   </si>
   <si>
     <t>Module H - Dynamic Host Configuration Protocol (DHCP)</t>
@@ -5761,6 +5755,19 @@
   </si>
   <si>
     <t>from factory to initialized state the user only needs to set a password ssh and the luci web-interface. No additional functionality is activated when setting a password. OpenWrt can be fully used even without a password. This is not recommended.</t>
+  </si>
+  <si>
+    <t>hping3 / nmap 7.90</t>
+  </si>
+  <si>
+    <t>https://openwrt.org/docs/guide-user/firewall/firewall_configuration</t>
+  </si>
+  <si>
+    <t>https://openwrt.org/docs/guide-user/firewall/firewall_configuration
+https://openwrt.org/docs/guide-user/firewall/start
+https://ipset.netfilter.org/iptables.man.html
+https://openwrt.org/docs/guide-user/firewall/netfilter_iptables/netfilter_openwrt
+Logging has to be enabled first.</t>
   </si>
 </sst>
 </file>
@@ -6432,7 +6439,7 @@
     <xf numFmtId="0" fontId="30" fillId="7" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6886,6 +6893,85 @@
     <xf numFmtId="0" fontId="25" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6898,80 +6984,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6983,22 +7006,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Excel Built-in 40% - Accent3" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -7395,29 +7403,29 @@
       <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.54296875" customWidth="1"/>
-    <col min="2" max="2" width="62.81640625" customWidth="1"/>
-    <col min="3" max="3" width="38.81640625" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="28.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="88.5" customHeight="1">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="157"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="157"/>
-      <c r="K2" s="157"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1"/>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
@@ -7427,10 +7435,10 @@
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A6" s="158" t="s">
+      <c r="A6" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="158"/>
+      <c r="B6" s="185"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7445,38 +7453,38 @@
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="159" t="s">
+      <c r="B7" s="186" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="159"/>
+      <c r="C7" s="186"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="187" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="160"/>
+      <c r="C8" s="187"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="160" t="s">
+      <c r="B9" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="160"/>
+      <c r="C9" s="187"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="161" t="s">
+      <c r="B10" s="181" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="161"/>
+      <c r="C10" s="181"/>
     </row>
     <row r="11" spans="1:11">
       <c r="B11" s="7"/>
@@ -7489,86 +7497,86 @@
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="64.5" customHeight="1">
-      <c r="A14" s="162" t="s">
+      <c r="A14" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="162"/>
+      <c r="B14" s="182"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="163" t="s">
+      <c r="B15" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="163"/>
-      <c r="D15" s="163"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="183"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="164"/>
-      <c r="D16" s="164"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="177"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="178" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="165"/>
-      <c r="E17" s="165"/>
-      <c r="F17" s="165"/>
-      <c r="G17" s="165"/>
-      <c r="H17" s="165"/>
+      <c r="C17" s="178"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="178"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="178"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="178" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="165"/>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
+      <c r="C18" s="178"/>
+      <c r="D18" s="178"/>
+      <c r="E18" s="178"/>
+      <c r="F18" s="178"/>
+      <c r="G18" s="178"/>
+      <c r="H18" s="178"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="166" t="s">
+      <c r="B19" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="166"/>
-      <c r="D19" s="166"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="167" t="s">
+      <c r="B20" s="179" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="179"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="164"/>
-      <c r="C21" s="164"/>
-      <c r="D21" s="164"/>
+      <c r="B21" s="177"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="177"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="14" t="s">
@@ -7576,70 +7584,70 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1">
-      <c r="A25" s="168" t="s">
+      <c r="A25" s="180" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="168"/>
+      <c r="B25" s="180"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="169" t="s">
+      <c r="B26" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="169"/>
-      <c r="D26" s="169"/>
+      <c r="C26" s="176"/>
+      <c r="D26" s="176"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="164" t="s">
+      <c r="B27" s="177" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="164"/>
-      <c r="D27" s="164"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="166" t="s">
+      <c r="B28" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
+      <c r="C28" s="175"/>
+      <c r="D28" s="175"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="166" t="s">
+      <c r="B29" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="166"/>
-      <c r="D29" s="166"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="175"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="166" t="s">
+      <c r="B30" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="166"/>
-      <c r="D30" s="166"/>
+      <c r="C30" s="175"/>
+      <c r="D30" s="175"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="166" t="s">
+      <c r="B31" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
+      <c r="C31" s="175"/>
+      <c r="D31" s="175"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="18"/>
@@ -7651,13 +7659,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="76.5" customHeight="1">
-      <c r="A34" s="170" t="s">
+      <c r="A34" s="172" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="170"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170"/>
-      <c r="E34" s="170"/>
+      <c r="B34" s="172"/>
+      <c r="C34" s="172"/>
+      <c r="D34" s="172"/>
+      <c r="E34" s="172"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="19" t="s">
@@ -8013,13 +8021,13 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="57" customHeight="1">
-      <c r="A58" s="170" t="s">
+      <c r="A58" s="172" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="170"/>
-      <c r="C58" s="170"/>
-      <c r="D58" s="170"/>
-      <c r="E58" s="170"/>
+      <c r="B58" s="172"/>
+      <c r="C58" s="172"/>
+      <c r="D58" s="172"/>
+      <c r="E58" s="172"/>
     </row>
     <row r="59" spans="1:11" ht="31.5" customHeight="1"/>
     <row r="60" spans="1:11" ht="44.25" customHeight="1">
@@ -8132,18 +8140,18 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A69" s="170" t="s">
+      <c r="A69" s="172" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="170"/>
-      <c r="C69" s="170"/>
-      <c r="D69" s="170"/>
-      <c r="E69" s="170"/>
+      <c r="B69" s="172"/>
+      <c r="C69" s="172"/>
+      <c r="D69" s="172"/>
+      <c r="E69" s="172"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="28"/>
     </row>
-    <row r="71" spans="1:5" ht="29">
+    <row r="71" spans="1:5" ht="30">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -8161,12 +8169,12 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="36" customHeight="1">
-      <c r="A74" s="170" t="s">
+      <c r="A74" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="170"/>
-      <c r="C74" s="170"/>
-      <c r="D74" s="170"/>
+      <c r="B74" s="172"/>
+      <c r="C74" s="172"/>
+      <c r="D74" s="172"/>
       <c r="E74" s="29"/>
     </row>
     <row r="76" spans="1:5">
@@ -8178,12 +8186,12 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1">
-      <c r="A79" s="170" t="s">
+      <c r="A79" s="172" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="170"/>
-      <c r="C79" s="170"/>
-      <c r="D79" s="170"/>
+      <c r="B79" s="172"/>
+      <c r="C79" s="172"/>
+      <c r="D79" s="172"/>
     </row>
     <row r="81" spans="1:5" ht="33.75" customHeight="1">
       <c r="A81" s="30" t="s">
@@ -8263,13 +8271,13 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A90" s="171" t="s">
+      <c r="A90" s="173" t="s">
         <v>86</v>
       </c>
-      <c r="B90" s="171"/>
-      <c r="C90" s="171"/>
-      <c r="D90" s="171"/>
-      <c r="E90" s="171"/>
+      <c r="B90" s="173"/>
+      <c r="C90" s="173"/>
+      <c r="D90" s="173"/>
+      <c r="E90" s="173"/>
     </row>
     <row r="92" spans="1:5" ht="35.25" customHeight="1">
       <c r="A92" s="15" t="s">
@@ -8299,7 +8307,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="29">
+    <row r="94" spans="1:5" ht="45">
       <c r="A94" s="21" t="s">
         <v>45</v>
       </c>
@@ -8369,13 +8377,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="30.65" customHeight="1">
-      <c r="A101" s="172" t="s">
+    <row r="101" spans="1:4" ht="30.6" customHeight="1">
+      <c r="A101" s="174" t="s">
         <v>95</v>
       </c>
-      <c r="B101" s="172"/>
-    </row>
-    <row r="103" spans="1:4" ht="29">
+      <c r="B101" s="174"/>
+    </row>
+    <row r="103" spans="1:4" ht="45">
       <c r="A103" s="3" t="s">
         <v>96</v>
       </c>
@@ -8389,12 +8397,12 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="70.5" customHeight="1">
-      <c r="A107" s="171" t="s">
+      <c r="A107" s="173" t="s">
         <v>99</v>
       </c>
-      <c r="B107" s="171"/>
-      <c r="C107" s="171"/>
-      <c r="D107" s="171"/>
+      <c r="B107" s="173"/>
+      <c r="C107" s="173"/>
+      <c r="D107" s="173"/>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
@@ -8510,12 +8518,12 @@
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" ht="56.25" customHeight="1">
-      <c r="A119" s="173" t="s">
+      <c r="A119" s="168" t="s">
         <v>103</v>
       </c>
-      <c r="B119" s="173"/>
-      <c r="C119" s="173"/>
-      <c r="D119" s="173"/>
+      <c r="B119" s="168"/>
+      <c r="C119" s="168"/>
+      <c r="D119" s="168"/>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="9" t="s">
@@ -8531,7 +8539,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="29">
+    <row r="121" spans="1:4" ht="45">
       <c r="A121" s="35" t="s">
         <v>67</v>
       </c>
@@ -8576,9 +8584,9 @@
       <c r="D126" s="24"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="174"/>
-      <c r="B127" s="174"/>
-      <c r="C127" s="174"/>
+      <c r="A127" s="171"/>
+      <c r="B127" s="171"/>
+      <c r="C127" s="171"/>
       <c r="D127" s="3"/>
     </row>
     <row r="128" spans="1:4">
@@ -8587,7 +8595,7 @@
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4" ht="20.5">
+    <row r="129" spans="1:4" ht="20.25">
       <c r="A129" s="38" t="s">
         <v>107</v>
       </c>
@@ -8596,14 +8604,14 @@
       <c r="D129" s="3"/>
     </row>
     <row r="130" spans="1:4" ht="113.25" customHeight="1">
-      <c r="A130" s="175" t="s">
+      <c r="A130" s="164" t="s">
         <v>108</v>
       </c>
-      <c r="B130" s="175"/>
-      <c r="C130" s="175"/>
-      <c r="D130" s="175"/>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="B130" s="164"/>
+      <c r="C130" s="164"/>
+      <c r="D130" s="164"/>
+    </row>
+    <row r="131" spans="1:4" ht="28.5">
       <c r="A131" s="9" t="s">
         <v>109</v>
       </c>
@@ -8615,7 +8623,7 @@
       </c>
       <c r="D131" s="3"/>
     </row>
-    <row r="132" spans="1:4" ht="29.15" customHeight="1">
+    <row r="132" spans="1:4" ht="29.1" customHeight="1">
       <c r="A132" s="25" t="s">
         <v>112</v>
       </c>
@@ -8639,7 +8647,7 @@
       </c>
       <c r="D133" s="3"/>
     </row>
-    <row r="134" spans="1:4" ht="63">
+    <row r="134" spans="1:4" ht="101.25">
       <c r="A134" s="25" t="s">
         <v>117</v>
       </c>
@@ -8651,7 +8659,7 @@
       </c>
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="1:4" ht="31.5">
+    <row r="135" spans="1:4" ht="56.25">
       <c r="A135" s="25" t="s">
         <v>119</v>
       </c>
@@ -8663,7 +8671,7 @@
       </c>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:4" ht="98">
+    <row r="136" spans="1:4" ht="105">
       <c r="A136" s="23" t="s">
         <v>121</v>
       </c>
@@ -8729,7 +8737,7 @@
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="1:4" ht="20.5">
+    <row r="142" spans="1:4" ht="20.25">
       <c r="A142" s="38" t="s">
         <v>125</v>
       </c>
@@ -8738,12 +8746,12 @@
       <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" ht="38.25" customHeight="1">
-      <c r="A143" s="175" t="s">
+      <c r="A143" s="164" t="s">
         <v>126</v>
       </c>
-      <c r="B143" s="175"/>
-      <c r="C143" s="175"/>
-      <c r="D143" s="175"/>
+      <c r="B143" s="164"/>
+      <c r="C143" s="164"/>
+      <c r="D143" s="164"/>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="9" t="s">
@@ -8792,10 +8800,10 @@
       <c r="D147" s="3"/>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="176" t="s">
+      <c r="A148" s="161" t="s">
         <v>134</v>
       </c>
-      <c r="B148" s="176"/>
+      <c r="B148" s="161"/>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
     </row>
@@ -8806,12 +8814,12 @@
       <c r="D149" s="3"/>
     </row>
     <row r="150" spans="1:4" ht="45.75" customHeight="1">
-      <c r="A150" s="175" t="s">
+      <c r="A150" s="164" t="s">
         <v>135</v>
       </c>
-      <c r="B150" s="175"/>
-      <c r="C150" s="175"/>
-      <c r="D150" s="175"/>
+      <c r="B150" s="164"/>
+      <c r="C150" s="164"/>
+      <c r="D150" s="164"/>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="9" t="s">
@@ -8858,14 +8866,14 @@
       <c r="D156" s="3"/>
     </row>
     <row r="157" spans="1:4" ht="49.5" customHeight="1">
-      <c r="A157" s="173" t="s">
+      <c r="A157" s="168" t="s">
         <v>137</v>
       </c>
-      <c r="B157" s="173"/>
-      <c r="C157" s="173"/>
-      <c r="D157" s="173"/>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="B157" s="168"/>
+      <c r="C157" s="168"/>
+      <c r="D157" s="168"/>
+    </row>
+    <row r="158" spans="1:4" ht="28.5">
       <c r="A158" s="9" t="s">
         <v>127</v>
       </c>
@@ -8934,10 +8942,10 @@
       <c r="D164" s="3"/>
     </row>
     <row r="165" spans="1:4" ht="39" customHeight="1">
-      <c r="A165" s="177" t="s">
+      <c r="A165" s="160" t="s">
         <v>141</v>
       </c>
-      <c r="B165" s="177"/>
+      <c r="B165" s="160"/>
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
     </row>
@@ -8951,7 +8959,7 @@
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
     </row>
-    <row r="167" spans="1:4" ht="28">
+    <row r="167" spans="1:4" ht="30">
       <c r="A167" s="23" t="s">
         <v>143</v>
       </c>
@@ -8982,10 +8990,10 @@
       <c r="D169" s="3"/>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="176" t="s">
+      <c r="A170" s="161" t="s">
         <v>147</v>
       </c>
-      <c r="B170" s="176"/>
+      <c r="B170" s="161"/>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
     </row>
@@ -8996,22 +9004,22 @@
       <c r="D171" s="3"/>
     </row>
     <row r="172" spans="1:4" ht="53.25" customHeight="1">
-      <c r="A172" s="175" t="s">
+      <c r="A172" s="164" t="s">
         <v>148</v>
       </c>
-      <c r="B172" s="175"/>
-      <c r="C172" s="175"/>
-      <c r="D172" s="175"/>
+      <c r="B172" s="164"/>
+      <c r="C172" s="164"/>
+      <c r="D172" s="164"/>
     </row>
     <row r="173" spans="1:4" ht="24" customHeight="1">
       <c r="A173" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="B173" s="178" t="s">
+      <c r="B173" s="170" t="s">
         <v>150</v>
       </c>
-      <c r="C173" s="178"/>
-      <c r="D173" s="178"/>
+      <c r="C173" s="170"/>
+      <c r="D173" s="170"/>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="3"/>
@@ -9020,12 +9028,12 @@
       <c r="D174" s="3"/>
     </row>
     <row r="175" spans="1:4" ht="75.75" customHeight="1">
-      <c r="A175" s="179" t="s">
+      <c r="A175" s="167" t="s">
         <v>151</v>
       </c>
-      <c r="B175" s="179"/>
-      <c r="C175" s="179"/>
-      <c r="D175" s="179"/>
+      <c r="B175" s="167"/>
+      <c r="C175" s="167"/>
+      <c r="D175" s="167"/>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="3"/>
@@ -9044,7 +9052,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="42">
+    <row r="178" spans="1:7" ht="45">
       <c r="A178" s="23" t="s">
         <v>154</v>
       </c>
@@ -9056,7 +9064,7 @@
       </c>
       <c r="G178" s="45"/>
     </row>
-    <row r="179" spans="1:7" ht="28">
+    <row r="179" spans="1:7" ht="30">
       <c r="A179" s="23" t="s">
         <v>157</v>
       </c>
@@ -9080,20 +9088,20 @@
       </c>
     </row>
     <row r="181" spans="1:7">
-      <c r="A181" s="176"/>
-      <c r="B181" s="176"/>
+      <c r="A181" s="161"/>
+      <c r="B181" s="161"/>
     </row>
     <row r="182" spans="1:7">
       <c r="A182" s="46"/>
       <c r="B182" s="46"/>
     </row>
     <row r="183" spans="1:7" ht="63" customHeight="1">
-      <c r="A183" s="173" t="s">
+      <c r="A183" s="168" t="s">
         <v>160</v>
       </c>
-      <c r="B183" s="173"/>
-      <c r="C183" s="173"/>
-      <c r="D183" s="173"/>
+      <c r="B183" s="168"/>
+      <c r="C183" s="168"/>
+      <c r="D183" s="168"/>
     </row>
     <row r="184" spans="1:7" ht="26.25" customHeight="1">
       <c r="A184" s="9" t="s">
@@ -9134,20 +9142,20 @@
       <c r="D187" s="24"/>
     </row>
     <row r="188" spans="1:7">
-      <c r="A188" s="180"/>
-      <c r="B188" s="180"/>
+      <c r="A188" s="169"/>
+      <c r="B188" s="169"/>
     </row>
     <row r="189" spans="1:7">
       <c r="A189" s="47"/>
       <c r="B189" s="47"/>
     </row>
     <row r="190" spans="1:7" ht="54.75" customHeight="1">
-      <c r="A190" s="175" t="s">
+      <c r="A190" s="164" t="s">
         <v>165</v>
       </c>
-      <c r="B190" s="175"/>
-      <c r="C190" s="175"/>
-      <c r="D190" s="175"/>
+      <c r="B190" s="164"/>
+      <c r="C190" s="164"/>
+      <c r="D190" s="164"/>
       <c r="F190" t="s">
         <v>166</v>
       </c>
@@ -9160,7 +9168,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="28">
+    <row r="193" spans="1:6" ht="30">
       <c r="A193" s="23" t="s">
         <v>168</v>
       </c>
@@ -9186,7 +9194,7 @@
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
     </row>
-    <row r="198" spans="1:6" ht="20.5">
+    <row r="198" spans="1:6" ht="20.25">
       <c r="A198" s="48" t="s">
         <v>170</v>
       </c>
@@ -9194,12 +9202,12 @@
       <c r="D198" s="3"/>
     </row>
     <row r="199" spans="1:6" ht="58.5" customHeight="1">
-      <c r="A199" s="181" t="s">
+      <c r="A199" s="165" t="s">
         <v>171</v>
       </c>
-      <c r="B199" s="181"/>
-      <c r="C199" s="181"/>
-      <c r="D199" s="181"/>
+      <c r="B199" s="165"/>
+      <c r="C199" s="165"/>
+      <c r="D199" s="165"/>
     </row>
     <row r="200" spans="1:6">
       <c r="A200" s="49" t="s">
@@ -9248,8 +9256,8 @@
       <c r="D204" s="3"/>
     </row>
     <row r="205" spans="1:6">
-      <c r="A205" s="176"/>
-      <c r="B205" s="176"/>
+      <c r="A205" s="161"/>
+      <c r="B205" s="161"/>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
@@ -9260,12 +9268,12 @@
       <c r="D206" s="3"/>
     </row>
     <row r="207" spans="1:6" ht="54.75" customHeight="1">
-      <c r="A207" s="182" t="s">
+      <c r="A207" s="159" t="s">
         <v>177</v>
       </c>
-      <c r="B207" s="182"/>
-      <c r="C207" s="182"/>
-      <c r="D207" s="182"/>
+      <c r="B207" s="159"/>
+      <c r="C207" s="159"/>
+      <c r="D207" s="159"/>
       <c r="F207" t="s">
         <v>178</v>
       </c>
@@ -9293,7 +9301,7 @@
       </c>
       <c r="B210" s="24"/>
     </row>
-    <row r="211" spans="1:4" ht="28">
+    <row r="211" spans="1:4" ht="30">
       <c r="A211" s="23" t="s">
         <v>182</v>
       </c>
@@ -9308,19 +9316,19 @@
       <c r="B213" s="24"/>
     </row>
     <row r="214" spans="1:4">
-      <c r="A214" s="176"/>
-      <c r="B214" s="176"/>
+      <c r="A214" s="161"/>
+      <c r="B214" s="161"/>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="51"/>
     </row>
     <row r="216" spans="1:4" ht="33" customHeight="1">
-      <c r="A216" s="183" t="s">
+      <c r="A216" s="166" t="s">
         <v>183</v>
       </c>
-      <c r="B216" s="183"/>
-      <c r="C216" s="183"/>
-      <c r="D216" s="183"/>
+      <c r="B216" s="166"/>
+      <c r="C216" s="166"/>
+      <c r="D216" s="166"/>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="9" t="s">
@@ -9369,14 +9377,14 @@
       <c r="B222" s="46"/>
     </row>
     <row r="223" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A223" s="175" t="s">
+      <c r="A223" s="164" t="s">
         <v>186</v>
       </c>
-      <c r="B223" s="175"/>
-      <c r="C223" s="175"/>
-      <c r="D223" s="175"/>
-    </row>
-    <row r="224" spans="1:4" ht="43.5">
+      <c r="B223" s="164"/>
+      <c r="C223" s="164"/>
+      <c r="D223" s="164"/>
+    </row>
+    <row r="224" spans="1:4" ht="45">
       <c r="A224" s="52" t="s">
         <v>187</v>
       </c>
@@ -9385,12 +9393,12 @@
       </c>
     </row>
     <row r="226" spans="1:5" ht="36" customHeight="1">
-      <c r="A226" s="182" t="s">
+      <c r="A226" s="159" t="s">
         <v>189</v>
       </c>
-      <c r="B226" s="182"/>
-      <c r="C226" s="182"/>
-      <c r="D226" s="182"/>
+      <c r="B226" s="159"/>
+      <c r="C226" s="159"/>
+      <c r="D226" s="159"/>
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="52" t="s">
@@ -9406,20 +9414,20 @@
       <c r="C228" s="3"/>
       <c r="D228" s="3"/>
     </row>
-    <row r="229" spans="1:5" ht="20">
+    <row r="229" spans="1:5" ht="20.25">
       <c r="A229" s="53" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="230" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A230" s="182" t="s">
+      <c r="A230" s="159" t="s">
         <v>192</v>
       </c>
-      <c r="B230" s="182"/>
-      <c r="C230" s="182"/>
-      <c r="D230" s="182"/>
-    </row>
-    <row r="231" spans="1:5" ht="87">
+      <c r="B230" s="159"/>
+      <c r="C230" s="159"/>
+      <c r="D230" s="159"/>
+    </row>
+    <row r="231" spans="1:5" ht="105">
       <c r="A231" s="52" t="s">
         <v>187</v>
       </c>
@@ -9427,18 +9435,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="20">
+    <row r="233" spans="1:5" ht="20.25">
       <c r="A233" s="53" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="234" spans="1:5" ht="49.5" customHeight="1">
-      <c r="A234" s="182" t="s">
+      <c r="A234" s="159" t="s">
         <v>195</v>
       </c>
-      <c r="B234" s="182"/>
-      <c r="C234" s="182"/>
-      <c r="D234" s="182"/>
+      <c r="B234" s="159"/>
+      <c r="C234" s="159"/>
+      <c r="D234" s="159"/>
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="52" t="s">
@@ -9465,12 +9473,12 @@
       </c>
     </row>
     <row r="239" spans="1:5" ht="33" customHeight="1">
-      <c r="A239" s="182" t="s">
+      <c r="A239" s="159" t="s">
         <v>200</v>
       </c>
-      <c r="B239" s="182"/>
-      <c r="C239" s="182"/>
-      <c r="D239" s="182"/>
+      <c r="B239" s="159"/>
+      <c r="C239" s="159"/>
+      <c r="D239" s="159"/>
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="52" t="s">
@@ -9484,10 +9492,10 @@
       </c>
     </row>
     <row r="241" spans="1:5" ht="144.75" customHeight="1">
-      <c r="D241" s="184" t="s">
+      <c r="D241" s="163" t="s">
         <v>203</v>
       </c>
-      <c r="E241" s="184"/>
+      <c r="E241" s="163"/>
     </row>
     <row r="242" spans="1:5">
       <c r="D242" t="s">
@@ -9503,12 +9511,12 @@
       </c>
     </row>
     <row r="245" spans="1:5" ht="41.25" customHeight="1">
-      <c r="A245" s="182" t="s">
+      <c r="A245" s="159" t="s">
         <v>207</v>
       </c>
-      <c r="B245" s="182"/>
-      <c r="C245" s="182"/>
-      <c r="D245" s="182"/>
+      <c r="B245" s="159"/>
+      <c r="C245" s="159"/>
+      <c r="D245" s="159"/>
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="52" t="s">
@@ -9519,12 +9527,12 @@
       </c>
     </row>
     <row r="248" spans="1:5" ht="38.25" customHeight="1">
-      <c r="A248" s="175" t="s">
+      <c r="A248" s="164" t="s">
         <v>209</v>
       </c>
-      <c r="B248" s="175"/>
-      <c r="C248" s="175"/>
-      <c r="D248" s="175"/>
+      <c r="B248" s="164"/>
+      <c r="C248" s="164"/>
+      <c r="D248" s="164"/>
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="52" t="s">
@@ -9537,18 +9545,18 @@
         <v>211</v>
       </c>
     </row>
-    <row r="251" spans="1:5" ht="20">
+    <row r="251" spans="1:5" ht="20.25">
       <c r="A251" s="53" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="45" customHeight="1">
-      <c r="A252" s="182" t="s">
+      <c r="A252" s="159" t="s">
         <v>213</v>
       </c>
-      <c r="B252" s="182"/>
-      <c r="C252" s="182"/>
-      <c r="D252" s="182"/>
+      <c r="B252" s="159"/>
+      <c r="C252" s="159"/>
+      <c r="D252" s="159"/>
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="52" t="s">
@@ -9575,18 +9583,18 @@
         <v>216</v>
       </c>
     </row>
-    <row r="256" spans="1:5" ht="20">
+    <row r="256" spans="1:5" ht="20.25">
       <c r="A256" s="53" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="42" customHeight="1">
-      <c r="A257" s="182" t="s">
+      <c r="A257" s="159" t="s">
         <v>218</v>
       </c>
-      <c r="B257" s="182"/>
-      <c r="C257" s="182"/>
-      <c r="D257" s="182"/>
+      <c r="B257" s="159"/>
+      <c r="C257" s="159"/>
+      <c r="D257" s="159"/>
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="9" t="s">
@@ -9596,7 +9604,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="260" spans="1:5" ht="70">
+    <row r="260" spans="1:5" ht="75">
       <c r="A260" s="23" t="s">
         <v>220</v>
       </c>
@@ -9607,7 +9615,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="56">
+    <row r="261" spans="1:5" ht="60">
       <c r="A261" s="23" t="s">
         <v>223</v>
       </c>
@@ -9618,7 +9626,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="154">
+    <row r="262" spans="1:5" ht="165">
       <c r="A262" s="23" t="s">
         <v>225</v>
       </c>
@@ -9636,42 +9644,42 @@
       <c r="B263" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="C263" s="185" t="s">
+      <c r="C263" s="162" t="s">
         <v>229</v>
       </c>
-      <c r="D263" s="185"/>
-      <c r="E263" s="185"/>
+      <c r="D263" s="162"/>
+      <c r="E263" s="162"/>
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="46"/>
       <c r="B264" s="46"/>
     </row>
-    <row r="265" spans="1:5" ht="20">
+    <row r="265" spans="1:5" ht="20.25">
       <c r="A265" s="53" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="266" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A266" s="182" t="s">
+      <c r="A266" s="159" t="s">
         <v>231</v>
       </c>
-      <c r="B266" s="182"/>
+      <c r="B266" s="159"/>
     </row>
     <row r="267" spans="1:5">
       <c r="A267" s="55"/>
     </row>
-    <row r="268" spans="1:5" ht="20">
+    <row r="268" spans="1:5" ht="20.25">
       <c r="A268" s="53" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="269" spans="1:5" ht="35.25" customHeight="1">
-      <c r="A269" s="182" t="s">
+      <c r="A269" s="159" t="s">
         <v>233</v>
       </c>
-      <c r="B269" s="182"/>
-      <c r="C269" s="182"/>
-      <c r="D269" s="182"/>
+      <c r="B269" s="159"/>
+      <c r="C269" s="159"/>
+      <c r="D269" s="159"/>
     </row>
     <row r="270" spans="1:5">
       <c r="A270" s="52" t="s">
@@ -9682,12 +9690,12 @@
       </c>
     </row>
     <row r="272" spans="1:5" ht="42.75" customHeight="1">
-      <c r="A272" s="182" t="s">
+      <c r="A272" s="159" t="s">
         <v>235</v>
       </c>
-      <c r="B272" s="182"/>
-      <c r="C272" s="182"/>
-      <c r="D272" s="182"/>
+      <c r="B272" s="159"/>
+      <c r="C272" s="159"/>
+      <c r="D272" s="159"/>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" s="52" t="s">
@@ -9699,16 +9707,16 @@
     </row>
     <row r="274" spans="1:4" ht="25.5" customHeight="1"/>
     <row r="275" spans="1:4" ht="49.5" customHeight="1">
-      <c r="A275" s="182" t="s">
+      <c r="A275" s="159" t="s">
         <v>236</v>
       </c>
-      <c r="B275" s="182"/>
+      <c r="B275" s="159"/>
     </row>
     <row r="276" spans="1:4" ht="59.25" customHeight="1">
-      <c r="A276" s="182" t="s">
+      <c r="A276" s="159" t="s">
         <v>237</v>
       </c>
-      <c r="B276" s="182"/>
+      <c r="B276" s="159"/>
     </row>
     <row r="277" spans="1:4">
       <c r="A277" s="52" t="s">
@@ -9719,12 +9727,12 @@
       </c>
     </row>
     <row r="279" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A279" s="177" t="s">
+      <c r="A279" s="160" t="s">
         <v>239</v>
       </c>
-      <c r="B279" s="177"/>
-      <c r="C279" s="177"/>
-      <c r="D279" s="177"/>
+      <c r="B279" s="160"/>
+      <c r="C279" s="160"/>
+      <c r="D279" s="160"/>
     </row>
     <row r="280" spans="1:4">
       <c r="A280" s="9" t="s">
@@ -9757,14 +9765,14 @@
       <c r="D282" s="26"/>
     </row>
     <row r="283" spans="1:4">
-      <c r="A283" s="176"/>
-      <c r="B283" s="176"/>
+      <c r="A283" s="161"/>
+      <c r="B283" s="161"/>
     </row>
     <row r="284" spans="1:4">
       <c r="A284" s="46"/>
       <c r="B284" s="46"/>
     </row>
-    <row r="285" spans="1:4" ht="20">
+    <row r="285" spans="1:4" ht="20.25">
       <c r="A285" s="53" t="s">
         <v>243</v>
       </c>
@@ -9774,21 +9782,21 @@
         <v>231</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="20">
+    <row r="287" spans="1:4" ht="20.25">
       <c r="A287" s="57"/>
     </row>
-    <row r="288" spans="1:4" ht="20">
+    <row r="288" spans="1:4" ht="20.25">
       <c r="A288" s="53" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="39" customHeight="1">
-      <c r="A289" s="182" t="s">
+      <c r="A289" s="159" t="s">
         <v>245</v>
       </c>
-      <c r="B289" s="182"/>
-      <c r="C289" s="182"/>
-      <c r="D289" s="182"/>
+      <c r="B289" s="159"/>
+      <c r="C289" s="159"/>
+      <c r="D289" s="159"/>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="52" t="s">
@@ -9799,12 +9807,12 @@
       </c>
     </row>
     <row r="292" spans="1:4" ht="44.25" customHeight="1">
-      <c r="A292" s="177" t="s">
+      <c r="A292" s="160" t="s">
         <v>247</v>
       </c>
-      <c r="B292" s="177"/>
-      <c r="C292" s="177"/>
-      <c r="D292" s="177"/>
+      <c r="B292" s="160"/>
+      <c r="C292" s="160"/>
+      <c r="D292" s="160"/>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="58" t="s">
@@ -9846,76 +9854,76 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A69:E69"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A150:D150"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="A172:D172"/>
+    <mergeCell ref="B173:D173"/>
+    <mergeCell ref="A175:D175"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="A183:D183"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A190:D190"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A205:B205"/>
+    <mergeCell ref="A207:D207"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A216:D216"/>
+    <mergeCell ref="A223:D223"/>
+    <mergeCell ref="A226:D226"/>
+    <mergeCell ref="A230:D230"/>
+    <mergeCell ref="A234:D234"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="D241:E241"/>
+    <mergeCell ref="A245:D245"/>
+    <mergeCell ref="A248:D248"/>
+    <mergeCell ref="A252:D252"/>
+    <mergeCell ref="A257:D257"/>
+    <mergeCell ref="C263:E263"/>
+    <mergeCell ref="A266:B266"/>
+    <mergeCell ref="A269:D269"/>
+    <mergeCell ref="A272:D272"/>
+    <mergeCell ref="A275:B275"/>
     <mergeCell ref="A276:B276"/>
     <mergeCell ref="A279:D279"/>
     <mergeCell ref="A283:B283"/>
     <mergeCell ref="A289:D289"/>
     <mergeCell ref="A292:D292"/>
-    <mergeCell ref="C263:E263"/>
-    <mergeCell ref="A266:B266"/>
-    <mergeCell ref="A269:D269"/>
-    <mergeCell ref="A272:D272"/>
-    <mergeCell ref="A275:B275"/>
-    <mergeCell ref="D241:E241"/>
-    <mergeCell ref="A245:D245"/>
-    <mergeCell ref="A248:D248"/>
-    <mergeCell ref="A252:D252"/>
-    <mergeCell ref="A257:D257"/>
-    <mergeCell ref="A223:D223"/>
-    <mergeCell ref="A226:D226"/>
-    <mergeCell ref="A230:D230"/>
-    <mergeCell ref="A234:D234"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A205:B205"/>
-    <mergeCell ref="A207:D207"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A216:D216"/>
-    <mergeCell ref="A175:D175"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="A183:D183"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A190:D190"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="A172:D172"/>
-    <mergeCell ref="B173:D173"/>
-    <mergeCell ref="A127:C127"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A150:D150"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A69:E69"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C132" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -9933,26 +9941,26 @@
   <dimension ref="A1:AMJ117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80:C82"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="61" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" style="61" customWidth="1"/>
-    <col min="3" max="3" width="142.1796875" style="62" customWidth="1"/>
-    <col min="4" max="6" width="5.7265625" style="63" customWidth="1"/>
-    <col min="7" max="11" width="8.7265625" style="63" customWidth="1"/>
-    <col min="12" max="12" width="78.7265625" style="61" customWidth="1"/>
-    <col min="13" max="13" width="26.7265625" style="61" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="61" customWidth="1"/>
+    <col min="3" max="3" width="142.140625" style="62" customWidth="1"/>
+    <col min="4" max="6" width="5.7109375" style="63" customWidth="1"/>
+    <col min="7" max="11" width="8.7109375" style="63" customWidth="1"/>
+    <col min="12" max="12" width="78.7109375" style="61" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="61" customWidth="1"/>
     <col min="14" max="14" width="29" style="61" customWidth="1"/>
-    <col min="15" max="15" width="73.7265625" style="61" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" style="61" customWidth="1"/>
-    <col min="17" max="1024" width="11.453125" style="61"/>
+    <col min="15" max="15" width="73.7109375" style="61" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="61" customWidth="1"/>
+    <col min="17" max="1024" width="11.42578125" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="67" customFormat="1" ht="51.65" customHeight="1" thickBot="1">
+    <row r="1" spans="1:20" s="67" customFormat="1" ht="51.6" customHeight="1" thickBot="1">
       <c r="A1" s="64" t="s">
         <v>250</v>
       </c>
@@ -9962,11 +9970,11 @@
       <c r="C1" s="64" t="s">
         <v>252</v>
       </c>
-      <c r="D1" s="186" t="s">
+      <c r="D1" s="191" t="s">
         <v>253</v>
       </c>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
       <c r="G1" s="65"/>
       <c r="H1" s="65"/>
       <c r="I1" s="65"/>
@@ -9980,7 +9988,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="2" spans="1:20" s="67" customFormat="1" ht="29.25" thickBot="1">
       <c r="A2" s="66"/>
       <c r="B2" s="66"/>
       <c r="C2" s="68"/>
@@ -10020,9 +10028,9 @@
       <c r="O2" s="69" t="s">
         <v>265</v>
       </c>
-      <c r="P2" s="192"/>
-    </row>
-    <row r="3" spans="1:20" s="67" customFormat="1" ht="15" thickBot="1">
+      <c r="P2" s="157"/>
+    </row>
+    <row r="3" spans="1:20" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="66"/>
       <c r="B3" s="66"/>
       <c r="C3" s="68"/>
@@ -10050,15 +10058,15 @@
       <c r="O3" s="76"/>
       <c r="P3" s="66"/>
     </row>
-    <row r="4" spans="1:20" s="67" customFormat="1" ht="17.149999999999999" customHeight="1" thickBot="1">
-      <c r="A4" s="187" t="s">
+    <row r="4" spans="1:20" s="67" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A4" s="192" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="187"/>
-      <c r="C4" s="187"/>
-      <c r="D4" s="187"/>
-      <c r="E4" s="187"/>
-      <c r="F4" s="187"/>
+      <c r="B4" s="192"/>
+      <c r="C4" s="192"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
+      <c r="F4" s="192"/>
       <c r="G4" s="77"/>
       <c r="H4" s="78"/>
       <c r="I4" s="78"/>
@@ -10150,12 +10158,12 @@
       <c r="P6" s="87" t="s">
         <v>278</v>
       </c>
-      <c r="Q6" s="188" t="s">
+      <c r="Q6" s="193" t="s">
         <v>284</v>
       </c>
-      <c r="R6" s="188"/>
-      <c r="S6" s="188"/>
-      <c r="T6" s="188"/>
+      <c r="R6" s="193"/>
+      <c r="S6" s="193"/>
+      <c r="T6" s="193"/>
     </row>
     <row r="7" spans="1:20" s="67" customFormat="1" ht="68.25" customHeight="1" thickBot="1">
       <c r="A7" s="87" t="s">
@@ -10192,10 +10200,10 @@
       <c r="P7" s="87" t="s">
         <v>285</v>
       </c>
-      <c r="Q7" s="188"/>
-      <c r="R7" s="188"/>
-      <c r="S7" s="188"/>
-      <c r="T7" s="188"/>
+      <c r="Q7" s="193"/>
+      <c r="R7" s="193"/>
+      <c r="S7" s="193"/>
+      <c r="T7" s="193"/>
     </row>
     <row r="8" spans="1:20" s="67" customFormat="1" ht="87.75" customHeight="1" thickBot="1">
       <c r="A8" s="87" t="s">
@@ -10228,10 +10236,10 @@
       <c r="P8" s="87" t="s">
         <v>290</v>
       </c>
-      <c r="Q8" s="188"/>
-      <c r="R8" s="188"/>
-      <c r="S8" s="188"/>
-      <c r="T8" s="188"/>
+      <c r="Q8" s="193"/>
+      <c r="R8" s="193"/>
+      <c r="S8" s="193"/>
+      <c r="T8" s="193"/>
     </row>
     <row r="9" spans="1:20" s="67" customFormat="1" ht="80.25" customHeight="1" thickBot="1">
       <c r="A9" s="87" t="s">
@@ -10266,12 +10274,12 @@
       <c r="P9" s="87" t="s">
         <v>292</v>
       </c>
-      <c r="Q9" s="188"/>
-      <c r="R9" s="188"/>
-      <c r="S9" s="188"/>
-      <c r="T9" s="188"/>
-    </row>
-    <row r="10" spans="1:20" s="67" customFormat="1" ht="28.5" thickBot="1">
+      <c r="Q9" s="193"/>
+      <c r="R9" s="193"/>
+      <c r="S9" s="193"/>
+      <c r="T9" s="193"/>
+    </row>
+    <row r="10" spans="1:20" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A10" s="87" t="s">
         <v>296</v>
       </c>
@@ -10306,10 +10314,10 @@
       <c r="P10" s="87" t="s">
         <v>296</v>
       </c>
-      <c r="Q10" s="188"/>
-      <c r="R10" s="188"/>
-      <c r="S10" s="188"/>
-      <c r="T10" s="188"/>
+      <c r="Q10" s="193"/>
+      <c r="R10" s="193"/>
+      <c r="S10" s="193"/>
+      <c r="T10" s="193"/>
     </row>
     <row r="11" spans="1:20" s="67" customFormat="1" ht="62.25" customHeight="1" thickBot="1">
       <c r="A11" s="87" t="s">
@@ -10346,10 +10354,10 @@
       <c r="P11" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="Q11" s="188"/>
-      <c r="R11" s="188"/>
-      <c r="S11" s="188"/>
-      <c r="T11" s="188"/>
+      <c r="Q11" s="193"/>
+      <c r="R11" s="193"/>
+      <c r="S11" s="193"/>
+      <c r="T11" s="193"/>
     </row>
     <row r="12" spans="1:20" s="67" customFormat="1" ht="103.5" customHeight="1" thickBot="1">
       <c r="A12" s="87" t="s">
@@ -10388,10 +10396,10 @@
       <c r="P12" s="87" t="s">
         <v>304</v>
       </c>
-      <c r="Q12" s="188"/>
-      <c r="R12" s="188"/>
-      <c r="S12" s="188"/>
-      <c r="T12" s="188"/>
+      <c r="Q12" s="193"/>
+      <c r="R12" s="193"/>
+      <c r="S12" s="193"/>
+      <c r="T12" s="193"/>
     </row>
     <row r="13" spans="1:20" s="67" customFormat="1" ht="129" customHeight="1" thickBot="1">
       <c r="A13" s="87" t="s">
@@ -10436,12 +10444,12 @@
       <c r="P13" s="87" t="s">
         <v>309</v>
       </c>
-      <c r="Q13" s="188"/>
-      <c r="R13" s="188"/>
-      <c r="S13" s="188"/>
-      <c r="T13" s="188"/>
-    </row>
-    <row r="14" spans="1:20" s="67" customFormat="1" ht="23.5" customHeight="1" thickBot="1">
+      <c r="Q13" s="193"/>
+      <c r="R13" s="193"/>
+      <c r="S13" s="193"/>
+      <c r="T13" s="193"/>
+    </row>
+    <row r="14" spans="1:20" s="67" customFormat="1" ht="23.45" customHeight="1" thickBot="1">
       <c r="A14" s="87" t="s">
         <v>314</v>
       </c>
@@ -10476,12 +10484,12 @@
       <c r="P14" s="87" t="s">
         <v>314</v>
       </c>
-      <c r="Q14" s="188"/>
-      <c r="R14" s="188"/>
-      <c r="S14" s="188"/>
-      <c r="T14" s="188"/>
-    </row>
-    <row r="15" spans="1:20" s="67" customFormat="1" ht="28.5" thickBot="1">
+      <c r="Q14" s="193"/>
+      <c r="R14" s="193"/>
+      <c r="S14" s="193"/>
+      <c r="T14" s="193"/>
+    </row>
+    <row r="15" spans="1:20" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A15" s="87" t="s">
         <v>317</v>
       </c>
@@ -10510,10 +10518,10 @@
       <c r="P15" s="87" t="s">
         <v>317</v>
       </c>
-      <c r="Q15" s="188"/>
-      <c r="R15" s="188"/>
-      <c r="S15" s="188"/>
-      <c r="T15" s="188"/>
+      <c r="Q15" s="193"/>
+      <c r="R15" s="193"/>
+      <c r="S15" s="193"/>
+      <c r="T15" s="193"/>
     </row>
     <row r="16" spans="1:20" s="67" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1">
       <c r="A16" s="87" t="s">
@@ -10544,12 +10552,12 @@
       <c r="P16" s="87" t="s">
         <v>320</v>
       </c>
-      <c r="Q16" s="188"/>
-      <c r="R16" s="188"/>
-      <c r="S16" s="188"/>
-      <c r="T16" s="188"/>
-    </row>
-    <row r="17" spans="1:20" s="67" customFormat="1" ht="91.75" customHeight="1" thickBot="1">
+      <c r="Q16" s="193"/>
+      <c r="R16" s="193"/>
+      <c r="S16" s="193"/>
+      <c r="T16" s="193"/>
+    </row>
+    <row r="17" spans="1:20" s="67" customFormat="1" ht="91.7" customHeight="1" thickBot="1">
       <c r="A17" s="87" t="s">
         <v>323</v>
       </c>
@@ -10588,12 +10596,12 @@
       <c r="P17" s="87" t="s">
         <v>323</v>
       </c>
-      <c r="Q17" s="188"/>
-      <c r="R17" s="188"/>
-      <c r="S17" s="188"/>
-      <c r="T17" s="188"/>
-    </row>
-    <row r="18" spans="1:20" s="67" customFormat="1" ht="42.5" thickBot="1">
+      <c r="Q17" s="193"/>
+      <c r="R17" s="193"/>
+      <c r="S17" s="193"/>
+      <c r="T17" s="193"/>
+    </row>
+    <row r="18" spans="1:20" s="67" customFormat="1" ht="45.75" thickBot="1">
       <c r="A18" s="112" t="s">
         <v>328</v>
       </c>
@@ -10633,7 +10641,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="67" customFormat="1" ht="42.65" customHeight="1" thickBot="1">
+    <row r="19" spans="1:20" s="67" customFormat="1" ht="42.6" customHeight="1" thickBot="1">
       <c r="A19" s="112" t="s">
         <v>333</v>
       </c>
@@ -10669,7 +10677,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="67" customFormat="1" ht="37.4" customHeight="1" thickBot="1">
+    <row r="20" spans="1:20" s="67" customFormat="1" ht="37.35" customHeight="1" thickBot="1">
       <c r="A20" s="112" t="s">
         <v>337</v>
       </c>
@@ -10729,7 +10737,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="67" customFormat="1" ht="112.5" thickBot="1">
+    <row r="22" spans="1:20" s="67" customFormat="1" ht="120.75" thickBot="1">
       <c r="A22" s="87" t="s">
         <v>343</v>
       </c>
@@ -10765,7 +10773,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="67" customFormat="1" ht="70.5" thickBot="1">
+    <row r="23" spans="1:20" s="67" customFormat="1" ht="75.75" thickBot="1">
       <c r="A23" s="87" t="s">
         <v>346</v>
       </c>
@@ -10799,7 +10807,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="24" spans="1:20" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A24" s="87" t="s">
         <v>351</v>
       </c>
@@ -10831,7 +10839,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="25" spans="1:20" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A25" s="112" t="s">
         <v>354</v>
       </c>
@@ -10861,7 +10869,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="26" spans="1:20" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A26" s="87" t="s">
         <v>358</v>
       </c>
@@ -10892,14 +10900,14 @@
       </c>
     </row>
     <row r="27" spans="1:20" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A27" s="189" t="s">
+      <c r="A27" s="188" t="s">
         <v>360</v>
       </c>
-      <c r="B27" s="189"/>
-      <c r="C27" s="189"/>
-      <c r="D27" s="189"/>
-      <c r="E27" s="189"/>
-      <c r="F27" s="189"/>
+      <c r="B27" s="188"/>
+      <c r="C27" s="188"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
       <c r="G27" s="122"/>
       <c r="H27" s="123"/>
       <c r="I27" s="123"/>
@@ -10911,7 +10919,7 @@
       <c r="O27" s="125"/>
       <c r="P27" s="124"/>
     </row>
-    <row r="28" spans="1:20" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="28" spans="1:20" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A28" s="87" t="s">
         <v>361</v>
       </c>
@@ -10939,7 +10947,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="29" spans="1:20" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A29" s="87" t="s">
         <v>363</v>
       </c>
@@ -10967,7 +10975,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="30" spans="1:20" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A30" s="87" t="s">
         <v>365</v>
       </c>
@@ -10995,7 +11003,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="31" spans="1:20" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A31" s="87" t="s">
         <v>367</v>
       </c>
@@ -11023,7 +11031,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="32" spans="1:20" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A32" s="87" t="s">
         <v>369</v>
       </c>
@@ -11051,7 +11059,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="33" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A33" s="87" t="s">
         <v>370</v>
       </c>
@@ -11079,7 +11087,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="34" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A34" s="87" t="s">
         <v>372</v>
       </c>
@@ -11107,7 +11115,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="35" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A35" s="87" t="s">
         <v>374</v>
       </c>
@@ -11136,14 +11144,14 @@
       </c>
     </row>
     <row r="36" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A36" s="189" t="s">
+      <c r="A36" s="188" t="s">
         <v>376</v>
       </c>
-      <c r="B36" s="189"/>
-      <c r="C36" s="189"/>
-      <c r="D36" s="189"/>
-      <c r="E36" s="189"/>
-      <c r="F36" s="189"/>
+      <c r="B36" s="188"/>
+      <c r="C36" s="188"/>
+      <c r="D36" s="188"/>
+      <c r="E36" s="188"/>
+      <c r="F36" s="188"/>
       <c r="G36" s="122"/>
       <c r="H36" s="123"/>
       <c r="I36" s="123"/>
@@ -11180,7 +11188,7 @@
       <c r="J37" s="107"/>
       <c r="K37" s="107"/>
       <c r="L37" s="109" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="M37" s="107" t="s">
         <v>379</v>
@@ -11195,7 +11203,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="67" customFormat="1" ht="23.5" customHeight="1" thickBot="1">
+    <row r="38" spans="1:16" s="67" customFormat="1" ht="23.45" customHeight="1" thickBot="1">
       <c r="A38" s="87" t="s">
         <v>381</v>
       </c>
@@ -11285,7 +11293,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="67" customFormat="1" ht="100" customHeight="1" thickBot="1">
+    <row r="41" spans="1:16" s="67" customFormat="1" ht="99.95" customHeight="1" thickBot="1">
       <c r="A41" s="87" t="s">
         <v>387</v>
       </c>
@@ -11323,7 +11331,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="67" customFormat="1" ht="70.5" thickBot="1">
+    <row r="42" spans="1:16" s="67" customFormat="1" ht="75.75" thickBot="1">
       <c r="A42" s="87" t="s">
         <v>391</v>
       </c>
@@ -11417,7 +11425,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="67" customFormat="1" ht="70.5" thickBot="1">
+    <row r="45" spans="1:16" s="67" customFormat="1" ht="75.75" thickBot="1">
       <c r="A45" s="87" t="s">
         <v>399</v>
       </c>
@@ -11441,19 +11449,19 @@
       <c r="K45" s="108"/>
       <c r="L45" s="131"/>
       <c r="M45" s="117" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N45" s="108" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="O45" s="111" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="P45" s="87" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="67" customFormat="1" ht="154.5" thickBot="1">
+    <row r="46" spans="1:16" s="67" customFormat="1" ht="157.5" thickBot="1">
       <c r="A46" s="87" t="s">
         <v>401</v>
       </c>
@@ -11478,18 +11486,18 @@
       <c r="J46" s="107"/>
       <c r="K46" s="107"/>
       <c r="L46" s="144" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="M46" s="107"/>
       <c r="N46" s="108" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="O46" s="107"/>
       <c r="P46" s="87" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="67" customFormat="1" ht="114.5" thickBot="1">
+    <row r="47" spans="1:16" s="67" customFormat="1" ht="114.75" thickBot="1">
       <c r="A47" s="87" t="s">
         <v>403</v>
       </c>
@@ -11512,7 +11520,7 @@
       <c r="J47" s="107"/>
       <c r="K47" s="107"/>
       <c r="L47" s="144" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="M47" s="107"/>
       <c r="N47" s="107"/>
@@ -11521,7 +11529,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="48" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A48" s="87" t="s">
         <v>405</v>
       </c>
@@ -11542,7 +11550,7 @@
       <c r="J48" s="107"/>
       <c r="K48" s="107"/>
       <c r="L48" s="144" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="M48" s="107"/>
       <c r="N48" s="107"/>
@@ -11551,7 +11559,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="67" customFormat="1" ht="86" thickBot="1">
+    <row r="49" spans="1:16" s="67" customFormat="1" ht="86.25" thickBot="1">
       <c r="A49" s="87" t="s">
         <v>407</v>
       </c>
@@ -11574,20 +11582,20 @@
       <c r="J49" s="107"/>
       <c r="K49" s="107"/>
       <c r="L49" s="144" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="M49" s="107"/>
       <c r="N49" s="108" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="O49" s="117" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="P49" s="87" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="67" customFormat="1" ht="126.5" thickBot="1">
+    <row r="50" spans="1:16" s="67" customFormat="1" ht="157.5" thickBot="1">
       <c r="A50" s="87" t="s">
         <v>409</v>
       </c>
@@ -11612,27 +11620,27 @@
       <c r="J50" s="107"/>
       <c r="K50" s="107"/>
       <c r="L50" s="144" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="M50" s="117" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="N50" s="107"/>
       <c r="O50" s="117" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="P50" s="87" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="67" customFormat="1" ht="168.5" thickBot="1">
+    <row r="51" spans="1:16" s="67" customFormat="1" ht="171.75" thickBot="1">
       <c r="A51" s="87" t="s">
         <v>411</v>
       </c>
       <c r="B51" s="126" t="s">
         <v>272</v>
       </c>
-      <c r="C51" s="193" t="s">
+      <c r="C51" s="158" t="s">
         <v>412</v>
       </c>
       <c r="D51" s="129" t="s">
@@ -11650,22 +11658,22 @@
       <c r="J51" s="107"/>
       <c r="K51" s="107"/>
       <c r="L51" s="144" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="M51" s="117" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="N51" s="107" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="O51" s="117" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="P51" s="87" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="67" customFormat="1" ht="70.5" thickBot="1">
+    <row r="52" spans="1:16" s="67" customFormat="1" ht="86.25" thickBot="1">
       <c r="A52" s="87" t="s">
         <v>413</v>
       </c>
@@ -11690,20 +11698,20 @@
       <c r="J52" s="108"/>
       <c r="K52" s="108"/>
       <c r="L52" s="144" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="M52" s="108"/>
       <c r="N52" s="108" t="s">
         <v>54</v>
       </c>
       <c r="O52" s="108" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="P52" s="87" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="67" customFormat="1" ht="210.5" thickBot="1">
+    <row r="53" spans="1:16" s="67" customFormat="1" ht="214.5" thickBot="1">
       <c r="A53" s="87" t="s">
         <v>415</v>
       </c>
@@ -11726,20 +11734,20 @@
       <c r="J53" s="107"/>
       <c r="K53" s="107"/>
       <c r="L53" s="144" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="M53" s="107"/>
       <c r="N53" s="107" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="O53" s="117" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="P53" s="87" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="67" customFormat="1" ht="42.5" thickBot="1">
+    <row r="54" spans="1:16" s="67" customFormat="1" ht="57.75" thickBot="1">
       <c r="A54" s="87" t="s">
         <v>417</v>
       </c>
@@ -11762,20 +11770,20 @@
       <c r="J54" s="107"/>
       <c r="K54" s="107"/>
       <c r="L54" s="144" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="M54" s="107"/>
       <c r="N54" s="107" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="O54" s="117" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="P54" s="87" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="55" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A55" s="87" t="s">
         <v>419</v>
       </c>
@@ -11803,7 +11811,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="56" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A56" s="87" t="s">
         <v>421</v>
       </c>
@@ -11831,7 +11839,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="57" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A57" s="87" t="s">
         <v>423</v>
       </c>
@@ -11854,18 +11862,18 @@
       <c r="J57" s="107"/>
       <c r="K57" s="107"/>
       <c r="L57" s="144" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="M57" s="107"/>
       <c r="N57" s="107"/>
       <c r="O57" s="117" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="P57" s="87" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="58" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A58" s="87" t="s">
         <v>425</v>
       </c>
@@ -11893,7 +11901,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="59" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A59" s="87" t="s">
         <v>426</v>
       </c>
@@ -11921,7 +11929,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="67" customFormat="1" ht="84.5" thickBot="1">
+    <row r="60" spans="1:16" s="67" customFormat="1" ht="90.75" thickBot="1">
       <c r="A60" s="87" t="s">
         <v>428</v>
       </c>
@@ -11946,12 +11954,12 @@
       <c r="J60" s="107"/>
       <c r="K60" s="107"/>
       <c r="L60" s="144" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="M60" s="107"/>
       <c r="N60" s="107"/>
       <c r="O60" s="117" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="P60" s="87" t="s">
         <v>428</v>
@@ -11978,7 +11986,7 @@
       <c r="J61" s="107"/>
       <c r="K61" s="107"/>
       <c r="L61" s="144" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="M61" s="107"/>
       <c r="N61" s="107"/>
@@ -11987,7 +11995,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="67" customFormat="1" ht="56.5" thickBot="1">
+    <row r="62" spans="1:16" s="67" customFormat="1" ht="57.75" thickBot="1">
       <c r="A62" s="87" t="s">
         <v>433</v>
       </c>
@@ -12012,20 +12020,20 @@
       <c r="J62" s="107"/>
       <c r="K62" s="107"/>
       <c r="L62" s="144" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="M62" s="107"/>
       <c r="N62" s="107" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="O62" s="117" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="P62" s="87" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="63" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A63" s="87" t="s">
         <v>436</v>
       </c>
@@ -12048,7 +12056,7 @@
       <c r="J63" s="107"/>
       <c r="K63" s="107"/>
       <c r="L63" s="144" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M63" s="107"/>
       <c r="N63" s="107"/>
@@ -12057,7 +12065,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="67" customFormat="1" ht="43" customHeight="1" thickBot="1">
+    <row r="64" spans="1:16" s="67" customFormat="1" ht="42.95" customHeight="1" thickBot="1">
       <c r="A64" s="87" t="s">
         <v>438</v>
       </c>
@@ -12080,7 +12088,7 @@
       <c r="J64" s="108"/>
       <c r="K64" s="108"/>
       <c r="L64" s="144" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="M64" s="108"/>
       <c r="N64" s="108"/>
@@ -12089,7 +12097,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="67" customFormat="1" ht="98.5" thickBot="1">
+    <row r="65" spans="1:16" s="67" customFormat="1" ht="105.75" thickBot="1">
       <c r="A65" s="87" t="s">
         <v>440</v>
       </c>
@@ -12114,18 +12122,18 @@
       <c r="J65" s="107"/>
       <c r="K65" s="107"/>
       <c r="L65" s="144" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="M65" s="107"/>
       <c r="N65" s="107"/>
       <c r="O65" s="117" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="P65" s="87" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="67" customFormat="1" ht="29.5" customHeight="1" thickBot="1">
+    <row r="66" spans="1:16" s="67" customFormat="1" ht="29.45" customHeight="1" thickBot="1">
       <c r="A66" s="87" t="s">
         <v>442</v>
       </c>
@@ -12153,7 +12161,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="67" customFormat="1" ht="42.5" thickBot="1">
+    <row r="67" spans="1:16" s="67" customFormat="1" ht="45.75" thickBot="1">
       <c r="A67" s="87" t="s">
         <v>444</v>
       </c>
@@ -12178,18 +12186,18 @@
       <c r="J67" s="107"/>
       <c r="K67" s="107"/>
       <c r="L67" s="144" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="M67" s="107"/>
       <c r="N67" s="107"/>
       <c r="O67" s="117" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="P67" s="87" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="67" customFormat="1" ht="70.5" thickBot="1">
+    <row r="68" spans="1:16" s="67" customFormat="1" ht="75.75" thickBot="1">
       <c r="A68" s="87" t="s">
         <v>446</v>
       </c>
@@ -12212,20 +12220,20 @@
       <c r="J68" s="107"/>
       <c r="K68" s="107"/>
       <c r="L68" s="144" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="M68" s="107" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="N68" s="107"/>
       <c r="O68" s="117" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="P68" s="87" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="67" customFormat="1" ht="84.5" thickBot="1">
+    <row r="69" spans="1:16" s="67" customFormat="1" ht="90.75" thickBot="1">
       <c r="A69" s="87" t="s">
         <v>448</v>
       </c>
@@ -12248,20 +12256,20 @@
       <c r="J69" s="107"/>
       <c r="K69" s="107"/>
       <c r="L69" s="153" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="M69" s="107" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="N69" s="107"/>
       <c r="O69" s="117" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="P69" s="87" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="67" customFormat="1" ht="70.5" thickBot="1">
+    <row r="70" spans="1:16" s="67" customFormat="1" ht="72" thickBot="1">
       <c r="A70" s="87" t="s">
         <v>450</v>
       </c>
@@ -12284,30 +12292,30 @@
       <c r="J70" s="107"/>
       <c r="K70" s="107"/>
       <c r="L70" s="144" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="M70" s="117" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="N70" s="107" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="O70" s="117" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="P70" s="87" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="71" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A71" s="189" t="s">
+      <c r="A71" s="188" t="s">
         <v>452</v>
       </c>
-      <c r="B71" s="189"/>
-      <c r="C71" s="189"/>
-      <c r="D71" s="189"/>
-      <c r="E71" s="189"/>
-      <c r="F71" s="189"/>
+      <c r="B71" s="188"/>
+      <c r="C71" s="188"/>
+      <c r="D71" s="188"/>
+      <c r="E71" s="188"/>
+      <c r="F71" s="188"/>
       <c r="G71" s="122"/>
       <c r="H71" s="123"/>
       <c r="I71" s="123"/>
@@ -12319,7 +12327,7 @@
       <c r="O71" s="125"/>
       <c r="P71" s="124"/>
     </row>
-    <row r="72" spans="1:16" s="67" customFormat="1" ht="42.5" thickBot="1">
+    <row r="72" spans="1:16" s="67" customFormat="1" ht="45.75" thickBot="1">
       <c r="A72" s="87" t="s">
         <v>453</v>
       </c>
@@ -12342,20 +12350,20 @@
       <c r="J72" s="107"/>
       <c r="K72" s="107"/>
       <c r="L72" s="117" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="M72" s="107"/>
       <c r="N72" s="107" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="O72" s="117" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="P72" s="87" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="73" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A73" s="87" t="s">
         <v>455</v>
       </c>
@@ -12378,18 +12386,18 @@
       <c r="J73" s="107"/>
       <c r="K73" s="107"/>
       <c r="L73" s="154" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="M73" s="107"/>
       <c r="N73" s="107" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="O73" s="107"/>
       <c r="P73" s="87" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="74" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A74" s="87" t="s">
         <v>457</v>
       </c>
@@ -12410,18 +12418,18 @@
       <c r="J74" s="107"/>
       <c r="K74" s="107"/>
       <c r="L74" s="154" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="M74" s="107"/>
       <c r="N74" s="107" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="O74" s="107"/>
       <c r="P74" s="87" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="75" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A75" s="87" t="s">
         <v>459</v>
       </c>
@@ -12449,7 +12457,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="67" customFormat="1" ht="42.5" thickBot="1">
+    <row r="76" spans="1:16" s="67" customFormat="1" ht="43.5" thickBot="1">
       <c r="A76" s="87" t="s">
         <v>461</v>
       </c>
@@ -12472,20 +12480,20 @@
       <c r="J76" s="107"/>
       <c r="K76" s="107"/>
       <c r="L76" s="144" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="M76" s="107"/>
       <c r="N76" s="107" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="O76" s="107" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="P76" s="87" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="67" customFormat="1" ht="42.5" thickBot="1">
+    <row r="77" spans="1:16" s="67" customFormat="1" ht="43.5" thickBot="1">
       <c r="A77" s="87" t="s">
         <v>463</v>
       </c>
@@ -12508,7 +12516,7 @@
       <c r="J77" s="107"/>
       <c r="K77" s="107"/>
       <c r="L77" s="144" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="M77" s="107"/>
       <c r="N77" s="107"/>
@@ -12540,7 +12548,7 @@
       <c r="J78" s="107"/>
       <c r="K78" s="107"/>
       <c r="L78" s="144" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="M78" s="107"/>
       <c r="N78" s="107"/>
@@ -12549,7 +12557,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="79" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A79" s="87" t="s">
         <v>467</v>
       </c>
@@ -12572,13 +12580,13 @@
       <c r="M79" s="107"/>
       <c r="N79" s="107"/>
       <c r="O79" s="117" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="P79" s="87" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="67" customFormat="1" ht="84.5" thickBot="1">
+    <row r="80" spans="1:16" s="67" customFormat="1" ht="86.25" thickBot="1">
       <c r="A80" s="87" t="s">
         <v>469</v>
       </c>
@@ -12601,7 +12609,7 @@
       <c r="J80" s="107"/>
       <c r="K80" s="107"/>
       <c r="L80" s="144" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="M80" s="107"/>
       <c r="N80" s="107"/>
@@ -12610,7 +12618,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="67" customFormat="1" ht="42.5" thickBot="1">
+    <row r="81" spans="1:16" s="67" customFormat="1" ht="43.5" thickBot="1">
       <c r="A81" s="87" t="s">
         <v>471</v>
       </c>
@@ -12633,7 +12641,7 @@
       <c r="J81" s="107"/>
       <c r="K81" s="107"/>
       <c r="L81" s="144" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="M81" s="107"/>
       <c r="N81" s="107"/>
@@ -12642,7 +12650,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="82" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A82" s="87" t="s">
         <v>473</v>
       </c>
@@ -12665,26 +12673,26 @@
       <c r="J82" s="107"/>
       <c r="K82" s="107"/>
       <c r="L82" s="144" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="M82" s="117"/>
       <c r="N82" s="107"/>
       <c r="O82" s="117" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="P82" s="87" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="83" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A83" s="189" t="s">
+      <c r="A83" s="188" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="189"/>
-      <c r="C83" s="189"/>
-      <c r="D83" s="189"/>
-      <c r="E83" s="189"/>
-      <c r="F83" s="189"/>
+      <c r="B83" s="188"/>
+      <c r="C83" s="188"/>
+      <c r="D83" s="188"/>
+      <c r="E83" s="188"/>
+      <c r="F83" s="188"/>
       <c r="G83" s="122"/>
       <c r="H83" s="123"/>
       <c r="I83" s="123"/>
@@ -12696,7 +12704,7 @@
       <c r="O83" s="125"/>
       <c r="P83" s="124"/>
     </row>
-    <row r="84" spans="1:16" s="67" customFormat="1" ht="42.5" thickBot="1">
+    <row r="84" spans="1:16" s="67" customFormat="1" ht="75.75" thickBot="1">
       <c r="A84" s="112" t="s">
         <v>475</v>
       </c>
@@ -12711,20 +12719,30 @@
       </c>
       <c r="E84" s="118"/>
       <c r="F84" s="119"/>
-      <c r="G84" s="107"/>
-      <c r="H84" s="107"/>
+      <c r="G84" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="H84" s="148" t="s">
+        <v>267</v>
+      </c>
       <c r="I84" s="107"/>
       <c r="J84" s="107"/>
       <c r="K84" s="107"/>
-      <c r="L84" s="107"/>
-      <c r="M84" s="107"/>
-      <c r="N84" s="107"/>
+      <c r="L84" s="117" t="s">
+        <v>593</v>
+      </c>
+      <c r="M84" s="107" t="s">
+        <v>591</v>
+      </c>
+      <c r="N84" s="107" t="s">
+        <v>546</v>
+      </c>
       <c r="O84" s="107"/>
       <c r="P84" s="89" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="85" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A85" s="87" t="s">
         <v>477</v>
       </c>
@@ -12739,12 +12757,16 @@
       </c>
       <c r="E85" s="118"/>
       <c r="F85" s="119"/>
-      <c r="G85" s="107"/>
+      <c r="G85" s="148" t="s">
+        <v>267</v>
+      </c>
       <c r="H85" s="107"/>
       <c r="I85" s="107"/>
       <c r="J85" s="107"/>
       <c r="K85" s="107"/>
-      <c r="L85" s="131"/>
+      <c r="L85" s="194" t="s">
+        <v>592</v>
+      </c>
       <c r="M85" s="107"/>
       <c r="N85" s="107"/>
       <c r="O85" s="107"/>
@@ -12752,7 +12774,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="86" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A86" s="87" t="s">
         <v>479</v>
       </c>
@@ -12767,7 +12789,9 @@
       </c>
       <c r="E86" s="118"/>
       <c r="F86" s="119"/>
-      <c r="G86" s="107"/>
+      <c r="G86" s="148" t="s">
+        <v>267</v>
+      </c>
       <c r="H86" s="107"/>
       <c r="I86" s="107"/>
       <c r="J86" s="107"/>
@@ -12780,7 +12804,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="87" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A87" s="87" t="s">
         <v>481</v>
       </c>
@@ -12795,12 +12819,16 @@
       </c>
       <c r="E87" s="118"/>
       <c r="F87" s="119"/>
-      <c r="G87" s="107"/>
+      <c r="G87" s="148" t="s">
+        <v>267</v>
+      </c>
       <c r="H87" s="107"/>
       <c r="I87" s="107"/>
       <c r="J87" s="107"/>
       <c r="K87" s="107"/>
-      <c r="L87" s="131"/>
+      <c r="L87" s="194" t="s">
+        <v>592</v>
+      </c>
       <c r="M87" s="107"/>
       <c r="N87" s="107"/>
       <c r="O87" s="107"/>
@@ -12808,7 +12836,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="88" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A88" s="87" t="s">
         <v>483</v>
       </c>
@@ -12837,14 +12865,14 @@
       </c>
     </row>
     <row r="89" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A89" s="189" t="s">
+      <c r="A89" s="188" t="s">
         <v>485</v>
       </c>
-      <c r="B89" s="189"/>
-      <c r="C89" s="189"/>
-      <c r="D89" s="189"/>
-      <c r="E89" s="189"/>
-      <c r="F89" s="189"/>
+      <c r="B89" s="188"/>
+      <c r="C89" s="188"/>
+      <c r="D89" s="188"/>
+      <c r="E89" s="188"/>
+      <c r="F89" s="188"/>
       <c r="G89" s="122"/>
       <c r="H89" s="123"/>
       <c r="I89" s="123"/>
@@ -12856,7 +12884,7 @@
       <c r="O89" s="125"/>
       <c r="P89" s="124"/>
     </row>
-    <row r="90" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="90" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A90" s="112" t="s">
         <v>486</v>
       </c>
@@ -12871,7 +12899,9 @@
       </c>
       <c r="E90" s="118"/>
       <c r="F90" s="119"/>
-      <c r="G90" s="107"/>
+      <c r="G90" s="148" t="s">
+        <v>267</v>
+      </c>
       <c r="H90" s="107"/>
       <c r="I90" s="107"/>
       <c r="J90" s="107"/>
@@ -12884,7 +12914,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="91" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A91" s="112" t="s">
         <v>488</v>
       </c>
@@ -12899,7 +12929,9 @@
       </c>
       <c r="E91" s="118"/>
       <c r="F91" s="119"/>
-      <c r="G91" s="107"/>
+      <c r="G91" s="148" t="s">
+        <v>267</v>
+      </c>
       <c r="H91" s="107"/>
       <c r="I91" s="107"/>
       <c r="J91" s="107"/>
@@ -12912,7 +12944,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="92" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A92" s="112" t="s">
         <v>490</v>
       </c>
@@ -12940,7 +12972,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="93" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="93" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A93" s="112" t="s">
         <v>492</v>
       </c>
@@ -12950,17 +12982,19 @@
       <c r="C93" s="89" t="s">
         <v>493</v>
       </c>
-      <c r="D93" s="129"/>
+      <c r="D93" s="129" t="s">
+        <v>266</v>
+      </c>
       <c r="E93" s="118"/>
       <c r="F93" s="119"/>
-      <c r="G93" s="107"/>
+      <c r="G93" s="148" t="s">
+        <v>267</v>
+      </c>
       <c r="H93" s="107"/>
       <c r="I93" s="107"/>
       <c r="J93" s="107"/>
       <c r="K93" s="107"/>
-      <c r="L93" s="109" t="s">
-        <v>494</v>
-      </c>
+      <c r="L93" s="109"/>
       <c r="M93" s="107"/>
       <c r="N93" s="107"/>
       <c r="O93" s="107"/>
@@ -12968,43 +13002,43 @@
         <v>492</v>
       </c>
     </row>
-    <row r="94" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="94" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A94" s="87" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B94" s="115" t="s">
         <v>272</v>
       </c>
       <c r="C94" s="89" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D94" s="129"/>
       <c r="E94" s="118"/>
       <c r="F94" s="119"/>
-      <c r="G94" s="108"/>
+      <c r="G94" s="108" t="s">
+        <v>349</v>
+      </c>
       <c r="H94" s="107"/>
       <c r="I94" s="107"/>
       <c r="J94" s="107"/>
       <c r="K94" s="107"/>
-      <c r="L94" s="109" t="s">
-        <v>497</v>
-      </c>
+      <c r="L94" s="109"/>
       <c r="M94" s="107"/>
       <c r="N94" s="107"/>
       <c r="O94" s="107"/>
       <c r="P94" s="87" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="95" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A95" s="189" t="s">
-        <v>498</v>
-      </c>
-      <c r="B95" s="189"/>
-      <c r="C95" s="189"/>
-      <c r="D95" s="189"/>
-      <c r="E95" s="189"/>
-      <c r="F95" s="189"/>
+      <c r="A95" s="188" t="s">
+        <v>496</v>
+      </c>
+      <c r="B95" s="188"/>
+      <c r="C95" s="188"/>
+      <c r="D95" s="188"/>
+      <c r="E95" s="188"/>
+      <c r="F95" s="188"/>
       <c r="G95" s="122"/>
       <c r="H95" s="123"/>
       <c r="I95" s="123"/>
@@ -13016,15 +13050,15 @@
       <c r="O95" s="125"/>
       <c r="P95" s="124"/>
     </row>
-    <row r="96" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="96" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A96" s="112" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B96" s="88" t="s">
         <v>272</v>
       </c>
       <c r="C96" s="89" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D96" s="118" t="s">
         <v>266</v>
@@ -13041,18 +13075,18 @@
       <c r="N96" s="107"/>
       <c r="O96" s="107"/>
       <c r="P96" s="112" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A97" s="87" t="s">
         <v>499</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
-      <c r="A97" s="87" t="s">
-        <v>501</v>
       </c>
       <c r="B97" s="115" t="s">
         <v>279</v>
       </c>
       <c r="C97" s="89" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D97" s="118" t="s">
         <v>266</v>
@@ -13069,18 +13103,18 @@
       <c r="N97" s="107"/>
       <c r="O97" s="107"/>
       <c r="P97" s="87" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A98" s="188" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="98" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A98" s="189" t="s">
-        <v>503</v>
-      </c>
-      <c r="B98" s="189"/>
-      <c r="C98" s="189"/>
-      <c r="D98" s="189"/>
-      <c r="E98" s="189"/>
-      <c r="F98" s="189"/>
+      <c r="B98" s="188"/>
+      <c r="C98" s="188"/>
+      <c r="D98" s="188"/>
+      <c r="E98" s="188"/>
+      <c r="F98" s="188"/>
       <c r="G98" s="122"/>
       <c r="H98" s="123"/>
       <c r="I98" s="123"/>
@@ -13092,15 +13126,15 @@
       <c r="O98" s="125"/>
       <c r="P98" s="124"/>
     </row>
-    <row r="99" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="99" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A99" s="87" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B99" s="115" t="s">
         <v>272</v>
       </c>
       <c r="C99" s="133" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D99" s="118" t="s">
         <v>266</v>
@@ -13117,18 +13151,18 @@
       <c r="N99" s="107"/>
       <c r="O99" s="107"/>
       <c r="P99" s="87" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A100" s="188" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="100" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A100" s="189" t="s">
-        <v>506</v>
-      </c>
-      <c r="B100" s="189"/>
-      <c r="C100" s="189"/>
-      <c r="D100" s="189"/>
-      <c r="E100" s="189"/>
-      <c r="F100" s="189"/>
+      <c r="B100" s="188"/>
+      <c r="C100" s="188"/>
+      <c r="D100" s="188"/>
+      <c r="E100" s="188"/>
+      <c r="F100" s="188"/>
       <c r="G100" s="122"/>
       <c r="H100" s="123"/>
       <c r="I100" s="123"/>
@@ -13140,15 +13174,15 @@
       <c r="O100" s="125"/>
       <c r="P100" s="124"/>
     </row>
-    <row r="101" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="101" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A101" s="112" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B101" s="88" t="s">
         <v>279</v>
       </c>
       <c r="C101" s="89" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D101" s="132" t="s">
         <v>266</v>
@@ -13165,18 +13199,18 @@
       <c r="N101" s="107"/>
       <c r="O101" s="107"/>
       <c r="P101" s="112" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A102" s="112" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="102" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
-      <c r="A102" s="112" t="s">
+      <c r="B102" s="88" t="s">
+        <v>508</v>
+      </c>
+      <c r="C102" s="89" t="s">
         <v>509</v>
-      </c>
-      <c r="B102" s="88" t="s">
-        <v>510</v>
-      </c>
-      <c r="C102" s="89" t="s">
-        <v>511</v>
       </c>
       <c r="D102" s="129"/>
       <c r="E102" s="118"/>
@@ -13191,18 +13225,18 @@
       <c r="N102" s="108"/>
       <c r="O102" s="108"/>
       <c r="P102" s="112" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A103" s="112" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B103" s="88" t="s">
         <v>352</v>
       </c>
       <c r="C103" s="89" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D103" s="129" t="s">
         <v>266</v>
@@ -13219,18 +13253,18 @@
       <c r="N103" s="107"/>
       <c r="O103" s="107"/>
       <c r="P103" s="112" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="104" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A104" s="191" t="s">
+      <c r="A104" s="189" t="s">
         <v>232</v>
       </c>
-      <c r="B104" s="191"/>
-      <c r="C104" s="191"/>
-      <c r="D104" s="191"/>
-      <c r="E104" s="191"/>
-      <c r="F104" s="191"/>
+      <c r="B104" s="189"/>
+      <c r="C104" s="189"/>
+      <c r="D104" s="189"/>
+      <c r="E104" s="189"/>
+      <c r="F104" s="189"/>
       <c r="G104" s="122"/>
       <c r="H104" s="123"/>
       <c r="I104" s="123"/>
@@ -13242,15 +13276,15 @@
       <c r="O104" s="125"/>
       <c r="P104" s="124"/>
     </row>
-    <row r="105" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="105" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A105" s="112" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B105" s="88" t="s">
         <v>272</v>
       </c>
       <c r="C105" s="89" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D105" s="129"/>
       <c r="E105" s="118" t="s">
@@ -13267,18 +13301,18 @@
       <c r="N105" s="107"/>
       <c r="O105" s="107"/>
       <c r="P105" s="112" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A106" s="112" t="s">
         <v>514</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
-      <c r="A106" s="112" t="s">
-        <v>516</v>
       </c>
       <c r="B106" s="88" t="s">
         <v>272</v>
       </c>
       <c r="C106" s="89" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D106" s="129"/>
       <c r="E106" s="118" t="s">
@@ -13295,12 +13329,12 @@
       <c r="N106" s="107"/>
       <c r="O106" s="107"/>
       <c r="P106" s="112" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A107" s="112" t="s">
         <v>516</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
-      <c r="A107" s="112" t="s">
-        <v>518</v>
       </c>
       <c r="B107" s="88" t="s">
         <v>352</v>
@@ -13323,18 +13357,18 @@
       <c r="N107" s="107"/>
       <c r="O107" s="107"/>
       <c r="P107" s="112" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A108" s="89" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B108" s="88" t="s">
         <v>272</v>
       </c>
       <c r="C108" s="135" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D108" s="136"/>
       <c r="E108" s="88" t="s">
@@ -13351,18 +13385,18 @@
       <c r="N108" s="107"/>
       <c r="O108" s="107"/>
       <c r="P108" s="89" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="109" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A109" s="189" t="s">
+      <c r="A109" s="188" t="s">
         <v>243</v>
       </c>
-      <c r="B109" s="189"/>
-      <c r="C109" s="189"/>
-      <c r="D109" s="189"/>
-      <c r="E109" s="189"/>
-      <c r="F109" s="189"/>
+      <c r="B109" s="188"/>
+      <c r="C109" s="188"/>
+      <c r="D109" s="188"/>
+      <c r="E109" s="188"/>
+      <c r="F109" s="188"/>
       <c r="G109" s="122"/>
       <c r="H109" s="123"/>
       <c r="I109" s="123"/>
@@ -13374,15 +13408,15 @@
       <c r="O109" s="125"/>
       <c r="P109" s="124"/>
     </row>
-    <row r="110" spans="1:16" s="67" customFormat="1" ht="28.5" thickBot="1">
+    <row r="110" spans="1:16" s="67" customFormat="1" ht="30.75" thickBot="1">
       <c r="A110" s="137" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B110" s="138" t="s">
         <v>279</v>
       </c>
       <c r="C110" s="139" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D110" s="129"/>
       <c r="E110" s="118" t="s">
@@ -13399,18 +13433,18 @@
       <c r="N110" s="140"/>
       <c r="O110" s="140"/>
       <c r="P110" s="137" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A111" s="141" t="s">
         <v>521</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
-      <c r="A111" s="141" t="s">
-        <v>523</v>
       </c>
       <c r="B111" s="138" t="s">
         <v>352</v>
       </c>
       <c r="C111" s="139" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D111" s="129" t="s">
         <v>266</v>
@@ -13427,16 +13461,16 @@
       <c r="N111" s="140"/>
       <c r="O111" s="140"/>
       <c r="P111" s="141" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A112" s="141" t="s">
         <v>523</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
-      <c r="A112" s="141" t="s">
-        <v>525</v>
       </c>
       <c r="B112" s="138"/>
       <c r="C112" s="139" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D112" s="129"/>
       <c r="E112" s="118" t="s">
@@ -13453,18 +13487,18 @@
       <c r="N112" s="140"/>
       <c r="O112" s="140"/>
       <c r="P112" s="141" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A113" s="141" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
-      <c r="A113" s="141" t="s">
-        <v>527</v>
       </c>
       <c r="B113" s="138" t="s">
         <v>272</v>
       </c>
       <c r="C113" s="139" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D113" s="129"/>
       <c r="E113" s="118" t="s">
@@ -13481,18 +13515,18 @@
       <c r="N113" s="140"/>
       <c r="O113" s="140"/>
       <c r="P113" s="141" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="114" spans="1:16" s="67" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A114" s="189" t="s">
+      <c r="A114" s="188" t="s">
         <v>244</v>
       </c>
-      <c r="B114" s="189"/>
-      <c r="C114" s="189"/>
-      <c r="D114" s="189"/>
-      <c r="E114" s="189"/>
-      <c r="F114" s="189"/>
+      <c r="B114" s="188"/>
+      <c r="C114" s="188"/>
+      <c r="D114" s="188"/>
+      <c r="E114" s="188"/>
+      <c r="F114" s="188"/>
       <c r="G114" s="122"/>
       <c r="H114" s="123"/>
       <c r="I114" s="123"/>
@@ -13504,15 +13538,15 @@
       <c r="O114" s="125"/>
       <c r="P114" s="124"/>
     </row>
-    <row r="115" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
+    <row r="115" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
       <c r="A115" s="137" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B115" s="138" t="s">
         <v>279</v>
       </c>
       <c r="C115" s="139" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D115" s="129"/>
       <c r="E115" s="118" t="s">
@@ -13529,18 +13563,18 @@
       <c r="N115" s="140"/>
       <c r="O115" s="140"/>
       <c r="P115" s="137" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A116" s="137" t="s">
         <v>529</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
-      <c r="A116" s="137" t="s">
-        <v>531</v>
       </c>
       <c r="B116" s="142" t="s">
         <v>279</v>
       </c>
       <c r="C116" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D116" s="129"/>
       <c r="E116" s="118" t="s">
@@ -13557,18 +13591,18 @@
       <c r="N116" s="140"/>
       <c r="O116" s="140"/>
       <c r="P116" s="137" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" s="67" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A117" s="143" t="s">
         <v>531</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16" s="67" customFormat="1" ht="15" thickBot="1">
-      <c r="A117" s="143" t="s">
-        <v>533</v>
       </c>
       <c r="B117" s="138" t="s">
         <v>352</v>
       </c>
       <c r="C117" s="139" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D117" s="136"/>
       <c r="E117" s="88" t="s">
@@ -13585,34 +13619,36 @@
       <c r="N117" s="140"/>
       <c r="O117" s="140"/>
       <c r="P117" s="143" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:B474" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="15">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="Q6:T17"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A95:F95"/>
     <mergeCell ref="A98:F98"/>
     <mergeCell ref="A100:F100"/>
     <mergeCell ref="A104:F104"/>
     <mergeCell ref="A109:F109"/>
     <mergeCell ref="A114:F114"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A71:F71"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A95:F95"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="Q6:T17"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A36:F36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L12" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="L23" r:id="rId2" display="no WLAN is configured in factory settings_x000a_TP.A.19.2: Because the user has complete control over everything the DUT does, the DUT could be configured to not seperate clients in the self defined guest WLAN and the other interfaces. Devices are properly separated if the instructions https://openwrt.org/docs/guide-user/network/wifi/guestwifi/guest-wlan are followed" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="L42" r:id="rId3" display="https://openwrt.org/docs/guide-user/services/webserver/uhttpd" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="L85" r:id="rId4" xr:uid="{6BFFEB1F-E727-4369-B0B8-5CC2A8CE848C}"/>
+    <hyperlink ref="L87" r:id="rId5" xr:uid="{2330E7B3-95D6-4E5B-B65E-F85857F89211}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="8" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="8" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>